<commit_message>
Update Processo realizado corretamente
Funcionando corretamente porem não foi testado em ambientes diversos apenas em alguns casos
</commit_message>
<xml_diff>
--- a/Teste.xlsx
+++ b/Teste.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <x:si>
     <x:t>Arquivo</x:t>
   </x:si>
@@ -25,383 +25,220 @@
     <x:t>Dados XML</x:t>
   </x:si>
   <x:si>
-    <x:t>31211292660604017662550500000170671478739470.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\31211292660604017662550500000170671478739470.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;nfeProc versao="4.00" xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;NFe xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;infNFe Id="NFe31211292660604017662550500000170671478739470" versao="4.00"&gt;&lt;ide&gt;&lt;cUF&gt;31&lt;/cUF&gt;&lt;cNF&gt;47873947&lt;/cNF&gt;&lt;natOp&gt;Remessa p/ deposito fechado ou arm.geral&lt;/natOp&gt;&lt;mod&gt;55&lt;/mod&gt;&lt;serie&gt;50&lt;/serie&gt;&lt;nNF&gt;17067&lt;/nNF&gt;&lt;dhEmi&gt;2021-12-21T18:48:14-03:00&lt;/dhEmi&gt;&lt;tpNF&gt;1&lt;/tpNF&gt;&lt;idDest&gt;2&lt;/idDest&gt;&lt;cMunFG&gt;3166808&lt;/cMunFG&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;0&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;finNFe&gt;1&lt;/finNFe&gt;&lt;indFinal&gt;0&lt;/indFinal&gt;&lt;indPres&gt;9&lt;/indPres&gt;&lt;indIntermed&gt;0&lt;/indIntermed&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;SAP NFE 4.00&lt;/verProc&gt;&lt;/ide&gt;&lt;emit&gt;&lt;CNPJ&gt;92660604017662&lt;/CNPJ&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;xFant&gt;CMISS-Compl.Min.Indl.S Salitre&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;Fazenda Salitre&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;Marrua&lt;/xBairro&gt;&lt;cMun&gt;3166808&lt;/cMun&gt;&lt;xMun&gt;Serra do Salitre&lt;/xMun&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;CEP&gt;38760000&lt;/CEP&gt;&lt;xPais&gt;Brasil&lt;/xPais&gt;&lt;/enderEmit&gt;&lt;IE&gt;2874585321020&lt;/IE&gt;&lt;CRT&gt;3&lt;/CRT&gt;&lt;/emit&gt;&lt;dest&gt;&lt;CNPJ&gt;06225292000147&lt;/CNPJ&gt;&lt;xNome&gt;TERLOC TERMINAL LOGISTICO CESARI LT DA&lt;/xNome&gt;&lt;enderDest&gt;&lt;xLgr&gt;EST ENGENHEIRO PLINIO DE QUEIROZ&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xCpl&gt;SP 55&lt;/xCpl&gt;&lt;xBairro&gt;PIACAGUERA&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;CUBATAO&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;CEP&gt;11570000&lt;/CEP&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;Brasil&lt;/xPais&gt;&lt;/enderDest&gt;&lt;indIEDest&gt;1&lt;/indIEDest&gt;&lt;IE&gt;283108491118&lt;/IE&gt;&lt;email&gt;expedicao@terloc.com.br&lt;/email&gt;&lt;/dest&gt;&lt;det nItem="1"&gt;&lt;prod&gt;&lt;cProd&gt;1000011243&lt;/cProd&gt;&lt;cEAN&gt;SEM GTIN&lt;/cEAN&gt;&lt;xProd&gt;CONCENTRADO FOSFATICO GROSSO UMIDO CMISS&lt;/xProd&gt;&lt;NCM&gt;25102010&lt;/NCM&gt;&lt;EXTIPI&gt;10&lt;/EXTIPI&gt;&lt;CFOP&gt;6905&lt;/CFOP&gt;&lt;uCom&gt;TO&lt;/uCom&gt;&lt;qCom&gt;47.7100&lt;/qCom&gt;&lt;vUnCom&gt;1194.5200167680&lt;/vUnCom&gt;&lt;vProd&gt;56990.55&lt;/vProd&gt;&lt;cEANTrib&gt;SEM GTIN&lt;/cEANTrib&gt;&lt;uTrib&gt;TO&lt;/uTrib&gt;&lt;qTrib&gt;47.7100&lt;/qTrib&gt;&lt;vUnTrib&gt;1194.5200167680&lt;/vUnTrib&gt;&lt;indTot&gt;1&lt;/indTot&gt;&lt;/prod&gt;&lt;imposto&gt;&lt;ICMS&gt;&lt;ICMS20&gt;&lt;orig&gt;0&lt;/orig&gt;&lt;CST&gt;20&lt;/CST&gt;&lt;modBC&gt;3&lt;/modBC&gt;&lt;pRedBC&gt;99.6000&lt;/pRedBC&gt;&lt;vBC&gt;24564.89&lt;/vBC&gt;&lt;pICMS&gt;12.0000&lt;/pICMS&gt;&lt;vICMS&gt;2947.79&lt;/vICMS&gt;&lt;/ICMS20&gt;&lt;/ICMS&gt;&lt;IPI&gt;&lt;cEnq&gt;103&lt;/cEnq&gt;&lt;IPINT&gt;&lt;CST&gt;55&lt;/CST&gt;&lt;/IPINT&gt;&lt;/IPI&gt;&lt;PIS&gt;&lt;PISOutr&gt;&lt;CST&gt;49&lt;/CST&gt;&lt;qBCProd&gt;47.7100&lt;/qBCProd&gt;&lt;vAliqProd&gt;0.0000&lt;/vAliqProd&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;/PISOutr&gt;&lt;/PIS&gt;&lt;COFINS&gt;&lt;COFINSOutr&gt;&lt;CST&gt;49&lt;/CST&gt;&lt;qBCProd&gt;47.7100&lt;/qBCProd&gt;&lt;vAliqProd&gt;0.0000&lt;/vAliqProd&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;/COFINSOutr&gt;&lt;/COFINS&gt;&lt;/imposto&gt;&lt;infAdProd&gt;Base de calculo reduzida em 60 cfe RICMSMG2002, Art. 43 cc Anexo IV, Item 8, b. IPI suspenso nos termos do RIPI, Decreto 7.21210, Art. 43, III. Nao incidencia de COFINS cfe. Lei 10.83303, art. 1o Nao incidencia de PIS cfe. Lei 10.83303, art. 1o&lt;/infAdProd&gt;&lt;/det&gt;&lt;total&gt;&lt;ICMSTot&gt;&lt;vBC&gt;24564.89&lt;/vBC&gt;&lt;vICMS&gt;2947.79&lt;/vICMS&gt;&lt;vICMSDeson&gt;0.00&lt;/vICMSDeson&gt;&lt;vFCP&gt;0.00&lt;/vFCP&gt;&lt;vBCST&gt;0.00&lt;/vBCST&gt;&lt;vST&gt;0.00&lt;/vST&gt;&lt;vFCPST&gt;0.00&lt;/vFCPST&gt;&lt;vFCPSTRet&gt;0.00&lt;/vFCPSTRet&gt;&lt;vProd&gt;56990.55&lt;/vProd&gt;&lt;vFrete&gt;0.00&lt;/vFrete&gt;&lt;vSeg&gt;0.00&lt;/vSeg&gt;&lt;vDesc&gt;0.00&lt;/vDesc&gt;&lt;vII&gt;0.00&lt;/vII&gt;&lt;vIPI&gt;0.00&lt;/vIPI&gt;&lt;vIPIDevol&gt;0.00&lt;/vIPIDevol&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;vOutro&gt;0.00&lt;/vOutro&gt;&lt;vNF&gt;56990.55&lt;/vNF&gt;&lt;/ICMSTot&gt;&lt;/total&gt;&lt;transp&gt;&lt;modFrete&gt;0&lt;/modFrete&gt;&lt;transporta&gt;&lt;CNPJ&gt;50505924000703&lt;/CNPJ&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA FILIAL&lt;/xNome&gt;&lt;xEnder&gt;FILOMENA CARTAFINA 22031&lt;/xEnder&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;/transporta&gt;&lt;vol&gt;&lt;qVol&gt;48&lt;/qVol&gt;&lt;esp&gt;GRANEL&lt;/esp&gt;&lt;marca&gt;YARA&lt;/marca&gt;&lt;pesoL&gt;47710.000&lt;/pesoL&gt;&lt;pesoB&gt;47710.000&lt;/pesoB&gt;&lt;/vol&gt;&lt;/transp&gt;&lt;pag&gt;&lt;detPag&gt;&lt;indPag&gt;0&lt;/indPag&gt;&lt;tPag&gt;15&lt;/tPag&gt;&lt;vPag&gt;56990.55&lt;/vPag&gt;&lt;/detPag&gt;&lt;/pag&gt;&lt;infAdic&gt;&lt;infCpl&gt;Ordem de venda n 0000623925 Ordem de Carregamento 0003109469 Base de calculo reduzida em 60 cfe RICMSMG2002 Art 43 cc Anexo IV Item 8 b IPI suspenso nos termos do RIPI Decreto 721210 Art 43 III Nao incidencia de COFINS cfe Lei 1083303 art 1o Nao incidencia de PIS cfe Lei 1083303 art 1o REGISTRO MAPA NAO SE APLICA Data de fabricacao 21122021 Origem INDUSTRIA BRASILEIRA Classificacao Quimica Modo de aplicacao NA Armazenar sempre sobre piso seco com boa drenagem e em local coberto Para outras condicoes consultar a Yara Brasil Uso exclusivo como fertilizante Prezado Cliente Observacoes sobre carga recebida anotar no verso do canhoto da NF Em caso de emergencia ligue para 08007708899 Remessa 0082307336 A Ficha de Informacoes de Seguranca de Produtos Quimicos pode ser obtida por meio do site wwwyarabrasilcombr&lt;/infCpl&gt;&lt;/infAdic&gt;&lt;/infNFe&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#NFe31211292660604017662550500000170671478739470"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;0D2xAMxnjkdWPu4d3xsRIxVX0hc=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;MI/xyEe0RdCmaGFm3KZeUxJzYaqCvaOR1d13anfueHSx219D15ffzZT6zbuuWsbUVUEqnbTnqKqL
-rXsR3ne9Q17nmTZLdO8YX5QGE3W7sQ5zpx9Dw+oZYgzzGP/wnaJbB1TShKLsfM0lfLIy4zeuvXGl
-ORHQ4WIf06sQkagXnoQGOq0BelDle6P/85RKhfdANs7h5ksQ7knhQdZw44CrwbeScBw/PrfXUAWW
-K6bZMFhvSVk0W8smsfqbLf2HXtbwpxY1NFHGlHIsx6o03LkVRlB+2uI7FoOKTogekHz2dJIBVupP
-XWl7N+6kx3Dc7ji/IOGa0R4SSOxkNFCx821WbQ==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIICzCCBfOgAwIBAgIQNjjNlSyNftb+ED1sesUuPTANBgkqhkiG9w0BAQsFADB4MQswCQYDVQQG
-EwJCUjETMBEGA1UEChMKSUNQLUJyYXNpbDE2MDQGA1UECxMtU2VjcmV0YXJpYSBkYSBSZWNlaXRh
-IEZlZGVyYWwgZG8gQnJhc2lsIC0gUkZCMRwwGgYDVQQDExNBQyBDZXJ0aXNpZ24gUkZCIEc1MB4X
-DTIxMTAwNjE1MDI0M1oXDTIyMTAwNjE1MDI0M1owggEBMQswCQYDVQQGEwJCUjETMBEGA1UECgwK
-SUNQLUJyYXNpbDELMAkGA1UECAwCUlMxFTATBgNVBAcMDFBvcnRvIEFsZWdyZTEZMBcGA1UECwwQ
-VmlkZW9Db25mZXJlbmNpYTEXMBUGA1UECwwOMTA4NjkwODAwMDAxNzAxNjA0BgNVBAsMLVNlY3Jl
-dGFyaWEgZGEgUmVjZWl0YSBGZWRlcmFsIGRvIEJyYXNpbCAtIFJGQjEWMBQGA1UECwwNUkZCIGUt
-Q05QSiBBMTE1MDMGA1UEAwwsWUFSQSBCUkFTSUwgRkVSVElMSVpBTlRFUyBTIEE6OTI2NjA2MDQw
-MDAxODIwggEiMA0GCSqGSIb3DQEBAQUAA4IBDwAwggEKAoIBAQCbDkPNSgzXLGqoqumwXPWkcZCj
-2iP6kjQtBerE4vrBR19Mc4BLYvGZvnniaDYwJxXy3bHVdz/RwGPoblcjEzyYoex7wCZb/1ZVow/w
-jVOIDt7ekV8sbxZMY0J26o2SXfDhcxMjK6i8v/4Ku9oVIJBPWs4QRT4y0t4Kynub1+Vnb2bVi4bI
-I7gHHE/XXwTv6y1pQOHmHTz2mkO/AX1JqCoIoj7XlRoEEnLyXqblE4cb5Gxi1uCSOcc4O00UOG8Y
-c83o3uu4LWnbdu7S056YFP6PWlaNqMkFhjIKGssfZZnEhUWfg/JWnkdyV0pS0LLtSLJa1r+BR/98
-XIWzjfmBc2RbAgMBAAGjggMEMIIDADCBswYDVR0RBIGrMIGooD0GBWBMAQMEoDQEMjI5MDUxOTY5
-NDk1ODkwOTEwOTEwMDAwMDAwMDAwMDAwMDAwNDAzOTU3NDg1MlNTUFJToCIGBWBMAQMCoBkEF0NM
-RUlUT04gTUVTUVVJVEEgVkFSR0FToBkGBWBMAQMDoBAEDjkyNjYwNjA0MDAwMTgyoBcGBWBMAQMH
-oA4EDDAwMDAwMDAwMDAwMIEPZmlzY2FsQHlhcmEuY29tMAkGA1UdEwQCMAAwHwYDVR0jBBgwFoAU
-U31/nb7RYdAgutqf44mnE3NYzUIwfwYDVR0gBHgwdjB0BgZgTAECAQwwajBoBggrBgEFBQcCARZc
-aHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9kcGMvQUNfQ2Vy
-dGlzaWduX1JGQi9EUENfQUNfQ2VydGlzaWduX1JGQi5wZGYwgbwGA1UdHwSBtDCBsTBXoFWgU4ZR
-aHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9sY3IvQUNDZXJ0
-aXNpZ25SRkJHNS9MYXRlc3RDUkwuY3JsMFagVKBShlBodHRwOi8vaWNwLWJyYXNpbC5vdXRyYWxj
-ci5jb20uYnIvcmVwb3NpdG9yaW8vbGNyL0FDQ2VydGlzaWduUkZCRzUvTGF0ZXN0Q1JMLmNybDAO
-BgNVHQ8BAf8EBAMCBeAwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGsBggrBgEFBQcB
-AQSBnzCBnDBfBggrBgEFBQcwAoZTaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9y
-ZXBvc2l0b3Jpby9jZXJ0aWZpY2Fkb3MvQUNfQ2VydGlzaWduX1JGQl9HNS5wN2MwOQYIKwYBBQUH
-MAGGLWh0dHA6Ly9vY3NwLWFjLWNlcnRpc2lnbi1yZmIuY2VydGlzaWduLmNvbS5icjANBgkqhkiG
-9w0BAQsFAAOCAgEASCNnP1ersGgcFlHfGmfzgtSBVH0oJrVrm7/LFr2FjM8AjX9PY97brv6UubUj
-swAD+yL+dwwsuv1TxnBHw8AE8MGbxiZQTnNf0OMkIPAEDvwlb8SXK7Gk137JKUaKKGup5P4dbA8X
-M22+GEw1dMYjCV6eqJ2bxP1EjRII3rb8EsQATZ/pDizsEauNXOmXqbIefqU9wWaQhTQVtLwflrN0
-zElGDSX9uwtR6j28usr3KiKf26MfhtWDAombY+m9Bhq2Hys6hZpyfL+ERFoWXmpzlhmEvUFnMzL1
-SWGNeyhn+na7r7cJvBFcdPPyriZlAdApkaZGXSQAGW78gvlJLD2YtYk/BN02v7qCfhcPHdZcQ4XV
-kdj8idIMcn3ZiweWanaZ9riR3yLStxBP7arsQrMGOrYkAyo9otufpJfYS+FHkrJapqfZxbo0qCTs
-ZPHvAcMw8vCojT/Z2FZrGi6aDK2rt7hPhKYRedZNbDmVgKSRNBoyPqSoqNwMSEiF7EmXA5zq27SM
-87v096EsX8COhgxvMqj/ENxfj8x94POwH8gif/xv9r/raWYCrOnKNP8uhXJPdeihFZBsbWanSUZW
-YlltN/lCaF/oSDqsQjVaG4MndtddEIwdfk3xg71iptYN1tYWHSMal0EwKkOA3A9obwTtxz1fkp8F
-nGxIgi6QuCLfPTU=&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/NFe&gt;&lt;protNFe versao="4.00"&gt;&lt;infProt Id="ID131214496666445"&gt;
+    <x:t>31211092660604015457550760000146171184325883.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\31211092660604015457550760000146171184325883.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;nfeProc versao="4.00" xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;NFe xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;infNFe Id="NFe31211092660604015457550760000146171184325883" versao="4.00"&gt;&lt;ide&gt;&lt;cUF&gt;31&lt;/cUF&gt;&lt;cNF&gt;18432588&lt;/cNF&gt;&lt;natOp&gt;TRANSFERNCIA&lt;/natOp&gt;&lt;mod&gt;55&lt;/mod&gt;&lt;serie&gt;76&lt;/serie&gt;&lt;nNF&gt;14617&lt;/nNF&gt;&lt;dhEmi&gt;2021-10-22T21:09:22-03:00&lt;/dhEmi&gt;&lt;dhSaiEnt&gt;2021-10-22T21:09:22-03:00&lt;/dhSaiEnt&gt;&lt;tpNF&gt;1&lt;/tpNF&gt;&lt;idDest&gt;2&lt;/idDest&gt;&lt;cMunFG&gt;3170107&lt;/cMunFG&gt;&lt;tpImp&gt;2&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;3&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;finNFe&gt;1&lt;/finNFe&gt;&lt;indFinal&gt;0&lt;/indFinal&gt;&lt;indPres&gt;9&lt;/indPres&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;200&lt;/verProc&gt;&lt;/ide&gt;&lt;emit&gt;&lt;CNPJ&gt;92660604015457&lt;/CNPJ&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES SA&lt;/xNome&gt;&lt;xFant&gt;YARA BRASIL FERTILIZANTES SA&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA ANTONIO CARLOS GUILLAUMON 800&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;CEP&gt;38044760&lt;/CEP&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;fone&gt;3433197198&lt;/fone&gt;&lt;/enderEmit&gt;&lt;IE&gt;3714585320678&lt;/IE&gt;&lt;CRT&gt;3&lt;/CRT&gt;&lt;/emit&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604013756&lt;/CNPJ&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES SA&lt;/xNome&gt;&lt;enderDest&gt;&lt;xLgr&gt;AVENIDA SAO JUDAS TADEU&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;JARDIM SAO JUDAS TAD&lt;/xBairro&gt;&lt;cMun&gt;3552403&lt;/cMun&gt;&lt;xMun&gt;SUMARE&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;CEP&gt;13180570&lt;/CEP&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;fone&gt;0000000000&lt;/fone&gt;&lt;/enderDest&gt;&lt;indIEDest&gt;1&lt;/indIEDest&gt;&lt;IE&gt;671143732119&lt;/IE&gt;&lt;/dest&gt;&lt;retirada&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;xLgr&gt;AV. CONS. RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;/retirada&gt;&lt;autXML&gt;&lt;CNPJ&gt;55681274000185&lt;/CNPJ&gt;&lt;/autXML&gt;&lt;autXML&gt;&lt;CNPJ&gt;92660604000182&lt;/CNPJ&gt;&lt;/autXML&gt;&lt;det nItem="1"&gt;&lt;prod&gt;&lt;cProd&gt;1000006142&lt;/cProd&gt;&lt;cEAN&gt;SEM GTIN&lt;/cEAN&gt;&lt;xProd&gt;00 00 60 KCL&lt;/xProd&gt;&lt;NCM&gt;31042090&lt;/NCM&gt;&lt;EXTIPI&gt;000&lt;/EXTIPI&gt;&lt;CFOP&gt;6152&lt;/CFOP&gt;&lt;uCom&gt;TO&lt;/uCom&gt;&lt;qCom&gt;48.0400&lt;/qCom&gt;&lt;vUnCom&gt;2135.3&lt;/vUnCom&gt;&lt;vProd&gt;102579.81&lt;/vProd&gt;&lt;cEANTrib&gt;SEM GTIN&lt;/cEANTrib&gt;&lt;uTrib&gt;TO&lt;/uTrib&gt;&lt;qTrib&gt;48.0400&lt;/qTrib&gt;&lt;vUnTrib&gt;2135.3&lt;/vUnTrib&gt;&lt;indTot&gt;1&lt;/indTot&gt;&lt;xPed&gt;4500713253&lt;/xPed&gt;&lt;/prod&gt;&lt;imposto&gt;&lt;ICMS&gt;&lt;ICMS20&gt;&lt;orig&gt;6&lt;/orig&gt;&lt;CST&gt;20&lt;/CST&gt;&lt;modBC&gt;3&lt;/modBC&gt;&lt;pRedBC&gt;30.00&lt;/pRedBC&gt;&lt;vBC&gt;74487.41&lt;/vBC&gt;&lt;pICMS&gt;12.00&lt;/pICMS&gt;&lt;vICMS&gt;8938.49&lt;/vICMS&gt;&lt;vICMSDeson&gt;3830.78&lt;/vICMSDeson&gt;&lt;motDesICMS&gt;3&lt;/motDesICMS&gt;&lt;/ICMS20&gt;&lt;/ICMS&gt;&lt;IPI&gt;&lt;cEnq&gt;112&lt;/cEnq&gt;&lt;IPINT&gt;&lt;CST&gt;53&lt;/CST&gt;&lt;/IPINT&gt;&lt;/IPI&gt;&lt;PIS&gt;&lt;PISOutr&gt;&lt;CST&gt;49&lt;/CST&gt;&lt;vBC&gt;0.00&lt;/vBC&gt;&lt;pPIS&gt;0.00&lt;/pPIS&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;/PISOutr&gt;&lt;/PIS&gt;&lt;COFINS&gt;&lt;COFINSOutr&gt;&lt;CST&gt;49&lt;/CST&gt;&lt;vBC&gt;0.00&lt;/vBC&gt;&lt;pCOFINS&gt;0.00&lt;/pCOFINS&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;/COFINSOutr&gt;&lt;/COFINS&gt;&lt;/imposto&gt;&lt;infAdProd&gt;CLORETO DE POTASSIO 60% GRANULADO&lt;/infAdProd&gt;&lt;/det&gt;&lt;total&gt;&lt;ICMSTot&gt;&lt;vBC&gt;74487.41&lt;/vBC&gt;&lt;vICMS&gt;8938.49&lt;/vICMS&gt;&lt;vICMSDeson&gt;3830.78&lt;/vICMSDeson&gt;&lt;vFCPUFDest&gt;0.00&lt;/vFCPUFDest&gt;&lt;vICMSUFDest&gt;0.00&lt;/vICMSUFDest&gt;&lt;vICMSUFRemet&gt;0.00&lt;/vICMSUFRemet&gt;&lt;vFCP&gt;0.00&lt;/vFCP&gt;&lt;vBCST&gt;0.00&lt;/vBCST&gt;&lt;vST&gt;0.00&lt;/vST&gt;&lt;vFCPST&gt;0.00&lt;/vFCPST&gt;&lt;vFCPSTRet&gt;0.00&lt;/vFCPSTRet&gt;&lt;vProd&gt;102579.81&lt;/vProd&gt;&lt;vFrete&gt;0.00&lt;/vFrete&gt;&lt;vSeg&gt;0.00&lt;/vSeg&gt;&lt;vDesc&gt;0.00&lt;/vDesc&gt;&lt;vII&gt;0.00&lt;/vII&gt;&lt;vIPI&gt;0.00&lt;/vIPI&gt;&lt;vIPIDevol&gt;0.00&lt;/vIPIDevol&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;vOutro&gt;0.00&lt;/vOutro&gt;&lt;vNF&gt;102579.81&lt;/vNF&gt;&lt;/ICMSTot&gt;&lt;/total&gt;&lt;transp&gt;&lt;modFrete&gt;1&lt;/modFrete&gt;&lt;transporta&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xEnder&gt;AV JOS AUGUSTO CARVALHO 4063&lt;/xEnder&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;/transporta&gt;&lt;vol&gt;&lt;qVol&gt;48&lt;/qVol&gt;&lt;esp&gt;GRANEL&lt;/esp&gt;&lt;marca&gt;00 00 60 KCL&lt;/marca&gt;&lt;nVol&gt;0&lt;/nVol&gt;&lt;pesoL&gt;48040.000&lt;/pesoL&gt;&lt;pesoB&gt;48040.000&lt;/pesoB&gt;&lt;/vol&gt;&lt;/transp&gt;&lt;pag&gt;&lt;detPag&gt;&lt;tPag&gt;01&lt;/tPag&gt;&lt;vPag&gt;102579.81&lt;/vPag&gt;&lt;/detPag&gt;&lt;/pag&gt;&lt;infAdic&gt;&lt;infCpl&gt;BRUTO 49.040 TARA 1.000 LIQUIDO 48.040  CARRETA 2 FNT 3C38  CV FKH 7H31REDUO BASE CLCULO ICMS P 70% NOS TERMOS DO ARTIGO 43, PARTE GERAL, COMBINADO ANEXO IV RICMSMGICMS DISPENSADO E REDUZIDO DO PRECO VL. INTEGRAL X REDUCAO BASE % X ALIQ %  VL DISPENSADO106410.59 X 30.0% X 12.0%  3830.78IPI NAO TRIBUTADO CONFORME CAPITULO 31 DA TIPIRMA PR 000664-5.000073PRODUTO IMPORTADO, ARMAZENAR EM LUGAR SECO, COBERTO E AREJADOMERCADORIA SAIDA DO PORTO DE SANTOS - SANTOSSPPEDIDO 4500713253DATA DE FABRICACAO 22102021 DATA DE VALIDADE 22102023DI 211807687-7, DATA DA DI 21092021, NAVIO SANTA JOHANNA, NR. IMP 0001806I21NR NF MAE 14204, DATA NF MAE 11102021, PEDIDO 4500713253, TIQUETE 0124042021&lt;/infCpl&gt;&lt;obsCont xCampo="NR_NF_MAE"&gt;&lt;xTexto&gt;14204&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NR_PEDIDO"&gt;&lt;xTexto&gt;4500713253&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NR_IMPORTACAO"&gt;&lt;xTexto&gt;0001806I21&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NR_TIQUETE"&gt;&lt;xTexto&gt;0124042021&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NAVIO"&gt;&lt;xTexto&gt;SANTA JOHANNA&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="ITEM_PEDIDO_CLIENTE"&gt;&lt;xTexto&gt;10&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="CD_TIPO_NF"&gt;&lt;xTexto&gt;S&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="CD_OPERACAO"&gt;&lt;xTexto&gt;06&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="CD_EMPRESA"&gt;&lt;xTexto&gt;1196&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;/infAdic&gt;&lt;compra&gt;&lt;xPed&gt;4500713253&lt;/xPed&gt;&lt;/compra&gt;&lt;infRespTec&gt;&lt;CNPJ&gt;11342233000199&lt;/CNPJ&gt;&lt;xContato&gt;Helpdesk&lt;/xContato&gt;&lt;email&gt;helpdesk@micsistemas.com.br&lt;/email&gt;&lt;fone&gt;1340422786&lt;/fone&gt;&lt;/infRespTec&gt;&lt;/infNFe&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#NFe31211092660604015457550760000146171184325883"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;U1ZehQNFqIuSTREdBOniIkHIZRs=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;KN8y1bizwnZwsy+nbw3+MhWklwP1l+S+/b/3zGr4OWO8XzHFlNOd/Zp4PIjRFeRlRW2RG13ds25NRfeb5KZgNVu2fnbJvyyYjDjo+fhgpX+SeUbwtXseXIzXsCy+usgeEVgvGtV8pQPK4PYA5Q8piN9gjA1G42605aN6JZBcccuLFlfZU+25UsmjyY+m+nNFI/HvfTncnXrVGllmQTq0SWi7iZV9RyQ+E45fHn4cLarR4wDBwB8xm8kpAA7tan1HrN9ByenpRDPXuaBjcRgK9Oisz5CywHp90wS3qwtWBfqMZTV/OatTTAY+E2XVJuFFhK4k8DePndWJrN2QclpHeg==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIICzCCBfOgAwIBAgIQNjjNlSyNftb+ED1sesUuPTANBgkqhkiG9w0BAQsFADB4MQswCQYDVQQGEwJCUjETMBEGA1UEChMKSUNQLUJyYXNpbDE2MDQGA1UECxMtU2VjcmV0YXJpYSBkYSBSZWNlaXRhIEZlZGVyYWwgZG8gQnJhc2lsIC0gUkZCMRwwGgYDVQQDExNBQyBDZXJ0aXNpZ24gUkZCIEc1MB4XDTIxMTAwNjE1MDI0M1oXDTIyMTAwNjE1MDI0M1owggEBMQswCQYDVQQGEwJCUjETMBEGA1UECgwKSUNQLUJyYXNpbDELMAkGA1UECAwCUlMxFTATBgNVBAcMDFBvcnRvIEFsZWdyZTEZMBcGA1UECwwQVmlkZW9Db25mZXJlbmNpYTEXMBUGA1UECwwOMTA4NjkwODAwMDAxNzAxNjA0BgNVBAsMLVNlY3JldGFyaWEgZGEgUmVjZWl0YSBGZWRlcmFsIGRvIEJyYXNpbCAtIFJGQjEWMBQGA1UECwwNUkZCIGUtQ05QSiBBMTE1MDMGA1UEAwwsWUFSQSBCUkFTSUwgRkVSVElMSVpBTlRFUyBTIEE6OTI2NjA2MDQwMDAxODIwggEiMA0GCSqGSIb3DQEBAQUAA4IBDwAwggEKAoIBAQCbDkPNSgzXLGqoqumwXPWkcZCj2iP6kjQtBerE4vrBR19Mc4BLYvGZvnniaDYwJxXy3bHVdz/RwGPoblcjEzyYoex7wCZb/1ZVow/wjVOIDt7ekV8sbxZMY0J26o2SXfDhcxMjK6i8v/4Ku9oVIJBPWs4QRT4y0t4Kynub1+Vnb2bVi4bII7gHHE/XXwTv6y1pQOHmHTz2mkO/AX1JqCoIoj7XlRoEEnLyXqblE4cb5Gxi1uCSOcc4O00UOG8Yc83o3uu4LWnbdu7S056YFP6PWlaNqMkFhjIKGssfZZnEhUWfg/JWnkdyV0pS0LLtSLJa1r+BR/98XIWzjfmBc2RbAgMBAAGjggMEMIIDADCBswYDVR0RBIGrMIGooD0GBWBMAQMEoDQEMjI5MDUxOTY5NDk1ODkwOTEwOTEwMDAwMDAwMDAwMDAwMDAwNDAzOTU3NDg1MlNTUFJToCIGBWBMAQMCoBkEF0NMRUlUT04gTUVTUVVJVEEgVkFSR0FToBkGBWBMAQMDoBAEDjkyNjYwNjA0MDAwMTgyoBcGBWBMAQMHoA4EDDAwMDAwMDAwMDAwMIEPZmlzY2FsQHlhcmEuY29tMAkGA1UdEwQCMAAwHwYDVR0jBBgwFoAUU31/nb7RYdAgutqf44mnE3NYzUIwfwYDVR0gBHgwdjB0BgZgTAECAQwwajBoBggrBgEFBQcCARZcaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9kcGMvQUNfQ2VydGlzaWduX1JGQi9EUENfQUNfQ2VydGlzaWduX1JGQi5wZGYwgbwGA1UdHwSBtDCBsTBXoFWgU4ZRaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9sY3IvQUNDZXJ0aXNpZ25SRkJHNS9MYXRlc3RDUkwuY3JsMFagVKBShlBodHRwOi8vaWNwLWJyYXNpbC5vdXRyYWxjci5jb20uYnIvcmVwb3NpdG9yaW8vbGNyL0FDQ2VydGlzaWduUkZCRzUvTGF0ZXN0Q1JMLmNybDAOBgNVHQ8BAf8EBAMCBeAwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGsBggrBgEFBQcBAQSBnzCBnDBfBggrBgEFBQcwAoZTaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9jZXJ0aWZpY2Fkb3MvQUNfQ2VydGlzaWduX1JGQl9HNS5wN2MwOQYIKwYBBQUHMAGGLWh0dHA6Ly9vY3NwLWFjLWNlcnRpc2lnbi1yZmIuY2VydGlzaWduLmNvbS5icjANBgkqhkiG9w0BAQsFAAOCAgEASCNnP1ersGgcFlHfGmfzgtSBVH0oJrVrm7/LFr2FjM8AjX9PY97brv6UubUjswAD+yL+dwwsuv1TxnBHw8AE8MGbxiZQTnNf0OMkIPAEDvwlb8SXK7Gk137JKUaKKGup5P4dbA8XM22+GEw1dMYjCV6eqJ2bxP1EjRII3rb8EsQATZ/pDizsEauNXOmXqbIefqU9wWaQhTQVtLwflrN0zElGDSX9uwtR6j28usr3KiKf26MfhtWDAombY+m9Bhq2Hys6hZpyfL+ERFoWXmpzlhmEvUFnMzL1SWGNeyhn+na7r7cJvBFcdPPyriZlAdApkaZGXSQAGW78gvlJLD2YtYk/BN02v7qCfhcPHdZcQ4XVkdj8idIMcn3ZiweWanaZ9riR3yLStxBP7arsQrMGOrYkAyo9otufpJfYS+FHkrJapqfZxbo0qCTsZPHvAcMw8vCojT/Z2FZrGi6aDK2rt7hPhKYRedZNbDmVgKSRNBoyPqSoqNwMSEiF7EmXA5zq27SM87v096EsX8COhgxvMqj/ENxfj8x94POwH8gif/xv9r/raWYCrOnKNP8uhXJPdeihFZBsbWanSUZWYlltN/lCaF/oSDqsQjVaG4MndtddEIwdfk3xg71iptYN1tYWHSMal0EwKkOA3A9obwTtxz1fkp8FnGxIgi6QuCLfPTU=&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/NFe&gt;&lt;protNFe versao="4.00"&gt;&lt;infProt Id="ID131214398270580"&gt;
   &lt;tpAmb&gt;1&lt;/tpAmb&gt;
-  &lt;verAplic&gt;14.4.46-SE4&lt;/verAplic&gt;
-  &lt;chNFe&gt;31211292660604017662550500000170671478739470&lt;/chNFe&gt;
-  &lt;dhRecbto&gt;2021-12-21T18:48:22-03:00&lt;/dhRecbto&gt;
-  &lt;nProt&gt;131214496666445&lt;/nProt&gt;
-  &lt;digVal&gt;0D2xAMxnjkdWPu4d3xsRIxVX0hc=&lt;/digVal&gt;
+  &lt;verAplic&gt;14.4.34-HA1&lt;/verAplic&gt;
+  &lt;chNFe&gt;31211092660604015457550760000146171184325883&lt;/chNFe&gt;
+  &lt;dhRecbto&gt;2021-10-22T21:09:30-03:00&lt;/dhRecbto&gt;
+  &lt;nProt&gt;131214398270580&lt;/nProt&gt;
+  &lt;digVal&gt;U1ZehQNFqIuSTREdBOniIkHIZRs=&lt;/digVal&gt;
   &lt;cStat&gt;100&lt;/cStat&gt;
   &lt;xMotivo&gt;Autorizado o uso da NF-e&lt;/xMotivo&gt;
 &lt;/infProt&gt;&lt;/protNFe&gt;&lt;/nfeProc&gt;</x:t>
   </x:si>
   <x:si>
-    <x:t>31211292660604017662550500000170691908499198.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\31211292660604017662550500000170691908499198.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;nfeProc versao="4.00" xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;NFe xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;infNFe Id="NFe31211292660604017662550500000170691908499198" versao="4.00"&gt;&lt;ide&gt;&lt;cUF&gt;31&lt;/cUF&gt;&lt;cNF&gt;90849919&lt;/cNF&gt;&lt;natOp&gt;Remessa p/ deposito fechado ou arm.geral&lt;/natOp&gt;&lt;mod&gt;55&lt;/mod&gt;&lt;serie&gt;50&lt;/serie&gt;&lt;nNF&gt;17069&lt;/nNF&gt;&lt;dhEmi&gt;2021-12-21T19:06:39-03:00&lt;/dhEmi&gt;&lt;tpNF&gt;1&lt;/tpNF&gt;&lt;idDest&gt;2&lt;/idDest&gt;&lt;cMunFG&gt;3166808&lt;/cMunFG&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;8&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;finNFe&gt;1&lt;/finNFe&gt;&lt;indFinal&gt;0&lt;/indFinal&gt;&lt;indPres&gt;9&lt;/indPres&gt;&lt;indIntermed&gt;0&lt;/indIntermed&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;SAP NFE 4.00&lt;/verProc&gt;&lt;/ide&gt;&lt;emit&gt;&lt;CNPJ&gt;92660604017662&lt;/CNPJ&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;xFant&gt;CMISS-Compl.Min.Indl.S Salitre&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;Fazenda Salitre&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;Marrua&lt;/xBairro&gt;&lt;cMun&gt;3166808&lt;/cMun&gt;&lt;xMun&gt;Serra do Salitre&lt;/xMun&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;CEP&gt;38760000&lt;/CEP&gt;&lt;xPais&gt;Brasil&lt;/xPais&gt;&lt;/enderEmit&gt;&lt;IE&gt;2874585321020&lt;/IE&gt;&lt;CRT&gt;3&lt;/CRT&gt;&lt;/emit&gt;&lt;dest&gt;&lt;CNPJ&gt;06225292000147&lt;/CNPJ&gt;&lt;xNome&gt;TERLOC TERMINAL LOGISTICO CESARI LT DA&lt;/xNome&gt;&lt;enderDest&gt;&lt;xLgr&gt;EST ENGENHEIRO PLINIO DE QUEIROZ&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xCpl&gt;SP 55&lt;/xCpl&gt;&lt;xBairro&gt;PIACAGUERA&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;CUBATAO&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;CEP&gt;11570000&lt;/CEP&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;Brasil&lt;/xPais&gt;&lt;/enderDest&gt;&lt;indIEDest&gt;1&lt;/indIEDest&gt;&lt;IE&gt;283108491118&lt;/IE&gt;&lt;email&gt;expedicao@terloc.com.br&lt;/email&gt;&lt;/dest&gt;&lt;det nItem="1"&gt;&lt;prod&gt;&lt;cProd&gt;1000011243&lt;/cProd&gt;&lt;cEAN&gt;SEM GTIN&lt;/cEAN&gt;&lt;xProd&gt;CONCENTRADO FOSFATICO GROSSO UMIDO CMISS&lt;/xProd&gt;&lt;NCM&gt;25102010&lt;/NCM&gt;&lt;EXTIPI&gt;10&lt;/EXTIPI&gt;&lt;CFOP&gt;6905&lt;/CFOP&gt;&lt;uCom&gt;TO&lt;/uCom&gt;&lt;qCom&gt;47.6700&lt;/qCom&gt;&lt;vUnCom&gt;1194.5200335641&lt;/vUnCom&gt;&lt;vProd&gt;56942.77&lt;/vProd&gt;&lt;cEANTrib&gt;SEM GTIN&lt;/cEANTrib&gt;&lt;uTrib&gt;TO&lt;/uTrib&gt;&lt;qTrib&gt;47.6700&lt;/qTrib&gt;&lt;vUnTrib&gt;1194.5200335641&lt;/vUnTrib&gt;&lt;indTot&gt;1&lt;/indTot&gt;&lt;/prod&gt;&lt;imposto&gt;&lt;ICMS&gt;&lt;ICMS20&gt;&lt;orig&gt;0&lt;/orig&gt;&lt;CST&gt;20&lt;/CST&gt;&lt;modBC&gt;3&lt;/modBC&gt;&lt;pRedBC&gt;99.6000&lt;/pRedBC&gt;&lt;vBC&gt;24544.30&lt;/vBC&gt;&lt;pICMS&gt;12.0000&lt;/pICMS&gt;&lt;vICMS&gt;2945.32&lt;/vICMS&gt;&lt;/ICMS20&gt;&lt;/ICMS&gt;&lt;IPI&gt;&lt;cEnq&gt;103&lt;/cEnq&gt;&lt;IPINT&gt;&lt;CST&gt;55&lt;/CST&gt;&lt;/IPINT&gt;&lt;/IPI&gt;&lt;PIS&gt;&lt;PISOutr&gt;&lt;CST&gt;49&lt;/CST&gt;&lt;qBCProd&gt;47.6700&lt;/qBCProd&gt;&lt;vAliqProd&gt;0.0000&lt;/vAliqProd&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;/PISOutr&gt;&lt;/PIS&gt;&lt;COFINS&gt;&lt;COFINSOutr&gt;&lt;CST&gt;49&lt;/CST&gt;&lt;qBCProd&gt;47.6700&lt;/qBCProd&gt;&lt;vAliqProd&gt;0.0000&lt;/vAliqProd&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;/COFINSOutr&gt;&lt;/COFINS&gt;&lt;/imposto&gt;&lt;infAdProd&gt;Base de calculo reduzida em 60 cfe RICMSMG2002, Art. 43 cc Anexo IV, Item 8, b. IPI suspenso nos termos do RIPI, Decreto 7.21210, Art. 43, III. Nao incidencia de COFINS cfe. Lei 10.83303, art. 1o Nao incidencia de PIS cfe. Lei 10.83303, art. 1o&lt;/infAdProd&gt;&lt;/det&gt;&lt;total&gt;&lt;ICMSTot&gt;&lt;vBC&gt;24544.30&lt;/vBC&gt;&lt;vICMS&gt;2945.32&lt;/vICMS&gt;&lt;vICMSDeson&gt;0.00&lt;/vICMSDeson&gt;&lt;vFCP&gt;0.00&lt;/vFCP&gt;&lt;vBCST&gt;0.00&lt;/vBCST&gt;&lt;vST&gt;0.00&lt;/vST&gt;&lt;vFCPST&gt;0.00&lt;/vFCPST&gt;&lt;vFCPSTRet&gt;0.00&lt;/vFCPSTRet&gt;&lt;vProd&gt;56942.77&lt;/vProd&gt;&lt;vFrete&gt;0.00&lt;/vFrete&gt;&lt;vSeg&gt;0.00&lt;/vSeg&gt;&lt;vDesc&gt;0.00&lt;/vDesc&gt;&lt;vII&gt;0.00&lt;/vII&gt;&lt;vIPI&gt;0.00&lt;/vIPI&gt;&lt;vIPIDevol&gt;0.00&lt;/vIPIDevol&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;vOutro&gt;0.00&lt;/vOutro&gt;&lt;vNF&gt;56942.77&lt;/vNF&gt;&lt;/ICMSTot&gt;&lt;/total&gt;&lt;transp&gt;&lt;modFrete&gt;0&lt;/modFrete&gt;&lt;transporta&gt;&lt;CNPJ&gt;50505924000703&lt;/CNPJ&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA FILIAL&lt;/xNome&gt;&lt;xEnder&gt;FILOMENA CARTAFINA 22031&lt;/xEnder&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;/transporta&gt;&lt;vol&gt;&lt;qVol&gt;48&lt;/qVol&gt;&lt;esp&gt;GRANEL&lt;/esp&gt;&lt;marca&gt;YARA&lt;/marca&gt;&lt;pesoL&gt;47670.000&lt;/pesoL&gt;&lt;pesoB&gt;47670.000&lt;/pesoB&gt;&lt;/vol&gt;&lt;/transp&gt;&lt;pag&gt;&lt;detPag&gt;&lt;indPag&gt;0&lt;/indPag&gt;&lt;tPag&gt;15&lt;/tPag&gt;&lt;vPag&gt;56942.77&lt;/vPag&gt;&lt;/detPag&gt;&lt;/pag&gt;&lt;infAdic&gt;&lt;infCpl&gt;Ordem de venda n 0000623925 Ordem de Carregamento 0003109530 Base de calculo reduzida em 60 cfe RICMSMG2002 Art 43 cc Anexo IV Item 8 b IPI suspenso nos termos do RIPI Decreto 721210 Art 43 III Nao incidencia de COFINS cfe Lei 1083303 art 1o Nao incidencia de PIS cfe Lei 1083303 art 1o REGISTRO MAPA NAO SE APLICA Data de fabricacao 21122021 Origem INDUSTRIA BRASILEIRA Classificacao Quimica Modo de aplicacao NA Armazenar sempre sobre piso seco com boa drenagem e em local coberto Para outras condicoes consultar a Yara Brasil Uso exclusivo como fertilizante Prezado Cliente Observacoes sobre carga recebida anotar no verso do canhoto da NF Em caso de emergencia ligue para 08007708899 Remessa 0082307409 A Ficha de Informacoes de Seguranca de Produtos Quimicos pode ser obtida por meio do site wwwyarabrasilcombr&lt;/infCpl&gt;&lt;/infAdic&gt;&lt;/infNFe&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#NFe31211292660604017662550500000170691908499198"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;mkKWkj2SymVXik3DMRRvKl3HtIE=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;PUUgugihzEtMHHs50dBpVZEQhvBiH0Dxh7zwwfJawbLM8Q0rh3hc39bj62d9TUDM61cklWR22QvP
-fGYuQzV1UOuc/XyXP0KJk0MEBedvPlGtO0q38y02/iWnLPHKDXVk7Mwh9664tOKKyKvrPbgO4JBf
-8elpYtw/cbs6ndZrhjBd9a18iyUV0kfDACYJmSJbliWMDnnyRIjWXnGI8oumQjoUT18puh7uczOB
-f+ifW6YJQqkj6SOx+Y9OP5EnbZmb0HZCrfMU4+XLumi2nXEDB8sdm7k7pEM8YOaylgYFPfUYJvFq
-1sJ+YtXihp9sgKxuYDc7djEus9JOOfXPIzJ/6g==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIICzCCBfOgAwIBAgIQNjjNlSyNftb+ED1sesUuPTANBgkqhkiG9w0BAQsFADB4MQswCQYDVQQG
-EwJCUjETMBEGA1UEChMKSUNQLUJyYXNpbDE2MDQGA1UECxMtU2VjcmV0YXJpYSBkYSBSZWNlaXRh
-IEZlZGVyYWwgZG8gQnJhc2lsIC0gUkZCMRwwGgYDVQQDExNBQyBDZXJ0aXNpZ24gUkZCIEc1MB4X
-DTIxMTAwNjE1MDI0M1oXDTIyMTAwNjE1MDI0M1owggEBMQswCQYDVQQGEwJCUjETMBEGA1UECgwK
-SUNQLUJyYXNpbDELMAkGA1UECAwCUlMxFTATBgNVBAcMDFBvcnRvIEFsZWdyZTEZMBcGA1UECwwQ
-VmlkZW9Db25mZXJlbmNpYTEXMBUGA1UECwwOMTA4NjkwODAwMDAxNzAxNjA0BgNVBAsMLVNlY3Jl
-dGFyaWEgZGEgUmVjZWl0YSBGZWRlcmFsIGRvIEJyYXNpbCAtIFJGQjEWMBQGA1UECwwNUkZCIGUt
-Q05QSiBBMTE1MDMGA1UEAwwsWUFSQSBCUkFTSUwgRkVSVElMSVpBTlRFUyBTIEE6OTI2NjA2MDQw
-MDAxODIwggEiMA0GCSqGSIb3DQEBAQUAA4IBDwAwggEKAoIBAQCbDkPNSgzXLGqoqumwXPWkcZCj
-2iP6kjQtBerE4vrBR19Mc4BLYvGZvnniaDYwJxXy3bHVdz/RwGPoblcjEzyYoex7wCZb/1ZVow/w
-jVOIDt7ekV8sbxZMY0J26o2SXfDhcxMjK6i8v/4Ku9oVIJBPWs4QRT4y0t4Kynub1+Vnb2bVi4bI
-I7gHHE/XXwTv6y1pQOHmHTz2mkO/AX1JqCoIoj7XlRoEEnLyXqblE4cb5Gxi1uCSOcc4O00UOG8Y
-c83o3uu4LWnbdu7S056YFP6PWlaNqMkFhjIKGssfZZnEhUWfg/JWnkdyV0pS0LLtSLJa1r+BR/98
-XIWzjfmBc2RbAgMBAAGjggMEMIIDADCBswYDVR0RBIGrMIGooD0GBWBMAQMEoDQEMjI5MDUxOTY5
-NDk1ODkwOTEwOTEwMDAwMDAwMDAwMDAwMDAwNDAzOTU3NDg1MlNTUFJToCIGBWBMAQMCoBkEF0NM
-RUlUT04gTUVTUVVJVEEgVkFSR0FToBkGBWBMAQMDoBAEDjkyNjYwNjA0MDAwMTgyoBcGBWBMAQMH
-oA4EDDAwMDAwMDAwMDAwMIEPZmlzY2FsQHlhcmEuY29tMAkGA1UdEwQCMAAwHwYDVR0jBBgwFoAU
-U31/nb7RYdAgutqf44mnE3NYzUIwfwYDVR0gBHgwdjB0BgZgTAECAQwwajBoBggrBgEFBQcCARZc
-aHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9kcGMvQUNfQ2Vy
-dGlzaWduX1JGQi9EUENfQUNfQ2VydGlzaWduX1JGQi5wZGYwgbwGA1UdHwSBtDCBsTBXoFWgU4ZR
-aHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9sY3IvQUNDZXJ0
-aXNpZ25SRkJHNS9MYXRlc3RDUkwuY3JsMFagVKBShlBodHRwOi8vaWNwLWJyYXNpbC5vdXRyYWxj
-ci5jb20uYnIvcmVwb3NpdG9yaW8vbGNyL0FDQ2VydGlzaWduUkZCRzUvTGF0ZXN0Q1JMLmNybDAO
-BgNVHQ8BAf8EBAMCBeAwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGsBggrBgEFBQcB
-AQSBnzCBnDBfBggrBgEFBQcwAoZTaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9y
-ZXBvc2l0b3Jpby9jZXJ0aWZpY2Fkb3MvQUNfQ2VydGlzaWduX1JGQl9HNS5wN2MwOQYIKwYBBQUH
-MAGGLWh0dHA6Ly9vY3NwLWFjLWNlcnRpc2lnbi1yZmIuY2VydGlzaWduLmNvbS5icjANBgkqhkiG
-9w0BAQsFAAOCAgEASCNnP1ersGgcFlHfGmfzgtSBVH0oJrVrm7/LFr2FjM8AjX9PY97brv6UubUj
-swAD+yL+dwwsuv1TxnBHw8AE8MGbxiZQTnNf0OMkIPAEDvwlb8SXK7Gk137JKUaKKGup5P4dbA8X
-M22+GEw1dMYjCV6eqJ2bxP1EjRII3rb8EsQATZ/pDizsEauNXOmXqbIefqU9wWaQhTQVtLwflrN0
-zElGDSX9uwtR6j28usr3KiKf26MfhtWDAombY+m9Bhq2Hys6hZpyfL+ERFoWXmpzlhmEvUFnMzL1
-SWGNeyhn+na7r7cJvBFcdPPyriZlAdApkaZGXSQAGW78gvlJLD2YtYk/BN02v7qCfhcPHdZcQ4XV
-kdj8idIMcn3ZiweWanaZ9riR3yLStxBP7arsQrMGOrYkAyo9otufpJfYS+FHkrJapqfZxbo0qCTs
-ZPHvAcMw8vCojT/Z2FZrGi6aDK2rt7hPhKYRedZNbDmVgKSRNBoyPqSoqNwMSEiF7EmXA5zq27SM
-87v096EsX8COhgxvMqj/ENxfj8x94POwH8gif/xv9r/raWYCrOnKNP8uhXJPdeihFZBsbWanSUZW
-YlltN/lCaF/oSDqsQjVaG4MndtddEIwdfk3xg71iptYN1tYWHSMal0EwKkOA3A9obwTtxz1fkp8F
-nGxIgi6QuCLfPTU=&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/NFe&gt;&lt;protNFe versao="4.00"&gt;&lt;infProt Id="ID131214496702999"&gt;
+    <x:t>31211092660604015457550760000146221569723315.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\31211092660604015457550760000146221569723315.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;nfeProc versao="4.00" xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;NFe xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;infNFe Id="NFe31211092660604015457550760000146221569723315" versao="4.00"&gt;&lt;ide&gt;&lt;cUF&gt;31&lt;/cUF&gt;&lt;cNF&gt;56972331&lt;/cNF&gt;&lt;natOp&gt;TRANSFERNCIA&lt;/natOp&gt;&lt;mod&gt;55&lt;/mod&gt;&lt;serie&gt;76&lt;/serie&gt;&lt;nNF&gt;14622&lt;/nNF&gt;&lt;dhEmi&gt;2021-10-22T21:27:37-03:00&lt;/dhEmi&gt;&lt;dhSaiEnt&gt;2021-10-22T21:27:37-03:00&lt;/dhSaiEnt&gt;&lt;tpNF&gt;1&lt;/tpNF&gt;&lt;idDest&gt;2&lt;/idDest&gt;&lt;cMunFG&gt;3170107&lt;/cMunFG&gt;&lt;tpImp&gt;2&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;5&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;finNFe&gt;1&lt;/finNFe&gt;&lt;indFinal&gt;0&lt;/indFinal&gt;&lt;indPres&gt;9&lt;/indPres&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;200&lt;/verProc&gt;&lt;/ide&gt;&lt;emit&gt;&lt;CNPJ&gt;92660604015457&lt;/CNPJ&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES SA&lt;/xNome&gt;&lt;xFant&gt;YARA BRASIL FERTILIZANTES SA&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA ANTONIO CARLOS GUILLAUMON 800&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;CEP&gt;38044760&lt;/CEP&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;fone&gt;3433197198&lt;/fone&gt;&lt;/enderEmit&gt;&lt;IE&gt;3714585320678&lt;/IE&gt;&lt;CRT&gt;3&lt;/CRT&gt;&lt;/emit&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604013756&lt;/CNPJ&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES SA&lt;/xNome&gt;&lt;enderDest&gt;&lt;xLgr&gt;AVENIDA SAO JUDAS TADEU&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;JARDIM SAO JUDAS TAD&lt;/xBairro&gt;&lt;cMun&gt;3552403&lt;/cMun&gt;&lt;xMun&gt;SUMARE&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;CEP&gt;13180570&lt;/CEP&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;fone&gt;0000000000&lt;/fone&gt;&lt;/enderDest&gt;&lt;indIEDest&gt;1&lt;/indIEDest&gt;&lt;IE&gt;671143732119&lt;/IE&gt;&lt;/dest&gt;&lt;retirada&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;xLgr&gt;AV. CONS. RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;/retirada&gt;&lt;autXML&gt;&lt;CNPJ&gt;55681274000185&lt;/CNPJ&gt;&lt;/autXML&gt;&lt;autXML&gt;&lt;CNPJ&gt;92660604000182&lt;/CNPJ&gt;&lt;/autXML&gt;&lt;det nItem="1"&gt;&lt;prod&gt;&lt;cProd&gt;1000006142&lt;/cProd&gt;&lt;cEAN&gt;SEM GTIN&lt;/cEAN&gt;&lt;xProd&gt;00 00 60 KCL&lt;/xProd&gt;&lt;NCM&gt;31042090&lt;/NCM&gt;&lt;EXTIPI&gt;000&lt;/EXTIPI&gt;&lt;CFOP&gt;6152&lt;/CFOP&gt;&lt;uCom&gt;TO&lt;/uCom&gt;&lt;qCom&gt;47.9200&lt;/qCom&gt;&lt;vUnCom&gt;2135.3&lt;/vUnCom&gt;&lt;vProd&gt;102323.58&lt;/vProd&gt;&lt;cEANTrib&gt;SEM GTIN&lt;/cEANTrib&gt;&lt;uTrib&gt;TO&lt;/uTrib&gt;&lt;qTrib&gt;47.9200&lt;/qTrib&gt;&lt;vUnTrib&gt;2135.3&lt;/vUnTrib&gt;&lt;indTot&gt;1&lt;/indTot&gt;&lt;xPed&gt;4500713253&lt;/xPed&gt;&lt;/prod&gt;&lt;imposto&gt;&lt;ICMS&gt;&lt;ICMS20&gt;&lt;orig&gt;6&lt;/orig&gt;&lt;CST&gt;20&lt;/CST&gt;&lt;modBC&gt;3&lt;/modBC&gt;&lt;pRedBC&gt;30.00&lt;/pRedBC&gt;&lt;vBC&gt;74301.35&lt;/vBC&gt;&lt;pICMS&gt;12.00&lt;/pICMS&gt;&lt;vICMS&gt;8916.16&lt;/vICMS&gt;&lt;vICMSDeson&gt;3821.21&lt;/vICMSDeson&gt;&lt;motDesICMS&gt;3&lt;/motDesICMS&gt;&lt;/ICMS20&gt;&lt;/ICMS&gt;&lt;IPI&gt;&lt;cEnq&gt;112&lt;/cEnq&gt;&lt;IPINT&gt;&lt;CST&gt;53&lt;/CST&gt;&lt;/IPINT&gt;&lt;/IPI&gt;&lt;PIS&gt;&lt;PISOutr&gt;&lt;CST&gt;49&lt;/CST&gt;&lt;vBC&gt;0.00&lt;/vBC&gt;&lt;pPIS&gt;0.00&lt;/pPIS&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;/PISOutr&gt;&lt;/PIS&gt;&lt;COFINS&gt;&lt;COFINSOutr&gt;&lt;CST&gt;49&lt;/CST&gt;&lt;vBC&gt;0.00&lt;/vBC&gt;&lt;pCOFINS&gt;0.00&lt;/pCOFINS&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;/COFINSOutr&gt;&lt;/COFINS&gt;&lt;/imposto&gt;&lt;infAdProd&gt;CLORETO DE POTASSIO 60% GRANULADO&lt;/infAdProd&gt;&lt;/det&gt;&lt;total&gt;&lt;ICMSTot&gt;&lt;vBC&gt;74301.35&lt;/vBC&gt;&lt;vICMS&gt;8916.16&lt;/vICMS&gt;&lt;vICMSDeson&gt;3821.21&lt;/vICMSDeson&gt;&lt;vFCPUFDest&gt;0.00&lt;/vFCPUFDest&gt;&lt;vICMSUFDest&gt;0.00&lt;/vICMSUFDest&gt;&lt;vICMSUFRemet&gt;0.00&lt;/vICMSUFRemet&gt;&lt;vFCP&gt;0.00&lt;/vFCP&gt;&lt;vBCST&gt;0.00&lt;/vBCST&gt;&lt;vST&gt;0.00&lt;/vST&gt;&lt;vFCPST&gt;0.00&lt;/vFCPST&gt;&lt;vFCPSTRet&gt;0.00&lt;/vFCPSTRet&gt;&lt;vProd&gt;102323.58&lt;/vProd&gt;&lt;vFrete&gt;0.00&lt;/vFrete&gt;&lt;vSeg&gt;0.00&lt;/vSeg&gt;&lt;vDesc&gt;0.00&lt;/vDesc&gt;&lt;vII&gt;0.00&lt;/vII&gt;&lt;vIPI&gt;0.00&lt;/vIPI&gt;&lt;vIPIDevol&gt;0.00&lt;/vIPIDevol&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;vOutro&gt;0.00&lt;/vOutro&gt;&lt;vNF&gt;102323.58&lt;/vNF&gt;&lt;/ICMSTot&gt;&lt;/total&gt;&lt;transp&gt;&lt;modFrete&gt;1&lt;/modFrete&gt;&lt;transporta&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xEnder&gt;AV JOS AUGUSTO CARVALHO 4063&lt;/xEnder&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;/transporta&gt;&lt;vol&gt;&lt;qVol&gt;48&lt;/qVol&gt;&lt;esp&gt;GRANEL&lt;/esp&gt;&lt;marca&gt;00 00 60 KCL&lt;/marca&gt;&lt;nVol&gt;0&lt;/nVol&gt;&lt;pesoL&gt;47920.000&lt;/pesoL&gt;&lt;pesoB&gt;47920.000&lt;/pesoB&gt;&lt;/vol&gt;&lt;/transp&gt;&lt;pag&gt;&lt;detPag&gt;&lt;tPag&gt;01&lt;/tPag&gt;&lt;vPag&gt;102323.58&lt;/vPag&gt;&lt;/detPag&gt;&lt;/pag&gt;&lt;infAdic&gt;&lt;infCpl&gt;BRUTO 48.920 TARA 1.000 LIQUIDO 47.920  CARRETA 2 CFP 2B93  CV EBX 6139REDUO BASE CLCULO ICMS P 70% NOS TERMOS DO ARTIGO 43, PARTE GERAL, COMBINADO ANEXO IV RICMSMGICMS DISPENSADO E REDUZIDO DO PRECO VL. INTEGRAL X REDUCAO BASE % X ALIQ %  VL DISPENSADO106144.79 X 30.0% X 12.0%  3821.21IPI NAO TRIBUTADO CONFORME CAPITULO 31 DA TIPIRMA PR 000664-5.000073PRODUTO IMPORTADO, ARMAZENAR EM LUGAR SECO, COBERTO E AREJADOMERCADORIA SAIDA DO PORTO DE SANTOS - SANTOSSPPEDIDO 4500713253DATA DE FABRICACAO 22102021 DATA DE VALIDADE 22102023DI 211807687-7, DATA DA DI 21092021, NAVIO SANTA JOHANNA, NR. IMP 0001806I21NR NF MAE 14204, DATA NF MAE 11102021, PEDIDO 4500713253, TIQUETE 0124192021&lt;/infCpl&gt;&lt;obsCont xCampo="NR_NF_MAE"&gt;&lt;xTexto&gt;14204&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NR_PEDIDO"&gt;&lt;xTexto&gt;4500713253&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NR_IMPORTACAO"&gt;&lt;xTexto&gt;0001806I21&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NR_TIQUETE"&gt;&lt;xTexto&gt;0124192021&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NAVIO"&gt;&lt;xTexto&gt;SANTA JOHANNA&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="ITEM_PEDIDO_CLIENTE"&gt;&lt;xTexto&gt;10&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="CD_TIPO_NF"&gt;&lt;xTexto&gt;S&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="CD_OPERACAO"&gt;&lt;xTexto&gt;06&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="CD_EMPRESA"&gt;&lt;xTexto&gt;1196&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;/infAdic&gt;&lt;compra&gt;&lt;xPed&gt;4500713253&lt;/xPed&gt;&lt;/compra&gt;&lt;infRespTec&gt;&lt;CNPJ&gt;11342233000199&lt;/CNPJ&gt;&lt;xContato&gt;Helpdesk&lt;/xContato&gt;&lt;email&gt;helpdesk@micsistemas.com.br&lt;/email&gt;&lt;fone&gt;1340422786&lt;/fone&gt;&lt;/infRespTec&gt;&lt;/infNFe&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#NFe31211092660604015457550760000146221569723315"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;rm110vN04DtVARrQD2vv6pxqQfw=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;SXtSxl4X9BX1XQ/zcUK3mrPeWsbgainGkasLLuvnk+2nu6Mpm6ZZ65RQnJzcwNNJjtYR08RrItubB3sRt16jyCZUJwQhZnUGhPjPaAx6+WLOIe4OB5a0Of6OgzrYRW6QTVwQLYaFMzBY4qCpL3FKB3M7tmYRmEW6upylJd7MNFhmUaNb+YPesPcPH/O5sbfW3h21/VNs9qQGIovokkwBEFLHK3o6ooRj04WwZAtZ/1zFtaNpV+XkQFlHxIJKQ2gGlCYE/PrekV63X7aX3pl6B0h0mfoijCN7wVw/d3qD2qOeyi4kWf9UdsjFeqv30t9RugYXjhZWbryJieJxh+/6Mw==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIICzCCBfOgAwIBAgIQNjjNlSyNftb+ED1sesUuPTANBgkqhkiG9w0BAQsFADB4MQswCQYDVQQGEwJCUjETMBEGA1UEChMKSUNQLUJyYXNpbDE2MDQGA1UECxMtU2VjcmV0YXJpYSBkYSBSZWNlaXRhIEZlZGVyYWwgZG8gQnJhc2lsIC0gUkZCMRwwGgYDVQQDExNBQyBDZXJ0aXNpZ24gUkZCIEc1MB4XDTIxMTAwNjE1MDI0M1oXDTIyMTAwNjE1MDI0M1owggEBMQswCQYDVQQGEwJCUjETMBEGA1UECgwKSUNQLUJyYXNpbDELMAkGA1UECAwCUlMxFTATBgNVBAcMDFBvcnRvIEFsZWdyZTEZMBcGA1UECwwQVmlkZW9Db25mZXJlbmNpYTEXMBUGA1UECwwOMTA4NjkwODAwMDAxNzAxNjA0BgNVBAsMLVNlY3JldGFyaWEgZGEgUmVjZWl0YSBGZWRlcmFsIGRvIEJyYXNpbCAtIFJGQjEWMBQGA1UECwwNUkZCIGUtQ05QSiBBMTE1MDMGA1UEAwwsWUFSQSBCUkFTSUwgRkVSVElMSVpBTlRFUyBTIEE6OTI2NjA2MDQwMDAxODIwggEiMA0GCSqGSIb3DQEBAQUAA4IBDwAwggEKAoIBAQCbDkPNSgzXLGqoqumwXPWkcZCj2iP6kjQtBerE4vrBR19Mc4BLYvGZvnniaDYwJxXy3bHVdz/RwGPoblcjEzyYoex7wCZb/1ZVow/wjVOIDt7ekV8sbxZMY0J26o2SXfDhcxMjK6i8v/4Ku9oVIJBPWs4QRT4y0t4Kynub1+Vnb2bVi4bII7gHHE/XXwTv6y1pQOHmHTz2mkO/AX1JqCoIoj7XlRoEEnLyXqblE4cb5Gxi1uCSOcc4O00UOG8Yc83o3uu4LWnbdu7S056YFP6PWlaNqMkFhjIKGssfZZnEhUWfg/JWnkdyV0pS0LLtSLJa1r+BR/98XIWzjfmBc2RbAgMBAAGjggMEMIIDADCBswYDVR0RBIGrMIGooD0GBWBMAQMEoDQEMjI5MDUxOTY5NDk1ODkwOTEwOTEwMDAwMDAwMDAwMDAwMDAwNDAzOTU3NDg1MlNTUFJToCIGBWBMAQMCoBkEF0NMRUlUT04gTUVTUVVJVEEgVkFSR0FToBkGBWBMAQMDoBAEDjkyNjYwNjA0MDAwMTgyoBcGBWBMAQMHoA4EDDAwMDAwMDAwMDAwMIEPZmlzY2FsQHlhcmEuY29tMAkGA1UdEwQCMAAwHwYDVR0jBBgwFoAUU31/nb7RYdAgutqf44mnE3NYzUIwfwYDVR0gBHgwdjB0BgZgTAECAQwwajBoBggrBgEFBQcCARZcaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9kcGMvQUNfQ2VydGlzaWduX1JGQi9EUENfQUNfQ2VydGlzaWduX1JGQi5wZGYwgbwGA1UdHwSBtDCBsTBXoFWgU4ZRaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9sY3IvQUNDZXJ0aXNpZ25SRkJHNS9MYXRlc3RDUkwuY3JsMFagVKBShlBodHRwOi8vaWNwLWJyYXNpbC5vdXRyYWxjci5jb20uYnIvcmVwb3NpdG9yaW8vbGNyL0FDQ2VydGlzaWduUkZCRzUvTGF0ZXN0Q1JMLmNybDAOBgNVHQ8BAf8EBAMCBeAwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGsBggrBgEFBQcBAQSBnzCBnDBfBggrBgEFBQcwAoZTaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9jZXJ0aWZpY2Fkb3MvQUNfQ2VydGlzaWduX1JGQl9HNS5wN2MwOQYIKwYBBQUHMAGGLWh0dHA6Ly9vY3NwLWFjLWNlcnRpc2lnbi1yZmIuY2VydGlzaWduLmNvbS5icjANBgkqhkiG9w0BAQsFAAOCAgEASCNnP1ersGgcFlHfGmfzgtSBVH0oJrVrm7/LFr2FjM8AjX9PY97brv6UubUjswAD+yL+dwwsuv1TxnBHw8AE8MGbxiZQTnNf0OMkIPAEDvwlb8SXK7Gk137JKUaKKGup5P4dbA8XM22+GEw1dMYjCV6eqJ2bxP1EjRII3rb8EsQATZ/pDizsEauNXOmXqbIefqU9wWaQhTQVtLwflrN0zElGDSX9uwtR6j28usr3KiKf26MfhtWDAombY+m9Bhq2Hys6hZpyfL+ERFoWXmpzlhmEvUFnMzL1SWGNeyhn+na7r7cJvBFcdPPyriZlAdApkaZGXSQAGW78gvlJLD2YtYk/BN02v7qCfhcPHdZcQ4XVkdj8idIMcn3ZiweWanaZ9riR3yLStxBP7arsQrMGOrYkAyo9otufpJfYS+FHkrJapqfZxbo0qCTsZPHvAcMw8vCojT/Z2FZrGi6aDK2rt7hPhKYRedZNbDmVgKSRNBoyPqSoqNwMSEiF7EmXA5zq27SM87v096EsX8COhgxvMqj/ENxfj8x94POwH8gif/xv9r/raWYCrOnKNP8uhXJPdeihFZBsbWanSUZWYlltN/lCaF/oSDqsQjVaG4MndtddEIwdfk3xg71iptYN1tYWHSMal0EwKkOA3A9obwTtxz1fkp8FnGxIgi6QuCLfPTU=&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/NFe&gt;&lt;protNFe versao="4.00"&gt;&lt;infProt Id="ID131214398295525"&gt;
   &lt;tpAmb&gt;1&lt;/tpAmb&gt;
-  &lt;verAplic&gt;14.4.46-AP5&lt;/verAplic&gt;
-  &lt;chNFe&gt;31211292660604017662550500000170691908499198&lt;/chNFe&gt;
-  &lt;dhRecbto&gt;2021-12-21T19:06:54-03:00&lt;/dhRecbto&gt;
-  &lt;nProt&gt;131214496702999&lt;/nProt&gt;
-  &lt;digVal&gt;mkKWkj2SymVXik3DMRRvKl3HtIE=&lt;/digVal&gt;
+  &lt;verAplic&gt;14.4.34-SE6&lt;/verAplic&gt;
+  &lt;chNFe&gt;31211092660604015457550760000146221569723315&lt;/chNFe&gt;
+  &lt;dhRecbto&gt;2021-10-22T21:27:50-03:00&lt;/dhRecbto&gt;
+  &lt;nProt&gt;131214398295525&lt;/nProt&gt;
+  &lt;digVal&gt;rm110vN04DtVARrQD2vv6pxqQfw=&lt;/digVal&gt;
   &lt;cStat&gt;100&lt;/cStat&gt;
   &lt;xMotivo&gt;Autorizado o uso da NF-e&lt;/xMotivo&gt;
 &lt;/infProt&gt;&lt;/protNFe&gt;&lt;/nfeProc&gt;</x:t>
   </x:si>
   <x:si>
-    <x:t>31211292660604017662550500000171131478426760.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\31211292660604017662550500000171131478426760.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;nfeProc versao="4.00" xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;NFe xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;infNFe Id="NFe31211292660604017662550500000171131478426760" versao="4.00"&gt;&lt;ide&gt;&lt;cUF&gt;31&lt;/cUF&gt;&lt;cNF&gt;47842676&lt;/cNF&gt;&lt;natOp&gt;Remessa p/ deposito fechado ou arm.geral&lt;/natOp&gt;&lt;mod&gt;55&lt;/mod&gt;&lt;serie&gt;50&lt;/serie&gt;&lt;nNF&gt;17113&lt;/nNF&gt;&lt;dhEmi&gt;2021-12-22T17:46:38-03:00&lt;/dhEmi&gt;&lt;tpNF&gt;1&lt;/tpNF&gt;&lt;idDest&gt;2&lt;/idDest&gt;&lt;cMunFG&gt;3166808&lt;/cMunFG&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;0&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;finNFe&gt;1&lt;/finNFe&gt;&lt;indFinal&gt;0&lt;/indFinal&gt;&lt;indPres&gt;9&lt;/indPres&gt;&lt;indIntermed&gt;0&lt;/indIntermed&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;SAP NFE 4.00&lt;/verProc&gt;&lt;/ide&gt;&lt;emit&gt;&lt;CNPJ&gt;92660604017662&lt;/CNPJ&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;xFant&gt;CMISS-Compl.Min.Indl.S Salitre&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;Fazenda Salitre&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;Marrua&lt;/xBairro&gt;&lt;cMun&gt;3166808&lt;/cMun&gt;&lt;xMun&gt;Serra do Salitre&lt;/xMun&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;CEP&gt;38760000&lt;/CEP&gt;&lt;xPais&gt;Brasil&lt;/xPais&gt;&lt;/enderEmit&gt;&lt;IE&gt;2874585321020&lt;/IE&gt;&lt;CRT&gt;3&lt;/CRT&gt;&lt;/emit&gt;&lt;dest&gt;&lt;CNPJ&gt;06225292000147&lt;/CNPJ&gt;&lt;xNome&gt;TERLOC TERMINAL LOGISTICO CESARI LT DA&lt;/xNome&gt;&lt;enderDest&gt;&lt;xLgr&gt;EST ENGENHEIRO PLINIO DE QUEIROZ&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xCpl&gt;SP 55&lt;/xCpl&gt;&lt;xBairro&gt;PIACAGUERA&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;CUBATAO&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;CEP&gt;11570000&lt;/CEP&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;Brasil&lt;/xPais&gt;&lt;/enderDest&gt;&lt;indIEDest&gt;1&lt;/indIEDest&gt;&lt;IE&gt;283108491118&lt;/IE&gt;&lt;email&gt;expedicao@terloc.com.br&lt;/email&gt;&lt;/dest&gt;&lt;det nItem="1"&gt;&lt;prod&gt;&lt;cProd&gt;1000011243&lt;/cProd&gt;&lt;cEAN&gt;SEM GTIN&lt;/cEAN&gt;&lt;xProd&gt;CONCENTRADO FOSFATICO GROSSO UMIDO CMISS&lt;/xProd&gt;&lt;NCM&gt;25102010&lt;/NCM&gt;&lt;EXTIPI&gt;10&lt;/EXTIPI&gt;&lt;CFOP&gt;6905&lt;/CFOP&gt;&lt;uCom&gt;TO&lt;/uCom&gt;&lt;qCom&gt;47.4200&lt;/qCom&gt;&lt;vUnCom&gt;1194.5200337410&lt;/vUnCom&gt;&lt;vProd&gt;56644.14&lt;/vProd&gt;&lt;cEANTrib&gt;SEM GTIN&lt;/cEANTrib&gt;&lt;uTrib&gt;TO&lt;/uTrib&gt;&lt;qTrib&gt;47.4200&lt;/qTrib&gt;&lt;vUnTrib&gt;1194.5200337410&lt;/vUnTrib&gt;&lt;indTot&gt;1&lt;/indTot&gt;&lt;/prod&gt;&lt;imposto&gt;&lt;ICMS&gt;&lt;ICMS20&gt;&lt;orig&gt;0&lt;/orig&gt;&lt;CST&gt;20&lt;/CST&gt;&lt;modBC&gt;3&lt;/modBC&gt;&lt;pRedBC&gt;99.6000&lt;/pRedBC&gt;&lt;vBC&gt;24415.58&lt;/vBC&gt;&lt;pICMS&gt;12.0000&lt;/pICMS&gt;&lt;vICMS&gt;2929.87&lt;/vICMS&gt;&lt;/ICMS20&gt;&lt;/ICMS&gt;&lt;IPI&gt;&lt;cEnq&gt;103&lt;/cEnq&gt;&lt;IPINT&gt;&lt;CST&gt;55&lt;/CST&gt;&lt;/IPINT&gt;&lt;/IPI&gt;&lt;PIS&gt;&lt;PISOutr&gt;&lt;CST&gt;49&lt;/CST&gt;&lt;qBCProd&gt;47.4200&lt;/qBCProd&gt;&lt;vAliqProd&gt;0.0000&lt;/vAliqProd&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;/PISOutr&gt;&lt;/PIS&gt;&lt;COFINS&gt;&lt;COFINSOutr&gt;&lt;CST&gt;49&lt;/CST&gt;&lt;qBCProd&gt;47.4200&lt;/qBCProd&gt;&lt;vAliqProd&gt;0.0000&lt;/vAliqProd&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;/COFINSOutr&gt;&lt;/COFINS&gt;&lt;/imposto&gt;&lt;infAdProd&gt;Base de calculo reduzida em 60 cfe RICMSMG2002, Art. 43 cc Anexo IV, Item 8, b. IPI suspenso nos termos do RIPI, Decreto 7.21210, Art. 43, III. Nao incidencia de COFINS cfe. Lei 10.83303, art. 1o Nao incidencia de PIS cfe. Lei 10.83303, art. 1o&lt;/infAdProd&gt;&lt;/det&gt;&lt;total&gt;&lt;ICMSTot&gt;&lt;vBC&gt;24415.58&lt;/vBC&gt;&lt;vICMS&gt;2929.87&lt;/vICMS&gt;&lt;vICMSDeson&gt;0.00&lt;/vICMSDeson&gt;&lt;vFCP&gt;0.00&lt;/vFCP&gt;&lt;vBCST&gt;0.00&lt;/vBCST&gt;&lt;vST&gt;0.00&lt;/vST&gt;&lt;vFCPST&gt;0.00&lt;/vFCPST&gt;&lt;vFCPSTRet&gt;0.00&lt;/vFCPSTRet&gt;&lt;vProd&gt;56644.14&lt;/vProd&gt;&lt;vFrete&gt;0.00&lt;/vFrete&gt;&lt;vSeg&gt;0.00&lt;/vSeg&gt;&lt;vDesc&gt;0.00&lt;/vDesc&gt;&lt;vII&gt;0.00&lt;/vII&gt;&lt;vIPI&gt;0.00&lt;/vIPI&gt;&lt;vIPIDevol&gt;0.00&lt;/vIPIDevol&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;vOutro&gt;0.00&lt;/vOutro&gt;&lt;vNF&gt;56644.14&lt;/vNF&gt;&lt;/ICMSTot&gt;&lt;/total&gt;&lt;transp&gt;&lt;modFrete&gt;0&lt;/modFrete&gt;&lt;transporta&gt;&lt;CNPJ&gt;50505924000703&lt;/CNPJ&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA FILIAL&lt;/xNome&gt;&lt;xEnder&gt;FILOMENA CARTAFINA 22031&lt;/xEnder&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;/transporta&gt;&lt;vol&gt;&lt;qVol&gt;47&lt;/qVol&gt;&lt;esp&gt;GRANEL&lt;/esp&gt;&lt;marca&gt;YARA&lt;/marca&gt;&lt;pesoL&gt;47420.000&lt;/pesoL&gt;&lt;pesoB&gt;47420.000&lt;/pesoB&gt;&lt;/vol&gt;&lt;/transp&gt;&lt;pag&gt;&lt;detPag&gt;&lt;indPag&gt;0&lt;/indPag&gt;&lt;tPag&gt;15&lt;/tPag&gt;&lt;vPag&gt;56644.14&lt;/vPag&gt;&lt;/detPag&gt;&lt;/pag&gt;&lt;infAdic&gt;&lt;infCpl&gt;Ordem de venda n 0000623925 Ordem de Carregamento 0003111061 Base de calculo reduzida em 60 cfe RICMSMG2002 Art 43 cc Anexo IV Item 8 b IPI suspenso nos termos do RIPI Decreto 721210 Art 43 III Nao incidencia de COFINS cfe Lei 1083303 art 1o Nao incidencia de PIS cfe Lei 1083303 art 1o REGISTRO MAPA NAO SE APLICA Data de fabricacao 22122021 Origem INDUSTRIA BRASILEIRA Classificacao Quimica Modo de aplicacao NA Armazenar sempre sobre piso seco com boa drenagem e em local coberto Para outras condicoes consultar a Yara Brasil Uso exclusivo como fertilizante Prezado Cliente Observacoes sobre carga recebida anotar no verso do canhoto da NF Em caso de emergencia ligue para 08007708899 Remessa 0082308671 A Ficha de Informacoes de Seguranca de Produtos Quimicos pode ser obtida por meio do site wwwyarabrasilcombr&lt;/infCpl&gt;&lt;/infAdic&gt;&lt;/infNFe&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#NFe31211292660604017662550500000171131478426760"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;RCABCaRgW7HjdLOPYd3SqG2BK5k=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;UcmqoKTtC4Vj2s9vyDsDGWu4NQNiPr5UsYQ0iGhY+JR7dqX5NJGnoUk0BSM4Ek1Dwv+zWiVKVTjM
-h4BCHo2uq86mofoeN8BoXIlj+mGnARuySgzU3tmM8bwCHcTTy43tPMPL+eGHV/SJRxF41mjI3lfl
-A5Yazq+Kcmk/WcCO/M0p+tQniVrfMF8qIwVQbHzOdjjkVUpffNIRddz2haq32c3pFUtBplC1jqCi
-4l448vyRz3ZxVJxZL17PTTsDru1Vp9kjypXcVnW27Y7ZuR77990lgo5Jy0LdXAhX8fJbHsDkwVGG
-nD8o5gNNf3Ojn397zSAfG3MZD79k2r7K/zDKWA==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIICzCCBfOgAwIBAgIQNjjNlSyNftb+ED1sesUuPTANBgkqhkiG9w0BAQsFADB4MQswCQYDVQQG
-EwJCUjETMBEGA1UEChMKSUNQLUJyYXNpbDE2MDQGA1UECxMtU2VjcmV0YXJpYSBkYSBSZWNlaXRh
-IEZlZGVyYWwgZG8gQnJhc2lsIC0gUkZCMRwwGgYDVQQDExNBQyBDZXJ0aXNpZ24gUkZCIEc1MB4X
-DTIxMTAwNjE1MDI0M1oXDTIyMTAwNjE1MDI0M1owggEBMQswCQYDVQQGEwJCUjETMBEGA1UECgwK
-SUNQLUJyYXNpbDELMAkGA1UECAwCUlMxFTATBgNVBAcMDFBvcnRvIEFsZWdyZTEZMBcGA1UECwwQ
-VmlkZW9Db25mZXJlbmNpYTEXMBUGA1UECwwOMTA4NjkwODAwMDAxNzAxNjA0BgNVBAsMLVNlY3Jl
-dGFyaWEgZGEgUmVjZWl0YSBGZWRlcmFsIGRvIEJyYXNpbCAtIFJGQjEWMBQGA1UECwwNUkZCIGUt
-Q05QSiBBMTE1MDMGA1UEAwwsWUFSQSBCUkFTSUwgRkVSVElMSVpBTlRFUyBTIEE6OTI2NjA2MDQw
-MDAxODIwggEiMA0GCSqGSIb3DQEBAQUAA4IBDwAwggEKAoIBAQCbDkPNSgzXLGqoqumwXPWkcZCj
-2iP6kjQtBerE4vrBR19Mc4BLYvGZvnniaDYwJxXy3bHVdz/RwGPoblcjEzyYoex7wCZb/1ZVow/w
-jVOIDt7ekV8sbxZMY0J26o2SXfDhcxMjK6i8v/4Ku9oVIJBPWs4QRT4y0t4Kynub1+Vnb2bVi4bI
-I7gHHE/XXwTv6y1pQOHmHTz2mkO/AX1JqCoIoj7XlRoEEnLyXqblE4cb5Gxi1uCSOcc4O00UOG8Y
-c83o3uu4LWnbdu7S056YFP6PWlaNqMkFhjIKGssfZZnEhUWfg/JWnkdyV0pS0LLtSLJa1r+BR/98
-XIWzjfmBc2RbAgMBAAGjggMEMIIDADCBswYDVR0RBIGrMIGooD0GBWBMAQMEoDQEMjI5MDUxOTY5
-NDk1ODkwOTEwOTEwMDAwMDAwMDAwMDAwMDAwNDAzOTU3NDg1MlNTUFJToCIGBWBMAQMCoBkEF0NM
-RUlUT04gTUVTUVVJVEEgVkFSR0FToBkGBWBMAQMDoBAEDjkyNjYwNjA0MDAwMTgyoBcGBWBMAQMH
-oA4EDDAwMDAwMDAwMDAwMIEPZmlzY2FsQHlhcmEuY29tMAkGA1UdEwQCMAAwHwYDVR0jBBgwFoAU
-U31/nb7RYdAgutqf44mnE3NYzUIwfwYDVR0gBHgwdjB0BgZgTAECAQwwajBoBggrBgEFBQcCARZc
-aHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9kcGMvQUNfQ2Vy
-dGlzaWduX1JGQi9EUENfQUNfQ2VydGlzaWduX1JGQi5wZGYwgbwGA1UdHwSBtDCBsTBXoFWgU4ZR
-aHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9sY3IvQUNDZXJ0
-aXNpZ25SRkJHNS9MYXRlc3RDUkwuY3JsMFagVKBShlBodHRwOi8vaWNwLWJyYXNpbC5vdXRyYWxj
-ci5jb20uYnIvcmVwb3NpdG9yaW8vbGNyL0FDQ2VydGlzaWduUkZCRzUvTGF0ZXN0Q1JMLmNybDAO
-BgNVHQ8BAf8EBAMCBeAwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGsBggrBgEFBQcB
-AQSBnzCBnDBfBggrBgEFBQcwAoZTaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9y
-ZXBvc2l0b3Jpby9jZXJ0aWZpY2Fkb3MvQUNfQ2VydGlzaWduX1JGQl9HNS5wN2MwOQYIKwYBBQUH
-MAGGLWh0dHA6Ly9vY3NwLWFjLWNlcnRpc2lnbi1yZmIuY2VydGlzaWduLmNvbS5icjANBgkqhkiG
-9w0BAQsFAAOCAgEASCNnP1ersGgcFlHfGmfzgtSBVH0oJrVrm7/LFr2FjM8AjX9PY97brv6UubUj
-swAD+yL+dwwsuv1TxnBHw8AE8MGbxiZQTnNf0OMkIPAEDvwlb8SXK7Gk137JKUaKKGup5P4dbA8X
-M22+GEw1dMYjCV6eqJ2bxP1EjRII3rb8EsQATZ/pDizsEauNXOmXqbIefqU9wWaQhTQVtLwflrN0
-zElGDSX9uwtR6j28usr3KiKf26MfhtWDAombY+m9Bhq2Hys6hZpyfL+ERFoWXmpzlhmEvUFnMzL1
-SWGNeyhn+na7r7cJvBFcdPPyriZlAdApkaZGXSQAGW78gvlJLD2YtYk/BN02v7qCfhcPHdZcQ4XV
-kdj8idIMcn3ZiweWanaZ9riR3yLStxBP7arsQrMGOrYkAyo9otufpJfYS+FHkrJapqfZxbo0qCTs
-ZPHvAcMw8vCojT/Z2FZrGi6aDK2rt7hPhKYRedZNbDmVgKSRNBoyPqSoqNwMSEiF7EmXA5zq27SM
-87v096EsX8COhgxvMqj/ENxfj8x94POwH8gif/xv9r/raWYCrOnKNP8uhXJPdeihFZBsbWanSUZW
-YlltN/lCaF/oSDqsQjVaG4MndtddEIwdfk3xg71iptYN1tYWHSMal0EwKkOA3A9obwTtxz1fkp8F
-nGxIgi6QuCLfPTU=&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/NFe&gt;&lt;protNFe versao="4.00"&gt;&lt;infProt Id="ID131214498686002"&gt;
+    <x:t>31211092660604015457550760000146311031134436.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\31211092660604015457550760000146311031134436.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;nfeProc versao="4.00" xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;NFe xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;infNFe Id="NFe31211092660604015457550760000146311031134436" versao="4.00"&gt;&lt;ide&gt;&lt;cUF&gt;31&lt;/cUF&gt;&lt;cNF&gt;03113443&lt;/cNF&gt;&lt;natOp&gt;TRANSFERNCIA&lt;/natOp&gt;&lt;mod&gt;55&lt;/mod&gt;&lt;serie&gt;76&lt;/serie&gt;&lt;nNF&gt;14631&lt;/nNF&gt;&lt;dhEmi&gt;2021-10-22T23:59:22-03:00&lt;/dhEmi&gt;&lt;dhSaiEnt&gt;2021-10-22T23:59:22-03:00&lt;/dhSaiEnt&gt;&lt;tpNF&gt;1&lt;/tpNF&gt;&lt;idDest&gt;2&lt;/idDest&gt;&lt;cMunFG&gt;3170107&lt;/cMunFG&gt;&lt;tpImp&gt;2&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;6&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;finNFe&gt;1&lt;/finNFe&gt;&lt;indFinal&gt;0&lt;/indFinal&gt;&lt;indPres&gt;9&lt;/indPres&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;200&lt;/verProc&gt;&lt;/ide&gt;&lt;emit&gt;&lt;CNPJ&gt;92660604015457&lt;/CNPJ&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES SA&lt;/xNome&gt;&lt;xFant&gt;YARA BRASIL FERTILIZANTES SA&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA ANTONIO CARLOS GUILLAUMON 800&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;CEP&gt;38044760&lt;/CEP&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;fone&gt;3433197198&lt;/fone&gt;&lt;/enderEmit&gt;&lt;IE&gt;3714585320678&lt;/IE&gt;&lt;CRT&gt;3&lt;/CRT&gt;&lt;/emit&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604013756&lt;/CNPJ&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES SA&lt;/xNome&gt;&lt;enderDest&gt;&lt;xLgr&gt;AVENIDA SAO JUDAS TADEU&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;JARDIM SAO JUDAS TAD&lt;/xBairro&gt;&lt;cMun&gt;3552403&lt;/cMun&gt;&lt;xMun&gt;SUMARE&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;CEP&gt;13180570&lt;/CEP&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;fone&gt;0000000000&lt;/fone&gt;&lt;/enderDest&gt;&lt;indIEDest&gt;1&lt;/indIEDest&gt;&lt;IE&gt;671143732119&lt;/IE&gt;&lt;/dest&gt;&lt;retirada&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;xLgr&gt;AV. CONS. RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;/retirada&gt;&lt;autXML&gt;&lt;CNPJ&gt;55681274000185&lt;/CNPJ&gt;&lt;/autXML&gt;&lt;autXML&gt;&lt;CNPJ&gt;92660604000182&lt;/CNPJ&gt;&lt;/autXML&gt;&lt;det nItem="1"&gt;&lt;prod&gt;&lt;cProd&gt;1000006142&lt;/cProd&gt;&lt;cEAN&gt;SEM GTIN&lt;/cEAN&gt;&lt;xProd&gt;00 00 60 KCL&lt;/xProd&gt;&lt;NCM&gt;31042090&lt;/NCM&gt;&lt;EXTIPI&gt;000&lt;/EXTIPI&gt;&lt;CFOP&gt;6152&lt;/CFOP&gt;&lt;uCom&gt;TO&lt;/uCom&gt;&lt;qCom&gt;47.9300&lt;/qCom&gt;&lt;vUnCom&gt;2135.3&lt;/vUnCom&gt;&lt;vProd&gt;102344.93&lt;/vProd&gt;&lt;cEANTrib&gt;SEM GTIN&lt;/cEANTrib&gt;&lt;uTrib&gt;TO&lt;/uTrib&gt;&lt;qTrib&gt;47.9300&lt;/qTrib&gt;&lt;vUnTrib&gt;2135.3&lt;/vUnTrib&gt;&lt;indTot&gt;1&lt;/indTot&gt;&lt;xPed&gt;4500713253&lt;/xPed&gt;&lt;/prod&gt;&lt;imposto&gt;&lt;ICMS&gt;&lt;ICMS20&gt;&lt;orig&gt;6&lt;/orig&gt;&lt;CST&gt;20&lt;/CST&gt;&lt;modBC&gt;3&lt;/modBC&gt;&lt;pRedBC&gt;30.00&lt;/pRedBC&gt;&lt;vBC&gt;74316.86&lt;/vBC&gt;&lt;pICMS&gt;12.00&lt;/pICMS&gt;&lt;vICMS&gt;8918.02&lt;/vICMS&gt;&lt;vICMSDeson&gt;3822.01&lt;/vICMSDeson&gt;&lt;motDesICMS&gt;3&lt;/motDesICMS&gt;&lt;/ICMS20&gt;&lt;/ICMS&gt;&lt;IPI&gt;&lt;cEnq&gt;112&lt;/cEnq&gt;&lt;IPINT&gt;&lt;CST&gt;53&lt;/CST&gt;&lt;/IPINT&gt;&lt;/IPI&gt;&lt;PIS&gt;&lt;PISOutr&gt;&lt;CST&gt;49&lt;/CST&gt;&lt;vBC&gt;0.00&lt;/vBC&gt;&lt;pPIS&gt;0.00&lt;/pPIS&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;/PISOutr&gt;&lt;/PIS&gt;&lt;COFINS&gt;&lt;COFINSOutr&gt;&lt;CST&gt;49&lt;/CST&gt;&lt;vBC&gt;0.00&lt;/vBC&gt;&lt;pCOFINS&gt;0.00&lt;/pCOFINS&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;/COFINSOutr&gt;&lt;/COFINS&gt;&lt;/imposto&gt;&lt;infAdProd&gt;CLORETO DE POTASSIO 60% GRANULADO&lt;/infAdProd&gt;&lt;/det&gt;&lt;total&gt;&lt;ICMSTot&gt;&lt;vBC&gt;74316.86&lt;/vBC&gt;&lt;vICMS&gt;8918.02&lt;/vICMS&gt;&lt;vICMSDeson&gt;3822.01&lt;/vICMSDeson&gt;&lt;vFCPUFDest&gt;0.00&lt;/vFCPUFDest&gt;&lt;vICMSUFDest&gt;0.00&lt;/vICMSUFDest&gt;&lt;vICMSUFRemet&gt;0.00&lt;/vICMSUFRemet&gt;&lt;vFCP&gt;0.00&lt;/vFCP&gt;&lt;vBCST&gt;0.00&lt;/vBCST&gt;&lt;vST&gt;0.00&lt;/vST&gt;&lt;vFCPST&gt;0.00&lt;/vFCPST&gt;&lt;vFCPSTRet&gt;0.00&lt;/vFCPSTRet&gt;&lt;vProd&gt;102344.93&lt;/vProd&gt;&lt;vFrete&gt;0.00&lt;/vFrete&gt;&lt;vSeg&gt;0.00&lt;/vSeg&gt;&lt;vDesc&gt;0.00&lt;/vDesc&gt;&lt;vII&gt;0.00&lt;/vII&gt;&lt;vIPI&gt;0.00&lt;/vIPI&gt;&lt;vIPIDevol&gt;0.00&lt;/vIPIDevol&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;vOutro&gt;0.00&lt;/vOutro&gt;&lt;vNF&gt;102344.93&lt;/vNF&gt;&lt;/ICMSTot&gt;&lt;/total&gt;&lt;transp&gt;&lt;modFrete&gt;1&lt;/modFrete&gt;&lt;transporta&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xEnder&gt;AV JOS AUGUSTO CARVALHO 4063&lt;/xEnder&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;/transporta&gt;&lt;vol&gt;&lt;qVol&gt;48&lt;/qVol&gt;&lt;esp&gt;GRANEL&lt;/esp&gt;&lt;marca&gt;00 00 60 KCL&lt;/marca&gt;&lt;nVol&gt;0&lt;/nVol&gt;&lt;pesoL&gt;47930.000&lt;/pesoL&gt;&lt;pesoB&gt;47930.000&lt;/pesoB&gt;&lt;/vol&gt;&lt;/transp&gt;&lt;pag&gt;&lt;detPag&gt;&lt;tPag&gt;01&lt;/tPag&gt;&lt;vPag&gt;102344.93&lt;/vPag&gt;&lt;/detPag&gt;&lt;/pag&gt;&lt;infAdic&gt;&lt;infCpl&gt;BRUTO 48.930 TARA 1.000 LIQUIDO 47.930  CARRETA 2 EGJ 4985  CV FWX 8247REDUO BASE CLCULO ICMS P 70% NOS TERMOS DO ARTIGO 43, PARTE GERAL, COMBINADO ANEXO IV RICMSMGICMS DISPENSADO E REDUZIDO DO PRECO VL. INTEGRAL X REDUCAO BASE % X ALIQ %  VL DISPENSADO106166.94 X 30.0% X 12.0%  3822.01IPI NAO TRIBUTADO CONFORME CAPITULO 31 DA TIPIRMA PR 000664-5.000073PRODUTO IMPORTADO, ARMAZENAR EM LUGAR SECO, COBERTO E AREJADOMERCADORIA SAIDA DO PORTO DE SANTOS - SANTOSSPPEDIDO 4500713253DATA DE FABRICACAO 22102021 DATA DE VALIDADE 22102023DI 211807687-7, DATA DA DI 21092021, NAVIO SANTA JOHANNA, NR. IMP 0001806I21NR NF MAE 14204, DATA NF MAE 11102021, PEDIDO 4500713253, TIQUETE 0124352021&lt;/infCpl&gt;&lt;obsCont xCampo="NR_NF_MAE"&gt;&lt;xTexto&gt;14204&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NR_PEDIDO"&gt;&lt;xTexto&gt;4500713253&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NR_IMPORTACAO"&gt;&lt;xTexto&gt;0001806I21&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NR_TIQUETE"&gt;&lt;xTexto&gt;0124352021&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NAVIO"&gt;&lt;xTexto&gt;SANTA JOHANNA&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="ITEM_PEDIDO_CLIENTE"&gt;&lt;xTexto&gt;10&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="CD_TIPO_NF"&gt;&lt;xTexto&gt;S&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="CD_OPERACAO"&gt;&lt;xTexto&gt;06&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="CD_EMPRESA"&gt;&lt;xTexto&gt;1196&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;/infAdic&gt;&lt;compra&gt;&lt;xPed&gt;4500713253&lt;/xPed&gt;&lt;/compra&gt;&lt;infRespTec&gt;&lt;CNPJ&gt;11342233000199&lt;/CNPJ&gt;&lt;xContato&gt;Helpdesk&lt;/xContato&gt;&lt;email&gt;helpdesk@micsistemas.com.br&lt;/email&gt;&lt;fone&gt;1340422786&lt;/fone&gt;&lt;/infRespTec&gt;&lt;/infNFe&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#NFe31211092660604015457550760000146311031134436"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;GMJrrVKO6dbZ/Vzea/UomExcTOc=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;RopcBtmukm2MRTjuORo2uNcpWuvTvBw7Q0f/WZfcyCaIn3hdgQKynn9Ca4jumfy69it4h6emsXRPHienOUH03/GE/hae4q4gYZgBSG6vQlnsSLgjMiOgH+xOueaetPmSZUdd5D/ljuWiaLNjgSbmZPW2oV3Zjq9JvoNjfL1A1MibHDdvUeRhDoVa9cgaaJj4uiqGZdzW6BMLXRqoKWN3wCL6S+TiG0v0X1fW5BPHO1kFD8FPa8GgbA6xHUvtLWgfVNObxe1TM/0LuplgNFY3ZAhs8f/RR35zKOqYjMrgPihGyRljPcZT/oJ+yybF8ablZ1w/BkKn1p4WWJW7jspsCA==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIICzCCBfOgAwIBAgIQNjjNlSyNftb+ED1sesUuPTANBgkqhkiG9w0BAQsFADB4MQswCQYDVQQGEwJCUjETMBEGA1UEChMKSUNQLUJyYXNpbDE2MDQGA1UECxMtU2VjcmV0YXJpYSBkYSBSZWNlaXRhIEZlZGVyYWwgZG8gQnJhc2lsIC0gUkZCMRwwGgYDVQQDExNBQyBDZXJ0aXNpZ24gUkZCIEc1MB4XDTIxMTAwNjE1MDI0M1oXDTIyMTAwNjE1MDI0M1owggEBMQswCQYDVQQGEwJCUjETMBEGA1UECgwKSUNQLUJyYXNpbDELMAkGA1UECAwCUlMxFTATBgNVBAcMDFBvcnRvIEFsZWdyZTEZMBcGA1UECwwQVmlkZW9Db25mZXJlbmNpYTEXMBUGA1UECwwOMTA4NjkwODAwMDAxNzAxNjA0BgNVBAsMLVNlY3JldGFyaWEgZGEgUmVjZWl0YSBGZWRlcmFsIGRvIEJyYXNpbCAtIFJGQjEWMBQGA1UECwwNUkZCIGUtQ05QSiBBMTE1MDMGA1UEAwwsWUFSQSBCUkFTSUwgRkVSVElMSVpBTlRFUyBTIEE6OTI2NjA2MDQwMDAxODIwggEiMA0GCSqGSIb3DQEBAQUAA4IBDwAwggEKAoIBAQCbDkPNSgzXLGqoqumwXPWkcZCj2iP6kjQtBerE4vrBR19Mc4BLYvGZvnniaDYwJxXy3bHVdz/RwGPoblcjEzyYoex7wCZb/1ZVow/wjVOIDt7ekV8sbxZMY0J26o2SXfDhcxMjK6i8v/4Ku9oVIJBPWs4QRT4y0t4Kynub1+Vnb2bVi4bII7gHHE/XXwTv6y1pQOHmHTz2mkO/AX1JqCoIoj7XlRoEEnLyXqblE4cb5Gxi1uCSOcc4O00UOG8Yc83o3uu4LWnbdu7S056YFP6PWlaNqMkFhjIKGssfZZnEhUWfg/JWnkdyV0pS0LLtSLJa1r+BR/98XIWzjfmBc2RbAgMBAAGjggMEMIIDADCBswYDVR0RBIGrMIGooD0GBWBMAQMEoDQEMjI5MDUxOTY5NDk1ODkwOTEwOTEwMDAwMDAwMDAwMDAwMDAwNDAzOTU3NDg1MlNTUFJToCIGBWBMAQMCoBkEF0NMRUlUT04gTUVTUVVJVEEgVkFSR0FToBkGBWBMAQMDoBAEDjkyNjYwNjA0MDAwMTgyoBcGBWBMAQMHoA4EDDAwMDAwMDAwMDAwMIEPZmlzY2FsQHlhcmEuY29tMAkGA1UdEwQCMAAwHwYDVR0jBBgwFoAUU31/nb7RYdAgutqf44mnE3NYzUIwfwYDVR0gBHgwdjB0BgZgTAECAQwwajBoBggrBgEFBQcCARZcaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9kcGMvQUNfQ2VydGlzaWduX1JGQi9EUENfQUNfQ2VydGlzaWduX1JGQi5wZGYwgbwGA1UdHwSBtDCBsTBXoFWgU4ZRaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9sY3IvQUNDZXJ0aXNpZ25SRkJHNS9MYXRlc3RDUkwuY3JsMFagVKBShlBodHRwOi8vaWNwLWJyYXNpbC5vdXRyYWxjci5jb20uYnIvcmVwb3NpdG9yaW8vbGNyL0FDQ2VydGlzaWduUkZCRzUvTGF0ZXN0Q1JMLmNybDAOBgNVHQ8BAf8EBAMCBeAwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGsBggrBgEFBQcBAQSBnzCBnDBfBggrBgEFBQcwAoZTaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9jZXJ0aWZpY2Fkb3MvQUNfQ2VydGlzaWduX1JGQl9HNS5wN2MwOQYIKwYBBQUHMAGGLWh0dHA6Ly9vY3NwLWFjLWNlcnRpc2lnbi1yZmIuY2VydGlzaWduLmNvbS5icjANBgkqhkiG9w0BAQsFAAOCAgEASCNnP1ersGgcFlHfGmfzgtSBVH0oJrVrm7/LFr2FjM8AjX9PY97brv6UubUjswAD+yL+dwwsuv1TxnBHw8AE8MGbxiZQTnNf0OMkIPAEDvwlb8SXK7Gk137JKUaKKGup5P4dbA8XM22+GEw1dMYjCV6eqJ2bxP1EjRII3rb8EsQATZ/pDizsEauNXOmXqbIefqU9wWaQhTQVtLwflrN0zElGDSX9uwtR6j28usr3KiKf26MfhtWDAombY+m9Bhq2Hys6hZpyfL+ERFoWXmpzlhmEvUFnMzL1SWGNeyhn+na7r7cJvBFcdPPyriZlAdApkaZGXSQAGW78gvlJLD2YtYk/BN02v7qCfhcPHdZcQ4XVkdj8idIMcn3ZiweWanaZ9riR3yLStxBP7arsQrMGOrYkAyo9otufpJfYS+FHkrJapqfZxbo0qCTsZPHvAcMw8vCojT/Z2FZrGi6aDK2rt7hPhKYRedZNbDmVgKSRNBoyPqSoqNwMSEiF7EmXA5zq27SM87v096EsX8COhgxvMqj/ENxfj8x94POwH8gif/xv9r/raWYCrOnKNP8uhXJPdeihFZBsbWanSUZWYlltN/lCaF/oSDqsQjVaG4MndtddEIwdfk3xg71iptYN1tYWHSMal0EwKkOA3A9obwTtxz1fkp8FnGxIgi6QuCLfPTU=&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/NFe&gt;&lt;protNFe versao="4.00"&gt;&lt;infProt Id="ID131214398469542"&gt;
   &lt;tpAmb&gt;1&lt;/tpAmb&gt;
-  &lt;verAplic&gt;14.4.46-MA1&lt;/verAplic&gt;
-  &lt;chNFe&gt;31211292660604017662550500000171131478426760&lt;/chNFe&gt;
-  &lt;dhRecbto&gt;2021-12-22T17:46:57-03:00&lt;/dhRecbto&gt;
-  &lt;nProt&gt;131214498686002&lt;/nProt&gt;
-  &lt;digVal&gt;RCABCaRgW7HjdLOPYd3SqG2BK5k=&lt;/digVal&gt;
+  &lt;verAplic&gt;14.4.34-ZB1&lt;/verAplic&gt;
+  &lt;chNFe&gt;31211092660604015457550760000146311031134436&lt;/chNFe&gt;
+  &lt;dhRecbto&gt;2021-10-22T23:59:31-03:00&lt;/dhRecbto&gt;
+  &lt;nProt&gt;131214398469542&lt;/nProt&gt;
+  &lt;digVal&gt;GMJrrVKO6dbZ/Vzea/UomExcTOc=&lt;/digVal&gt;
   &lt;cStat&gt;100&lt;/cStat&gt;
   &lt;xMotivo&gt;Autorizado o uso da NF-e&lt;/xMotivo&gt;
 &lt;/infProt&gt;&lt;/protNFe&gt;&lt;/nfeProc&gt;</x:t>
   </x:si>
   <x:si>
-    <x:t>31211292660604017662550500000171731944724056.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\31211292660604017662550500000171731944724056.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;nfeProc versao="4.00" xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;NFe xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;infNFe Id="NFe31211292660604017662550500000171731944724056" versao="4.00"&gt;&lt;ide&gt;&lt;cUF&gt;31&lt;/cUF&gt;&lt;cNF&gt;94472405&lt;/cNF&gt;&lt;natOp&gt;Transferencia producao estabelecimento&lt;/natOp&gt;&lt;mod&gt;55&lt;/mod&gt;&lt;serie&gt;50&lt;/serie&gt;&lt;nNF&gt;17173&lt;/nNF&gt;&lt;dhEmi&gt;2021-12-27T19:38:49-03:00&lt;/dhEmi&gt;&lt;tpNF&gt;1&lt;/tpNF&gt;&lt;idDest&gt;2&lt;/idDest&gt;&lt;cMunFG&gt;3166808&lt;/cMunFG&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;6&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;finNFe&gt;1&lt;/finNFe&gt;&lt;indFinal&gt;0&lt;/indFinal&gt;&lt;indPres&gt;9&lt;/indPres&gt;&lt;indIntermed&gt;0&lt;/indIntermed&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;SAP NFE 4.00&lt;/verProc&gt;&lt;/ide&gt;&lt;emit&gt;&lt;CNPJ&gt;92660604017662&lt;/CNPJ&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;xFant&gt;CMISS-Compl.Min.Indl.S Salitre&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;Fazenda Salitre&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;Marrua&lt;/xBairro&gt;&lt;cMun&gt;3166808&lt;/cMun&gt;&lt;xMun&gt;Serra do Salitre&lt;/xMun&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;CEP&gt;38760000&lt;/CEP&gt;&lt;xPais&gt;Brasil&lt;/xPais&gt;&lt;/enderEmit&gt;&lt;IE&gt;2874585321020&lt;/IE&gt;&lt;CRT&gt;3&lt;/CRT&gt;&lt;/emit&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604017158&lt;/CNPJ&gt;&lt;xNome&gt;Yara Brasil Fertilizantes S/A. Unidade Cubatao 2&lt;/xNome&gt;&lt;enderDest&gt;&lt;xLgr&gt;Avenida Eng. Plinio de Queiroz&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;Zona Industrial&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;Cubatao&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;CEP&gt;11570901&lt;/CEP&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;Brasil&lt;/xPais&gt;&lt;fone&gt;1333699000&lt;/fone&gt;&lt;/enderDest&gt;&lt;indIEDest&gt;1&lt;/indIEDest&gt;&lt;IE&gt;283129851112&lt;/IE&gt;&lt;email&gt;luciano.pinto@yara.com&lt;/email&gt;&lt;/dest&gt;&lt;det nItem="1"&gt;&lt;prod&gt;&lt;cProd&gt;1000011243&lt;/cProd&gt;&lt;cEAN&gt;SEM GTIN&lt;/cEAN&gt;&lt;xProd&gt;CONCENTRADO FOSFATICO GROSSO UMIDO CMISS&lt;/xProd&gt;&lt;NCM&gt;25102010&lt;/NCM&gt;&lt;EXTIPI&gt;10&lt;/EXTIPI&gt;&lt;CFOP&gt;6151&lt;/CFOP&gt;&lt;uCom&gt;TO&lt;/uCom&gt;&lt;qCom&gt;48.0400&lt;/qCom&gt;&lt;vUnCom&gt;1254.5849292256&lt;/vUnCom&gt;&lt;vProd&gt;60270.26&lt;/vProd&gt;&lt;cEANTrib&gt;SEM GTIN&lt;/cEANTrib&gt;&lt;uTrib&gt;TO&lt;/uTrib&gt;&lt;qTrib&gt;48.0400&lt;/qTrib&gt;&lt;vUnTrib&gt;1254.5849292256&lt;/vUnTrib&gt;&lt;indTot&gt;1&lt;/indTot&gt;&lt;/prod&gt;&lt;imposto&gt;&lt;ICMS&gt;&lt;ICMS20&gt;&lt;orig&gt;0&lt;/orig&gt;&lt;CST&gt;20&lt;/CST&gt;&lt;modBC&gt;3&lt;/modBC&gt;&lt;pRedBC&gt;100.0000&lt;/pRedBC&gt;&lt;vBC&gt;24045.99&lt;/vBC&gt;&lt;pICMS&gt;12.0000&lt;/pICMS&gt;&lt;vICMS&gt;2885.52&lt;/vICMS&gt;&lt;/ICMS20&gt;&lt;/ICMS&gt;&lt;IPI&gt;&lt;cEnq&gt;999&lt;/cEnq&gt;&lt;IPINT&gt;&lt;CST&gt;53&lt;/CST&gt;&lt;/IPINT&gt;&lt;/IPI&gt;&lt;PIS&gt;&lt;PISNT&gt;&lt;CST&gt;06&lt;/CST&gt;&lt;/PISNT&gt;&lt;/PIS&gt;&lt;COFINS&gt;&lt;COFINSNT&gt;&lt;CST&gt;06&lt;/CST&gt;&lt;/COFINSNT&gt;&lt;/COFINS&gt;&lt;/imposto&gt;&lt;infAdProd&gt;Lote: 0001436599 Validade ate: 21.05.2022&lt;/infAdProd&gt;&lt;/det&gt;&lt;total&gt;&lt;ICMSTot&gt;&lt;vBC&gt;24045.99&lt;/vBC&gt;&lt;vICMS&gt;2885.52&lt;/vICMS&gt;&lt;vICMSDeson&gt;0.00&lt;/vICMSDeson&gt;&lt;vFCP&gt;0.00&lt;/vFCP&gt;&lt;vBCST&gt;0.00&lt;/vBCST&gt;&lt;vST&gt;0.00&lt;/vST&gt;&lt;vFCPST&gt;0.00&lt;/vFCPST&gt;&lt;vFCPSTRet&gt;0.00&lt;/vFCPSTRet&gt;&lt;vProd&gt;60270.26&lt;/vProd&gt;&lt;vFrete&gt;0.00&lt;/vFrete&gt;&lt;vSeg&gt;0.00&lt;/vSeg&gt;&lt;vDesc&gt;0.00&lt;/vDesc&gt;&lt;vII&gt;0.00&lt;/vII&gt;&lt;vIPI&gt;0.00&lt;/vIPI&gt;&lt;vIPIDevol&gt;0.00&lt;/vIPIDevol&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;vOutro&gt;0.00&lt;/vOutro&gt;&lt;vNF&gt;60270.26&lt;/vNF&gt;&lt;/ICMSTot&gt;&lt;/total&gt;&lt;transp&gt;&lt;modFrete&gt;0&lt;/modFrete&gt;&lt;transporta&gt;&lt;CNPJ&gt;50505924000703&lt;/CNPJ&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA FILIAL&lt;/xNome&gt;&lt;xEnder&gt;FILOMENA CARTAFINA 22031&lt;/xEnder&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;/transporta&gt;&lt;vol&gt;&lt;qVol&gt;48&lt;/qVol&gt;&lt;esp&gt;GRANEL&lt;/esp&gt;&lt;marca&gt;YARA&lt;/marca&gt;&lt;pesoL&gt;48040.000&lt;/pesoL&gt;&lt;pesoB&gt;48040.000&lt;/pesoB&gt;&lt;/vol&gt;&lt;/transp&gt;&lt;pag&gt;&lt;detPag&gt;&lt;tPag&gt;90&lt;/tPag&gt;&lt;vPag&gt;0.00&lt;/vPag&gt;&lt;/detPag&gt;&lt;/pag&gt;&lt;infAdic&gt;&lt;infCpl&gt;Pedido de Transferencia 4500718868 Ordem de Carregamento 0003115717 Base de calculo reduzida em 60 cfe RICMSMG2002 Art 43 cc Anexo IV Item 74 quotaquot IPI nao tributado conforme classificacao fiscal da TIPI Decreto 895016 cc RIPI Decreto 721210 Art 2o COFINS tributado c aliquota zero cfe Lei 1092504 art 1o PIS tributado c aliquota zero cfe Lei 1092504 art 1o REGISTRO MAPA NAO SE APLICA Produto 1000011243 Origem INDUSTRIA BRASILEIRA Classificacao Quimica Modo de aplicacao NA Armazenar sempre sobre piso seco com boa drenagem e em local coberto Para outras condicoes consultar a Yara Brasil Uso exclusivo como fertilizante Prezado Cliente Observacoes sobre carga recebida anotar no verso do canhoto da NF Em caso de emergencia ligue para 08007708899 Remessa 0082312626 A Ficha de Informacoes de Seguranca de Produtos Quimicos pode ser obtida por meio do site wwwyarabrasilcombr&lt;/infCpl&gt;&lt;/infAdic&gt;&lt;/infNFe&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#NFe31211292660604017662550500000171731944724056"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;Djka290DHdCz6hT6qZ9suLPJBhY=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;OsL3kiWNHgLl1OUsUQ6EsB/D0NbOMQq2QKykHJ/eMNhiaiFfZqedfyrQBsKpyjAaL0BYEZnMzWHr
-Znw4hNmJO3AKpMMQHkotOOKoTbtqtnTrDl57l79OTSUkWMSNa1NKeQqMroNOQVN3KkL09vsa0weO
-CuCQhVjkHmmIjDm9FJ6NGokifOJs0JCbRnfCVq6spxOF9wHk52jb7oKTiZN8QGTIoUfSv+4nA79Q
-GHpKEi+UzMsd+MvmOMbXPDNjqfGFrvjw6yHj9+Lm6RoBMDPZ0DzeCW7FU208W8EkrEwguIX8VmRl
-xMbM7xaxbtJNCQGXyg+exgSyj8A432r8+4sc6A==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIICzCCBfOgAwIBAgIQNjjNlSyNftb+ED1sesUuPTANBgkqhkiG9w0BAQsFADB4MQswCQYDVQQG
-EwJCUjETMBEGA1UEChMKSUNQLUJyYXNpbDE2MDQGA1UECxMtU2VjcmV0YXJpYSBkYSBSZWNlaXRh
-IEZlZGVyYWwgZG8gQnJhc2lsIC0gUkZCMRwwGgYDVQQDExNBQyBDZXJ0aXNpZ24gUkZCIEc1MB4X
-DTIxMTAwNjE1MDI0M1oXDTIyMTAwNjE1MDI0M1owggEBMQswCQYDVQQGEwJCUjETMBEGA1UECgwK
-SUNQLUJyYXNpbDELMAkGA1UECAwCUlMxFTATBgNVBAcMDFBvcnRvIEFsZWdyZTEZMBcGA1UECwwQ
-VmlkZW9Db25mZXJlbmNpYTEXMBUGA1UECwwOMTA4NjkwODAwMDAxNzAxNjA0BgNVBAsMLVNlY3Jl
-dGFyaWEgZGEgUmVjZWl0YSBGZWRlcmFsIGRvIEJyYXNpbCAtIFJGQjEWMBQGA1UECwwNUkZCIGUt
-Q05QSiBBMTE1MDMGA1UEAwwsWUFSQSBCUkFTSUwgRkVSVElMSVpBTlRFUyBTIEE6OTI2NjA2MDQw
-MDAxODIwggEiMA0GCSqGSIb3DQEBAQUAA4IBDwAwggEKAoIBAQCbDkPNSgzXLGqoqumwXPWkcZCj
-2iP6kjQtBerE4vrBR19Mc4BLYvGZvnniaDYwJxXy3bHVdz/RwGPoblcjEzyYoex7wCZb/1ZVow/w
-jVOIDt7ekV8sbxZMY0J26o2SXfDhcxMjK6i8v/4Ku9oVIJBPWs4QRT4y0t4Kynub1+Vnb2bVi4bI
-I7gHHE/XXwTv6y1pQOHmHTz2mkO/AX1JqCoIoj7XlRoEEnLyXqblE4cb5Gxi1uCSOcc4O00UOG8Y
-c83o3uu4LWnbdu7S056YFP6PWlaNqMkFhjIKGssfZZnEhUWfg/JWnkdyV0pS0LLtSLJa1r+BR/98
-XIWzjfmBc2RbAgMBAAGjggMEMIIDADCBswYDVR0RBIGrMIGooD0GBWBMAQMEoDQEMjI5MDUxOTY5
-NDk1ODkwOTEwOTEwMDAwMDAwMDAwMDAwMDAwNDAzOTU3NDg1MlNTUFJToCIGBWBMAQMCoBkEF0NM
-RUlUT04gTUVTUVVJVEEgVkFSR0FToBkGBWBMAQMDoBAEDjkyNjYwNjA0MDAwMTgyoBcGBWBMAQMH
-oA4EDDAwMDAwMDAwMDAwMIEPZmlzY2FsQHlhcmEuY29tMAkGA1UdEwQCMAAwHwYDVR0jBBgwFoAU
-U31/nb7RYdAgutqf44mnE3NYzUIwfwYDVR0gBHgwdjB0BgZgTAECAQwwajBoBggrBgEFBQcCARZc
-aHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9kcGMvQUNfQ2Vy
-dGlzaWduX1JGQi9EUENfQUNfQ2VydGlzaWduX1JGQi5wZGYwgbwGA1UdHwSBtDCBsTBXoFWgU4ZR
-aHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9sY3IvQUNDZXJ0
-aXNpZ25SRkJHNS9MYXRlc3RDUkwuY3JsMFagVKBShlBodHRwOi8vaWNwLWJyYXNpbC5vdXRyYWxj
-ci5jb20uYnIvcmVwb3NpdG9yaW8vbGNyL0FDQ2VydGlzaWduUkZCRzUvTGF0ZXN0Q1JMLmNybDAO
-BgNVHQ8BAf8EBAMCBeAwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGsBggrBgEFBQcB
-AQSBnzCBnDBfBggrBgEFBQcwAoZTaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9y
-ZXBvc2l0b3Jpby9jZXJ0aWZpY2Fkb3MvQUNfQ2VydGlzaWduX1JGQl9HNS5wN2MwOQYIKwYBBQUH
-MAGGLWh0dHA6Ly9vY3NwLWFjLWNlcnRpc2lnbi1yZmIuY2VydGlzaWduLmNvbS5icjANBgkqhkiG
-9w0BAQsFAAOCAgEASCNnP1ersGgcFlHfGmfzgtSBVH0oJrVrm7/LFr2FjM8AjX9PY97brv6UubUj
-swAD+yL+dwwsuv1TxnBHw8AE8MGbxiZQTnNf0OMkIPAEDvwlb8SXK7Gk137JKUaKKGup5P4dbA8X
-M22+GEw1dMYjCV6eqJ2bxP1EjRII3rb8EsQATZ/pDizsEauNXOmXqbIefqU9wWaQhTQVtLwflrN0
-zElGDSX9uwtR6j28usr3KiKf26MfhtWDAombY+m9Bhq2Hys6hZpyfL+ERFoWXmpzlhmEvUFnMzL1
-SWGNeyhn+na7r7cJvBFcdPPyriZlAdApkaZGXSQAGW78gvlJLD2YtYk/BN02v7qCfhcPHdZcQ4XV
-kdj8idIMcn3ZiweWanaZ9riR3yLStxBP7arsQrMGOrYkAyo9otufpJfYS+FHkrJapqfZxbo0qCTs
-ZPHvAcMw8vCojT/Z2FZrGi6aDK2rt7hPhKYRedZNbDmVgKSRNBoyPqSoqNwMSEiF7EmXA5zq27SM
-87v096EsX8COhgxvMqj/ENxfj8x94POwH8gif/xv9r/raWYCrOnKNP8uhXJPdeihFZBsbWanSUZW
-YlltN/lCaF/oSDqsQjVaG4MndtddEIwdfk3xg71iptYN1tYWHSMal0EwKkOA3A9obwTtxz1fkp8F
-nGxIgi6QuCLfPTU=&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/NFe&gt;&lt;protNFe versao="4.00"&gt;&lt;infProt Id="ID131214505207714"&gt;
-  &lt;tpAmb&gt;1&lt;/tpAmb&gt;
-  &lt;verAplic&gt;14.4.46-SE6&lt;/verAplic&gt;
-  &lt;chNFe&gt;31211292660604017662550500000171731944724056&lt;/chNFe&gt;
-  &lt;dhRecbto&gt;2021-12-27T19:39:02-03:00&lt;/dhRecbto&gt;
-  &lt;nProt&gt;131214505207714&lt;/nProt&gt;
-  &lt;digVal&gt;Djka290DHdCz6hT6qZ9suLPJBhY=&lt;/digVal&gt;
-  &lt;cStat&gt;100&lt;/cStat&gt;
-  &lt;xMotivo&gt;Autorizado o uso da NF-e&lt;/xMotivo&gt;
-&lt;/infProt&gt;&lt;/protNFe&gt;&lt;/nfeProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35210904400329000109570010000586741000586744-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35210904400329000109570010000586741000586744-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35210904400329000109570010000586741000586744"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00058674&lt;/cCT&gt;&lt;CFOP&gt;5352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;58674&lt;/nCT&gt;&lt;dhEmi&gt;2021-09-18T08:05:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;4&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3517406&lt;/cMunEnv&gt;&lt;xMunEnv&gt;GUAIRA&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3547304&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTANA DE PARNAIBA&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3540804&lt;/cMunFim&gt;&lt;xMunFim&gt;POTIRENDABA&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;RODRIGO FERNANDES DE&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;SAP&lt;/xOrig&gt;&lt;xDest&gt;CTV&lt;/xDest&gt;&lt;xRota&gt;SAPCTV&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTANA DE PARNAIBA&lt;/origCalc&gt;&lt;destCalc&gt;CATANDUVA&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 131,78;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;C0254&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;75.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;DIVANJIR DOS SANTOS&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;141.798.608-56&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;EGG3H59&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FPZ2F54&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FKM6A76&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FPC-8J55&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;04400329000109&lt;/CNPJ&gt;&lt;IE&gt;322079785116&lt;/IE&gt;&lt;xNome&gt;RODOTAC TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;RODOTAC (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOAO JORGE GARCIA LEAL&lt;/xLgr&gt;&lt;nro&gt;607&lt;/nro&gt;&lt;xBairro&gt;PARQUE INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3517406&lt;/cMun&gt;&lt;xMun&gt;GUAIRA&lt;/xMun&gt;&lt;CEP&gt;14790000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733302455&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;00255910000115&lt;/CNPJ&gt;&lt;IE&gt;623015454110&lt;/IE&gt;&lt;xNome&gt;GEOCAL MINERACAO LTDA&lt;/xNome&gt;&lt;xFant&gt;GEOCAL MINERACAO&lt;/xFant&gt;&lt;fone&gt;01141568999&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;EST ANA PROCOPIO DE MORAES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;VARZEA DO SOUZA&lt;/xBairro&gt;&lt;cMun&gt;3547304&lt;/cMun&gt;&lt;xMun&gt;SANTANA DE PARNAIBA&lt;/xMun&gt;&lt;CEP&gt;06528551&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;06315338015060&lt;/CNPJ&gt;&lt;IE&gt;556013690112&lt;/IE&gt;&lt;xNome&gt;COFCO BRASIL S.A&lt;/xNome&gt;&lt;fone&gt;01738279900&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;ESTRADA MUNICIPAL IBIRA A POTIRENDABA&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;ZONA RURAL&lt;/xBairro&gt;&lt;cMun&gt;3540804&lt;/cMun&gt;&lt;xMun&gt;POTIRENDABA&lt;/xMun&gt;&lt;CEP&gt;15105000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;3610.50&lt;/vTPrest&gt;&lt;vRec&gt;3610.50&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;2962.50&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;648.00&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;131.79&lt;/vTotTrib&gt;&lt;infAdFisco&gt;ICMS DIFERIDO CONFORME ARTIGO 358 DO RICMS&lt;/infAdFisco&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;2888.40&lt;/vCarga&gt;&lt;proPred&gt;CALCARIO AGRICOLA GEOFERTIL&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;48140.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;0.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;2888.40&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35210900255910000115550010005056511503387767&lt;/chave&gt;&lt;dPrev&gt;2021-09-18&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;02625527&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-09-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35210904400329000109570010000586741000586744&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35210904400329000109570010000586741000586744"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;OW4QuRBv3xmZunu85fl4gWKUneE=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;HBFGob9CcRx6P2neumY6wjxip8VD6DsUqdU8H4CJbTOFajDucAeQmY9DECDq89RAlED3Fo52apTT84DBhnBPbDKEHS0KX4zpaJ/d156dJ6WWFTus2Mu3+XkuVNxl4p/PSA7gq3GeCFV/f1e6S/RV86AkzzQig8spYAJDa3jLjBtL9CluLEPod6g6hweysz/LcIe0fSkdx+rKDKaTgJh2wOmLUPWsMaK+Gg5wy0+P3ALfLvyESq6sBedm6WvN9ih0uAnDuQm04Wjtjnwz2oQkvI8Hm5hyWls6YTr5U9nRp2GRj38ZrQOmuIricvwdjlf9oF8M7/ysM7Xa97hR8+c+yQ==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHNzCCBR+gAwIBAgIIfFghCRNtqPgwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDIwMFoXDTIyMDkxNDEzNDIwMFowgdwxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDEPMA0GA1UEBxMGR3VhaXJhMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTEwMC4GA1UEAxMnUk9ET1RBQyBUUkFOU1BPUlRFUyBMVERBOjA0NDAwMzI5MDAwMTA5MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAp04ol/u6OamuPQYiuYvmBoabm9447ej3qfCk6KQY+gVddtzabeHC4yK1n9UOseY/2g2Wz2OQuVjZBz1mLb5aKDW9Hx4Hg4JXosEhRgHv+FxtlrgGJps+vVSke1fDiRKB9RxkryP5ngl3fOTaDXyXKAVw5Xir/ireILJkxoa7yItj3qOoX3WXO0e8IBBjeOJ3PyllIvh06I3LHaeqr6+hWxwuNsSxdYVLl+x0J5A1p8O+9MWEgTL6zEuST5aIoeESpEKC/oiOZwHujV8Zp6Ld3tbV45cNmE5qyq0Cv6WMxvySvmtBwBIS/2ftmk8dMnZb+R+iiO4Gh5gEFQ36XU3ezQIDAQABo4ICfTCCAnkwHwYDVR0jBBgwFoAUP9NcqRlN14gWLZgMrwre4U8kFrAwWQYIKwYBBQUHAQEETTBLMEkGCCsGAQUFBzAChj1odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUucDdiMIGvBgNVHREEgacwgaSBFnJvZG90YWNAcm9kb3RhYy5uZXQuYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMOMDQ0MDAzMjkwMDAxMDmgOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBTmf74GOUuAKM5iWH+pal5k4kRQYDAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAKffeE7P7VJywGR4dL48Nfq75Oa0zAPHLV/DXwo/bs847MeSBdauzpEiZ5xsUssJS/n73euRm/aaQ0Ai0fTYDcl6DAj0Bpn0kE3N9MF0/rb/35Ion/zwbhfzLHSby6MuH+NXvZheexyZV+LdWMnTY875AhHqFTLMH/e7TML3AukZFVrZDZ/KyjVGNji6XTmOxg0qt3hiEapOR+ODEqZO6FiYYS/7DGu+akrOzT8eOTddbUUzx2eZ6PctqSV7TZXTYtkfrq9pZgcFMjKUxwtnaQ9iE1ZttFTcVqIOWxPFLc/5pxFRfaFL+/5dhRs777Fox5nHBE9GjaI2alR9fidF4BJ+4UkcEZ17NaS8tzGYuP3XjieSWQD5eEAaGDA4eS+0zpNP6Z30UFqc5gmfj8EZaRuxaAUe+egORdxErP3J7CBPFEei/t1V/+E56JKHe75TgM+hTb+gxKyVThQULKZQgv/OiXD0O+cRBNHx0wNyvr/Srh61E9os66kg37kgfNZnMwBZOG4QmUtjJA5ChzJ99yXk6hNKhWXZrB+WwlBa2X/b/cff2nKx9wnw0ii3xjIAnkcWs2koAw5QaLUpNlHBTdTDVTMYZsXP9fSGKeom+/QDE6tZ5EstYiopzB2LRCGIB/PAwuYJX5fbcyMQTiu0A/6OCjQ3Bk9dK6myCbqSXJDb&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35210904400329000109570010000586741000586744&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-09-18T08:06:28-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214243583602&lt;/nProt&gt;&lt;digVal&gt;OW4QuRBv3xmZunu85fl4gWKUneE=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35211004400329000109570010000591261000591268-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211004400329000109570010000591261000591268-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211004400329000109570010000591261000591268"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00059126&lt;/cCT&gt;&lt;CFOP&gt;1206&lt;/CFOP&gt;&lt;natOp&gt;ANULACAO DE VR REF PRESTACAO SERV DE TRANSPORTE&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;59126&lt;/nCT&gt;&lt;dhEmi&gt;2021-10-08T10:52:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;8&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;2&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3517406&lt;/cMunEnv&gt;&lt;xMunEnv&gt;GUAIRA&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3547304&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTANA DE PARNAIBA&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3540804&lt;/cMunFim&gt;&lt;xMunFim&gt;POTIRENDABA&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Anulacao&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;SAP&lt;/xOrig&gt;&lt;xDest&gt;PO1&lt;/xDest&gt;&lt;xRota&gt;SAPPO1&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTANA DE PARNAIBA&lt;/origCalc&gt;&lt;destCalc&gt;POTIRENDABA&lt;/destCalc&gt;&lt;xObs&gt;ANULACAO DE VALOR RELATIVO A PRESTACAO DE SERVICO DE TRANSPORTE REF. AO CT-e 58674 DO DIA 18/09/2021. CONFORME EVENTO DE RECUSA DO TOMADOR COFCO BRASIL S.A - CPJ: 06.315.338/0150-60.&lt;/xObs&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;DIVANJIR DOS SANTOS&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;141.798.608-56&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;EGG3H59&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FPZ2F54&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FKM6A76&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FPC-8J55&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;04400329000109&lt;/CNPJ&gt;&lt;IE&gt;322079785116&lt;/IE&gt;&lt;xNome&gt;RODOTAC TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;RODOTAC (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOAO JORGE GARCIA LEAL&lt;/xLgr&gt;&lt;nro&gt;607&lt;/nro&gt;&lt;xBairro&gt;PARQUE INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3517406&lt;/cMun&gt;&lt;xMun&gt;GUAIRA&lt;/xMun&gt;&lt;CEP&gt;14790000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733302455&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;00255910000115&lt;/CNPJ&gt;&lt;IE&gt;623015454110&lt;/IE&gt;&lt;xNome&gt;GEOCAL MINERACAO LTDA&lt;/xNome&gt;&lt;xFant&gt;GEOCAL MINERACAO&lt;/xFant&gt;&lt;fone&gt;01141568999&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;EST ANA PROCOPIO DE MORAES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;VARZEA DO SOUZA&lt;/xBairro&gt;&lt;cMun&gt;3547304&lt;/cMun&gt;&lt;xMun&gt;SANTANA DE PARNAIBA&lt;/xMun&gt;&lt;CEP&gt;06528551&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;06315338015060&lt;/CNPJ&gt;&lt;IE&gt;556013690112&lt;/IE&gt;&lt;xNome&gt;COFCO BRASIL S.A&lt;/xNome&gt;&lt;fone&gt;01738279900&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;ESTRADA MUNICIPAL IBIRA A POTIRENDABA&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;ZONA RURAL&lt;/xBairro&gt;&lt;cMun&gt;3540804&lt;/cMun&gt;&lt;xMun&gt;POTIRENDABA&lt;/xMun&gt;&lt;CEP&gt;15105000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;3610.50&lt;/vTPrest&gt;&lt;vRec&gt;3610.50&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;2962.50&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;648.00&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;131.79&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCteAnu&gt;&lt;chCte&gt;35210904400329000109570010000586741000586744&lt;/chCte&gt;&lt;dEmi&gt;2021-10-08&lt;/dEmi&gt;&lt;/infCteAnu&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211004400329000109570010000591261000591268&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211004400329000109570010000591261000591268"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;ggIv8Z1F6UTdw/9c+83jPoR43Cc=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;JRIjJcWxhuWMVY61VmLZUQtby0wkTyNC583vUDexP3QblFiilhTlh8e5A3Snv6Jd0jCVTQcW55+Uux+tlA//XHfMzrWKrT8pAon6l3SSudO5b1kgLaDwsaUqLrmymCN1qdI07XJZRDG4Lxwe+CmPgAvqjoDtEetT1ng+C+R2mxaiHCzVbwWvoiZqcogkBdXhZdGOTK3iC391LrJbHeNC2Fpgawv5rwQavRyFIH3wAOh1lN6cbvcgv3vZKlOjUHQnFL5vVeGNe4MmQM56Q0LWJlp5UrLYTQ4yzLcEQoYEh3xKfGlZ0bd9M+LqSPZqGC4zi2WCLc0Kop5bRpYVbvE7DA==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHNzCCBR+gAwIBAgIIfFghCRNtqPgwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDIwMFoXDTIyMDkxNDEzNDIwMFowgdwxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDEPMA0GA1UEBxMGR3VhaXJhMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTEwMC4GA1UEAxMnUk9ET1RBQyBUUkFOU1BPUlRFUyBMVERBOjA0NDAwMzI5MDAwMTA5MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAp04ol/u6OamuPQYiuYvmBoabm9447ej3qfCk6KQY+gVddtzabeHC4yK1n9UOseY/2g2Wz2OQuVjZBz1mLb5aKDW9Hx4Hg4JXosEhRgHv+FxtlrgGJps+vVSke1fDiRKB9RxkryP5ngl3fOTaDXyXKAVw5Xir/ireILJkxoa7yItj3qOoX3WXO0e8IBBjeOJ3PyllIvh06I3LHaeqr6+hWxwuNsSxdYVLl+x0J5A1p8O+9MWEgTL6zEuST5aIoeESpEKC/oiOZwHujV8Zp6Ld3tbV45cNmE5qyq0Cv6WMxvySvmtBwBIS/2ftmk8dMnZb+R+iiO4Gh5gEFQ36XU3ezQIDAQABo4ICfTCCAnkwHwYDVR0jBBgwFoAUP9NcqRlN14gWLZgMrwre4U8kFrAwWQYIKwYBBQUHAQEETTBLMEkGCCsGAQUFBzAChj1odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUucDdiMIGvBgNVHREEgacwgaSBFnJvZG90YWNAcm9kb3RhYy5uZXQuYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMOMDQ0MDAzMjkwMDAxMDmgOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBTmf74GOUuAKM5iWH+pal5k4kRQYDAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAKffeE7P7VJywGR4dL48Nfq75Oa0zAPHLV/DXwo/bs847MeSBdauzpEiZ5xsUssJS/n73euRm/aaQ0Ai0fTYDcl6DAj0Bpn0kE3N9MF0/rb/35Ion/zwbhfzLHSby6MuH+NXvZheexyZV+LdWMnTY875AhHqFTLMH/e7TML3AukZFVrZDZ/KyjVGNji6XTmOxg0qt3hiEapOR+ODEqZO6FiYYS/7DGu+akrOzT8eOTddbUUzx2eZ6PctqSV7TZXTYtkfrq9pZgcFMjKUxwtnaQ9iE1ZttFTcVqIOWxPFLc/5pxFRfaFL+/5dhRs777Fox5nHBE9GjaI2alR9fidF4BJ+4UkcEZ17NaS8tzGYuP3XjieSWQD5eEAaGDA4eS+0zpNP6Z30UFqc5gmfj8EZaRuxaAUe+egORdxErP3J7CBPFEei/t1V/+E56JKHe75TgM+hTb+gxKyVThQULKZQgv/OiXD0O+cRBNHx0wNyvr/Srh61E9os66kg37kgfNZnMwBZOG4QmUtjJA5ChzJ99yXk6hNKhWXZrB+WwlBa2X/b/cff2nKx9wnw0ii3xjIAnkcWs2koAw5QaLUpNlHBTdTDVTMYZsXP9fSGKeom+/QDE6tZ5EstYiopzB2LRCGIB/PAwuYJX5fbcyMQTiu0A/6OCjQ3Bk9dK6myCbqSXJDb&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211004400329000109570010000591261000591268&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-10-08T10:56:54-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214330960036&lt;/nProt&gt;&lt;digVal&gt;ggIv8Z1F6UTdw/9c+83jPoR43Cc=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35211204400329000109570010000605331000605338-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211204400329000109570010000605331000605338-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211204400329000109570010000605331000605338"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00060533&lt;/cCT&gt;&lt;CFOP&gt;6932&lt;/CFOP&gt;&lt;natOp&gt;PR.SERV.TRANSP.INIC.FORA ESTAD&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;60533&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-22T15:02:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;8&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3517406&lt;/cMunEnv&gt;&lt;xMunEnv&gt;GUAIRA&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;1&lt;/tpServ&gt;&lt;cMunIni&gt;3166808&lt;/cMunIni&gt;&lt;xMunIni&gt;SERRA DO SALITRE&lt;/xMunIni&gt;&lt;UFIni&gt;MG&lt;/UFIni&gt;&lt;cMunFim&gt;3513504&lt;/cMunFim&gt;&lt;xMunFim&gt;CUBATAO&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma4&gt;&lt;toma&gt;4&lt;/toma&gt;&lt;CNPJ&gt;50505924000703&lt;/CNPJ&gt;&lt;IE&gt;0034911940042&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (F.UBE)&lt;/xFant&gt;&lt;enderToma&gt;&lt;xLgr&gt;FILOMENA CARTAFINA&lt;/xLgr&gt;&lt;nro&gt;22031&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044750&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderToma&gt;&lt;/toma4&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Subcontratacao&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;SSL&lt;/xOrig&gt;&lt;xDest&gt;CBT&lt;/xDest&gt;&lt;xRota&gt;SSLCBT&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SERRA DO SALITRE&lt;/origCalc&gt;&lt;destCalc&gt;CUBATAO&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 235,39;CT-e EMITIDO SOMENTE P/EFEITO DE COBRANCA, NAO INC.ICMS, CONF.INC I DO ART.205 DO RICMS/00 - SUBCONTRATADO POR TRANSMOB TRANSPORTE LTDA CNPJ:50.505.924/0007-03, N°8576 Referencia do Cliente : 1-8576-1;&lt;/xObs&gt;&lt;ObsCont xCampo="frotas"&gt;&lt;xTexto&gt;C0192&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_clientes"&gt;&lt;xTexto&gt;1-8576-1&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_tons"&gt;&lt;xTexto&gt;135.170000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;FABIO PRADO MARQUES VIEIRA&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;138.685.928-14&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;GFN2119&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FEY9191&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FWJ9B53&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FQA-7202&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;04400329000109&lt;/CNPJ&gt;&lt;IE&gt;322079785116&lt;/IE&gt;&lt;xNome&gt;RODOTAC TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;RODOTAC (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOAO JORGE GARCIA LEAL&lt;/xLgr&gt;&lt;nro&gt;607&lt;/nro&gt;&lt;xBairro&gt;PARQUE INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3517406&lt;/cMun&gt;&lt;xMun&gt;GUAIRA&lt;/xMun&gt;&lt;CEP&gt;14790000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733302455&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;92660604017662&lt;/CNPJ&gt;&lt;IE&gt;2874585321020&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;xFant&gt;YARA BRASIL&lt;/xFant&gt;&lt;fone&gt;01938849300&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;FAZENDA SALITRE S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MARRUA&lt;/xBairro&gt;&lt;cMun&gt;3166808&lt;/cMun&gt;&lt;xMun&gt;SERRA DO SALITRE&lt;/xMun&gt;&lt;CEP&gt;38760000&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;06225292000147&lt;/CNPJ&gt;&lt;IE&gt;283108491118&lt;/IE&gt;&lt;xNome&gt;TERLOC - TERMINAL LOGISTICO CESARI LTDA&lt;/xNome&gt;&lt;fone&gt;01321028013&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV ENGENHEIRO PLINIO DE QUEIROZ S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xCpl&gt;SP 55&lt;/xCpl&gt;&lt;xBairro&gt;PIACAGUERA&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;CUBATAO&lt;/xMun&gt;&lt;CEP&gt;11570000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;6448.96&lt;/vTPrest&gt;&lt;vRec&gt;6448.96&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;5312.26&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;1136.70&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;235.39&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;56990.55&lt;/vCarga&gt;&lt;proPred&gt;ROCHA&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;47710.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;48.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;56990.55&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;31211292660604017662550500000170671478739470&lt;/chave&gt;&lt;dPrev&gt;2021-12-23&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;docAnt&gt;&lt;emiDocAnt&gt;&lt;CNPJ&gt;50505924000703&lt;/CNPJ&gt;&lt;IE&gt;0034911940042&lt;/IE&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;idDocAnt&gt;&lt;idDocAntEle&gt;&lt;chCTe&gt;31211250505924000703570010000085761000085764&lt;/chCTe&gt;&lt;/idDocAntEle&gt;&lt;/idDocAnt&gt;&lt;/emiDocAnt&gt;&lt;/docAnt&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;02625527&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211204400329000109570010000605331000605338&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211204400329000109570010000605331000605338"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;KKZCCpyMgSz5Wd9oeGPIJ2PKMvU=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;V/5T8AkwSk6SJbrfeMUlwxzvZwnrrqVr8PQyQpnguNUj5tY9MGWBIQPKCpjSFY7trudTYIHTs8bircaC0Py/hd8iUTWsW8utZDpZHauJtOfKQpekTKAffdhbseFdTkXzDMWywFBLPuQ2rO0wjcDeXqbXhcthrRl/oj2V+j1dd/o3n+iO9Ng+qrKtBEO8hTtv0BTaWHbERJ4mXwOcyZB1EnmmXdRg/3WCsh5Z+AgHwZx8bYmww/hLE+WDUdFp4PKsU4qgKMsvHQXgbuHLFgA99kIUsj2PDaD7zkD4bgUNPCfNEV1XCi243bEwr2LIUNpVGOiJNUJbc1C4eVRBegdLKQ==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHNzCCBR+gAwIBAgIIfFghCRNtqPgwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDIwMFoXDTIyMDkxNDEzNDIwMFowgdwxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDEPMA0GA1UEBxMGR3VhaXJhMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTEwMC4GA1UEAxMnUk9ET1RBQyBUUkFOU1BPUlRFUyBMVERBOjA0NDAwMzI5MDAwMTA5MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAp04ol/u6OamuPQYiuYvmBoabm9447ej3qfCk6KQY+gVddtzabeHC4yK1n9UOseY/2g2Wz2OQuVjZBz1mLb5aKDW9Hx4Hg4JXosEhRgHv+FxtlrgGJps+vVSke1fDiRKB9RxkryP5ngl3fOTaDXyXKAVw5Xir/ireILJkxoa7yItj3qOoX3WXO0e8IBBjeOJ3PyllIvh06I3LHaeqr6+hWxwuNsSxdYVLl+x0J5A1p8O+9MWEgTL6zEuST5aIoeESpEKC/oiOZwHujV8Zp6Ld3tbV45cNmE5qyq0Cv6WMxvySvmtBwBIS/2ftmk8dMnZb+R+iiO4Gh5gEFQ36XU3ezQIDAQABo4ICfTCCAnkwHwYDVR0jBBgwFoAUP9NcqRlN14gWLZgMrwre4U8kFrAwWQYIKwYBBQUHAQEETTBLMEkGCCsGAQUFBzAChj1odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUucDdiMIGvBgNVHREEgacwgaSBFnJvZG90YWNAcm9kb3RhYy5uZXQuYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMOMDQ0MDAzMjkwMDAxMDmgOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBTmf74GOUuAKM5iWH+pal5k4kRQYDAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAKffeE7P7VJywGR4dL48Nfq75Oa0zAPHLV/DXwo/bs847MeSBdauzpEiZ5xsUssJS/n73euRm/aaQ0Ai0fTYDcl6DAj0Bpn0kE3N9MF0/rb/35Ion/zwbhfzLHSby6MuH+NXvZheexyZV+LdWMnTY875AhHqFTLMH/e7TML3AukZFVrZDZ/KyjVGNji6XTmOxg0qt3hiEapOR+ODEqZO6FiYYS/7DGu+akrOzT8eOTddbUUzx2eZ6PctqSV7TZXTYtkfrq9pZgcFMjKUxwtnaQ9iE1ZttFTcVqIOWxPFLc/5pxFRfaFL+/5dhRs777Fox5nHBE9GjaI2alR9fidF4BJ+4UkcEZ17NaS8tzGYuP3XjieSWQD5eEAaGDA4eS+0zpNP6Z30UFqc5gmfj8EZaRuxaAUe+egORdxErP3J7CBPFEei/t1V/+E56JKHe75TgM+hTb+gxKyVThQULKZQgv/OiXD0O+cRBNHx0wNyvr/Srh61E9os66kg37kgfNZnMwBZOG4QmUtjJA5ChzJ99yXk6hNKhWXZrB+WwlBa2X/b/cff2nKx9wnw0ii3xjIAnkcWs2koAw5QaLUpNlHBTdTDVTMYZsXP9fSGKeom+/QDE6tZ5EstYiopzB2LRCGIB/PAwuYJX5fbcyMQTiu0A/6OCjQ3Bk9dK6myCbqSXJDb&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211204400329000109570010000605331000605338&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-22T15:16:13-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214662606854&lt;/nProt&gt;&lt;digVal&gt;KKZCCpyMgSz5Wd9oeGPIJ2PKMvU=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35211204400329000109570010000605341000605343-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211204400329000109570010000605341000605343-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211204400329000109570010000605341000605343"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00060534&lt;/cCT&gt;&lt;CFOP&gt;6932&lt;/CFOP&gt;&lt;natOp&gt;PR.SERV.TRANSP.INIC.FORA ESTAD&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;60534&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-22T15:02:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;3&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3517406&lt;/cMunEnv&gt;&lt;xMunEnv&gt;GUAIRA&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;1&lt;/tpServ&gt;&lt;cMunIni&gt;3166808&lt;/cMunIni&gt;&lt;xMunIni&gt;SERRA DO SALITRE&lt;/xMunIni&gt;&lt;UFIni&gt;MG&lt;/UFIni&gt;&lt;cMunFim&gt;3513504&lt;/cMunFim&gt;&lt;xMunFim&gt;CUBATAO&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma4&gt;&lt;toma&gt;4&lt;/toma&gt;&lt;CNPJ&gt;50505924000703&lt;/CNPJ&gt;&lt;IE&gt;0034911940042&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (F.UBE)&lt;/xFant&gt;&lt;enderToma&gt;&lt;xLgr&gt;FILOMENA CARTAFINA&lt;/xLgr&gt;&lt;nro&gt;22031&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044750&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderToma&gt;&lt;/toma4&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Subcontratacao&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;SSL&lt;/xOrig&gt;&lt;xDest&gt;CBT&lt;/xDest&gt;&lt;xRota&gt;SSLCBT&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SERRA DO SALITRE&lt;/origCalc&gt;&lt;destCalc&gt;CUBATAO&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 235,19;CT-e EMITIDO SOMENTE P/EFEITO DE COBRANCA, NAO INC.ICMS, CONF.INC I DO ART.205 DO RICMS/00 - SUBCONTRATADO POR TRANSMOB TRANSPORTE LTDA CNPJ:50.505.924/0007-03, N°8578 Referencia do Cliente : 1-8578-1;&lt;/xObs&gt;&lt;ObsCont xCampo="frotas"&gt;&lt;xTexto&gt;C0204&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_clientes"&gt;&lt;xTexto&gt;1-8578-1&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_tons"&gt;&lt;xTexto&gt;135.170000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;JOSE CARLOS DOS SANTOS&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;504.765.569-53&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;GDG9454&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FUE9704&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;GGI4766&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FUP-0535&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;04400329000109&lt;/CNPJ&gt;&lt;IE&gt;322079785116&lt;/IE&gt;&lt;xNome&gt;RODOTAC TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;RODOTAC (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOAO JORGE GARCIA LEAL&lt;/xLgr&gt;&lt;nro&gt;607&lt;/nro&gt;&lt;xBairro&gt;PARQUE INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3517406&lt;/cMun&gt;&lt;xMun&gt;GUAIRA&lt;/xMun&gt;&lt;CEP&gt;14790000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733302455&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;92660604017662&lt;/CNPJ&gt;&lt;IE&gt;2874585321020&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;xFant&gt;YARA BRASIL&lt;/xFant&gt;&lt;fone&gt;01938849300&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;FAZENDA SALITRE S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MARRUA&lt;/xBairro&gt;&lt;cMun&gt;3166808&lt;/cMun&gt;&lt;xMun&gt;SERRA DO SALITRE&lt;/xMun&gt;&lt;CEP&gt;38760000&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;06225292000147&lt;/CNPJ&gt;&lt;IE&gt;283108491118&lt;/IE&gt;&lt;xNome&gt;TERLOC - TERMINAL LOGISTICO CESARI LTDA&lt;/xNome&gt;&lt;fone&gt;01321028013&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV ENGENHEIRO PLINIO DE QUEIROZ S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xCpl&gt;SP 55&lt;/xCpl&gt;&lt;xBairro&gt;PIACAGUERA&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;CUBATAO&lt;/xMun&gt;&lt;CEP&gt;11570000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;6443.55&lt;/vTPrest&gt;&lt;vRec&gt;6443.55&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;5306.85&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;1136.70&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;235.19&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;56942.77&lt;/vCarga&gt;&lt;proPred&gt;ROCHA&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;47670.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;48.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;56942.77&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;31211292660604017662550500000170691908499198&lt;/chave&gt;&lt;dPrev&gt;2021-12-23&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;docAnt&gt;&lt;emiDocAnt&gt;&lt;CNPJ&gt;50505924000703&lt;/CNPJ&gt;&lt;IE&gt;0034911940042&lt;/IE&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;idDocAnt&gt;&lt;idDocAntEle&gt;&lt;chCTe&gt;31211250505924000703570010000085781000085785&lt;/chCTe&gt;&lt;/idDocAntEle&gt;&lt;/idDocAnt&gt;&lt;/emiDocAnt&gt;&lt;/docAnt&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;02625527&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211204400329000109570010000605341000605343&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211204400329000109570010000605341000605343"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;umO9aChCes6otUORd1rXra3i2ew=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;JPZ11sv6wvKyNB09EnX/r7LLf1H0pc6B5JySt5GFVePR0jedQT95KdMVEm6GsCy/Z+ZkVWM9V5y37ICHeZQXututouGI3OpLBWGNKfbUXsocb0zlst9DfEPmEKQrg72soCt4LYQfACQRPeBgvwxReMRFgbexPAss5KEyfi90i9mJCmRowYpq6/+AI7nu+eJ6XjWjidJ4qXpmOs3itmWJqXqrACsH4caOnqTYm387R20UrCteQocStnms5MdiQcB3EcT5epa7QFxSzSRd5IKBDQNsimoZgdxXMUsU7Vs9/9C5GfqcUtUYY+yhcGk9UaMFQe4n7qJRT+duLO10+KUO6A==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHNzCCBR+gAwIBAgIIfFghCRNtqPgwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDIwMFoXDTIyMDkxNDEzNDIwMFowgdwxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDEPMA0GA1UEBxMGR3VhaXJhMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTEwMC4GA1UEAxMnUk9ET1RBQyBUUkFOU1BPUlRFUyBMVERBOjA0NDAwMzI5MDAwMTA5MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAp04ol/u6OamuPQYiuYvmBoabm9447ej3qfCk6KQY+gVddtzabeHC4yK1n9UOseY/2g2Wz2OQuVjZBz1mLb5aKDW9Hx4Hg4JXosEhRgHv+FxtlrgGJps+vVSke1fDiRKB9RxkryP5ngl3fOTaDXyXKAVw5Xir/ireILJkxoa7yItj3qOoX3WXO0e8IBBjeOJ3PyllIvh06I3LHaeqr6+hWxwuNsSxdYVLl+x0J5A1p8O+9MWEgTL6zEuST5aIoeESpEKC/oiOZwHujV8Zp6Ld3tbV45cNmE5qyq0Cv6WMxvySvmtBwBIS/2ftmk8dMnZb+R+iiO4Gh5gEFQ36XU3ezQIDAQABo4ICfTCCAnkwHwYDVR0jBBgwFoAUP9NcqRlN14gWLZgMrwre4U8kFrAwWQYIKwYBBQUHAQEETTBLMEkGCCsGAQUFBzAChj1odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUucDdiMIGvBgNVHREEgacwgaSBFnJvZG90YWNAcm9kb3RhYy5uZXQuYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMOMDQ0MDAzMjkwMDAxMDmgOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBTmf74GOUuAKM5iWH+pal5k4kRQYDAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAKffeE7P7VJywGR4dL48Nfq75Oa0zAPHLV/DXwo/bs847MeSBdauzpEiZ5xsUssJS/n73euRm/aaQ0Ai0fTYDcl6DAj0Bpn0kE3N9MF0/rb/35Ion/zwbhfzLHSby6MuH+NXvZheexyZV+LdWMnTY875AhHqFTLMH/e7TML3AukZFVrZDZ/KyjVGNji6XTmOxg0qt3hiEapOR+ODEqZO6FiYYS/7DGu+akrOzT8eOTddbUUzx2eZ6PctqSV7TZXTYtkfrq9pZgcFMjKUxwtnaQ9iE1ZttFTcVqIOWxPFLc/5pxFRfaFL+/5dhRs777Fox5nHBE9GjaI2alR9fidF4BJ+4UkcEZ17NaS8tzGYuP3XjieSWQD5eEAaGDA4eS+0zpNP6Z30UFqc5gmfj8EZaRuxaAUe+egORdxErP3J7CBPFEei/t1V/+E56JKHe75TgM+hTb+gxKyVThQULKZQgv/OiXD0O+cRBNHx0wNyvr/Srh61E9os66kg37kgfNZnMwBZOG4QmUtjJA5ChzJ99yXk6hNKhWXZrB+WwlBa2X/b/cff2nKx9wnw0ii3xjIAnkcWs2koAw5QaLUpNlHBTdTDVTMYZsXP9fSGKeom+/QDE6tZ5EstYiopzB2LRCGIB/PAwuYJX5fbcyMQTiu0A/6OCjQ3Bk9dK6myCbqSXJDb&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211204400329000109570010000605341000605343&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-22T15:16:15-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214662606945&lt;/nProt&gt;&lt;digVal&gt;umO9aChCes6otUORd1rXra3i2ew=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35211204400329000109570010000605431000605431-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211204400329000109570010000605431000605431-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211204400329000109570010000605431000605431"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00060543&lt;/cCT&gt;&lt;CFOP&gt;6932&lt;/CFOP&gt;&lt;natOp&gt;PR.SERV.TRANSP.INIC.FORA ESTAD&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;60543&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-23T15:21:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;1&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3517406&lt;/cMunEnv&gt;&lt;xMunEnv&gt;GUAIRA&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;1&lt;/tpServ&gt;&lt;cMunIni&gt;3166808&lt;/cMunIni&gt;&lt;xMunIni&gt;SERRA DO SALITRE&lt;/xMunIni&gt;&lt;UFIni&gt;MG&lt;/UFIni&gt;&lt;cMunFim&gt;3513504&lt;/cMunFim&gt;&lt;xMunFim&gt;CUBATAO&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma4&gt;&lt;toma&gt;4&lt;/toma&gt;&lt;CNPJ&gt;50505924000703&lt;/CNPJ&gt;&lt;IE&gt;0034911940042&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (F.UBE)&lt;/xFant&gt;&lt;enderToma&gt;&lt;xLgr&gt;FILOMENA CARTAFINA&lt;/xLgr&gt;&lt;nro&gt;22031&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044750&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderToma&gt;&lt;/toma4&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Subcontratacao&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;SSL&lt;/xOrig&gt;&lt;xDest&gt;CBT&lt;/xDest&gt;&lt;xRota&gt;SSLCBT&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SERRA DO SALITRE&lt;/origCalc&gt;&lt;destCalc&gt;CUBATAO&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 233,96;CT-e EMITIDO SOMENTE P/EFEITO DE COBRANCA, NAO INC.ICMS, CONF.INC I DO ART.205 DO RICMS/00 - SUBCONTRATADO POR TRANSMOB TRANSPORTE LTDA CNPJ:50.505.924/0007-03, N°8588 Referencia do Cliente : 1-8588-1;&lt;/xObs&gt;&lt;ObsCont xCampo="frotas"&gt;&lt;xTexto&gt;C0260&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_clientes"&gt;&lt;xTexto&gt;1-8588-1&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_tons"&gt;&lt;xTexto&gt;135.170000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;WILSON APARECIDO DOS SANTOS&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;077.771.038-22&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;GHL1A73&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FFK5B74&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FMJ8I56&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FPE-8F35&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;04400329000109&lt;/CNPJ&gt;&lt;IE&gt;322079785116&lt;/IE&gt;&lt;xNome&gt;RODOTAC TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;RODOTAC (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOAO JORGE GARCIA LEAL&lt;/xLgr&gt;&lt;nro&gt;607&lt;/nro&gt;&lt;xBairro&gt;PARQUE INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3517406&lt;/cMun&gt;&lt;xMun&gt;GUAIRA&lt;/xMun&gt;&lt;CEP&gt;14790000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733302455&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;92660604017662&lt;/CNPJ&gt;&lt;IE&gt;2874585321020&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;xFant&gt;YARA BRASIL&lt;/xFant&gt;&lt;fone&gt;01938849300&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;FAZENDA SALITRE S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MARRUA&lt;/xBairro&gt;&lt;cMun&gt;3166808&lt;/cMun&gt;&lt;xMun&gt;SERRA DO SALITRE&lt;/xMun&gt;&lt;CEP&gt;38760000&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;06225292000147&lt;/CNPJ&gt;&lt;IE&gt;283108491118&lt;/IE&gt;&lt;xNome&gt;TERLOC - TERMINAL LOGISTICO CESARI LTDA&lt;/xNome&gt;&lt;fone&gt;01321028013&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV ENGENHEIRO PLINIO DE QUEIROZ S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xCpl&gt;SP 55&lt;/xCpl&gt;&lt;xBairro&gt;PIACAGUERA&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;CUBATAO&lt;/xMun&gt;&lt;CEP&gt;11570000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;6409.76&lt;/vTPrest&gt;&lt;vRec&gt;6409.76&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;5273.06&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;1136.70&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;233.95&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;56644.14&lt;/vCarga&gt;&lt;proPred&gt;ROCHA&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;47420.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;1.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;56644.14&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;31211292660604017662550500000171131478426760&lt;/chave&gt;&lt;dPrev&gt;2021-12-24&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;docAnt&gt;&lt;emiDocAnt&gt;&lt;CNPJ&gt;50505924000703&lt;/CNPJ&gt;&lt;IE&gt;0034911940042&lt;/IE&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;idDocAnt&gt;&lt;idDocAntEle&gt;&lt;chCTe&gt;31211250505924000703570010000085881000085889&lt;/chCTe&gt;&lt;/idDocAntEle&gt;&lt;/idDocAnt&gt;&lt;/emiDocAnt&gt;&lt;/docAnt&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;02625527&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211204400329000109570010000605431000605431&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211204400329000109570010000605431000605431"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;vzv0sCukuogBoZeqbccqOO1OzOw=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;UIMulv2y5qCu70XJDO0p8YV9UeZAfenFzb8WCCoc8AopoCykWTLrDk88mpvkM43kBkEFeEg7Bvyw9cAaqRMm8UtvreteEDe+Ajr9YjPfnwSQHuSnJqljL9uVYKOhLplLvOPs2wkpDlpVJRCOMDVzr09X3tXSBd1gihnfztrkfyOCLownv0FOAPPBRq8nZ+cFd1420F7aZpI73saC7HBVf4k2u27Uwy691lDDbaS+7Ak/73u4T/V9WKujf7T1n0JpDlCh4zxY3GWSePZ1zDA6bKjjyzhOZjZWME2rohvNoz6NcWJvhWdfnKVrvlfQWjKQKnjnQTJcQsGH8tV8o1q3lQ==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHNzCCBR+gAwIBAgIIfFghCRNtqPgwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDIwMFoXDTIyMDkxNDEzNDIwMFowgdwxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDEPMA0GA1UEBxMGR3VhaXJhMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTEwMC4GA1UEAxMnUk9ET1RBQyBUUkFOU1BPUlRFUyBMVERBOjA0NDAwMzI5MDAwMTA5MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAp04ol/u6OamuPQYiuYvmBoabm9447ej3qfCk6KQY+gVddtzabeHC4yK1n9UOseY/2g2Wz2OQuVjZBz1mLb5aKDW9Hx4Hg4JXosEhRgHv+FxtlrgGJps+vVSke1fDiRKB9RxkryP5ngl3fOTaDXyXKAVw5Xir/ireILJkxoa7yItj3qOoX3WXO0e8IBBjeOJ3PyllIvh06I3LHaeqr6+hWxwuNsSxdYVLl+x0J5A1p8O+9MWEgTL6zEuST5aIoeESpEKC/oiOZwHujV8Zp6Ld3tbV45cNmE5qyq0Cv6WMxvySvmtBwBIS/2ftmk8dMnZb+R+iiO4Gh5gEFQ36XU3ezQIDAQABo4ICfTCCAnkwHwYDVR0jBBgwFoAUP9NcqRlN14gWLZgMrwre4U8kFrAwWQYIKwYBBQUHAQEETTBLMEkGCCsGAQUFBzAChj1odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUucDdiMIGvBgNVHREEgacwgaSBFnJvZG90YWNAcm9kb3RhYy5uZXQuYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMOMDQ0MDAzMjkwMDAxMDmgOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBTmf74GOUuAKM5iWH+pal5k4kRQYDAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAKffeE7P7VJywGR4dL48Nfq75Oa0zAPHLV/DXwo/bs847MeSBdauzpEiZ5xsUssJS/n73euRm/aaQ0Ai0fTYDcl6DAj0Bpn0kE3N9MF0/rb/35Ion/zwbhfzLHSby6MuH+NXvZheexyZV+LdWMnTY875AhHqFTLMH/e7TML3AukZFVrZDZ/KyjVGNji6XTmOxg0qt3hiEapOR+ODEqZO6FiYYS/7DGu+akrOzT8eOTddbUUzx2eZ6PctqSV7TZXTYtkfrq9pZgcFMjKUxwtnaQ9iE1ZttFTcVqIOWxPFLc/5pxFRfaFL+/5dhRs777Fox5nHBE9GjaI2alR9fidF4BJ+4UkcEZ17NaS8tzGYuP3XjieSWQD5eEAaGDA4eS+0zpNP6Z30UFqc5gmfj8EZaRuxaAUe+egORdxErP3J7CBPFEei/t1V/+E56JKHe75TgM+hTb+gxKyVThQULKZQgv/OiXD0O+cRBNHx0wNyvr/Srh61E9os66kg37kgfNZnMwBZOG4QmUtjJA5ChzJ99yXk6hNKhWXZrB+WwlBa2X/b/cff2nKx9wnw0ii3xjIAnkcWs2koAw5QaLUpNlHBTdTDVTMYZsXP9fSGKeom+/QDE6tZ5EstYiopzB2LRCGIB/PAwuYJX5fbcyMQTiu0A/6OCjQ3Bk9dK6myCbqSXJDb&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211204400329000109570010000605431000605431&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-23T15:43:02-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214667787512&lt;/nProt&gt;&lt;digVal&gt;vzv0sCukuogBoZeqbccqOO1OzOw=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35211204400329000109570010000605821000605820-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211204400329000109570010000605821000605820-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211204400329000109570010000605821000605820"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00060582&lt;/cCT&gt;&lt;CFOP&gt;6932&lt;/CFOP&gt;&lt;natOp&gt;PR.SERV.TRANSP.INIC.FORA ESTAD&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;60582&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-28T10:13:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;0&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3517406&lt;/cMunEnv&gt;&lt;xMunEnv&gt;GUAIRA&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;1&lt;/tpServ&gt;&lt;cMunIni&gt;3166808&lt;/cMunIni&gt;&lt;xMunIni&gt;SERRA DO SALITRE&lt;/xMunIni&gt;&lt;UFIni&gt;MG&lt;/UFIni&gt;&lt;cMunFim&gt;3513504&lt;/cMunFim&gt;&lt;xMunFim&gt;CUBATAO&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma4&gt;&lt;toma&gt;4&lt;/toma&gt;&lt;CNPJ&gt;50505924000703&lt;/CNPJ&gt;&lt;IE&gt;0034911940042&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (F.UBE)&lt;/xFant&gt;&lt;enderToma&gt;&lt;xLgr&gt;FILOMENA CARTAFINA&lt;/xLgr&gt;&lt;nro&gt;22031&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044750&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderToma&gt;&lt;/toma4&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Subcontratacao&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;SSL&lt;/xOrig&gt;&lt;xDest&gt;CBT&lt;/xDest&gt;&lt;xRota&gt;SSLCBT&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SERRA DO SALITRE&lt;/origCalc&gt;&lt;destCalc&gt;CUBATAO&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 237,02;CT-e EMITIDO SOMENTE P/EFEITO DE COBRANCA, NAO INC.ICMS, CONF.INC I DO ART.205 DO RICMS/00 - SUBCONTRATADO POR TRANSMOB TRANSPORTE LTDA CNPJ:50.505.924/0007-03, N°8591 Referencia do Cliente : 1-8591-1;&lt;/xObs&gt;&lt;ObsCont xCampo="frotas"&gt;&lt;xTexto&gt;C0220&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_clientes"&gt;&lt;xTexto&gt;1-8591-1&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_tons"&gt;&lt;xTexto&gt;135.170000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;JOSE MALAGOGIM&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;084.770.188-39&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;DTE6867&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;DKU3317&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;04400329000109&lt;/CNPJ&gt;&lt;IE&gt;322079785116&lt;/IE&gt;&lt;xNome&gt;RODOTAC TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;RODOTAC (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOAO JORGE GARCIA LEAL&lt;/xLgr&gt;&lt;nro&gt;607&lt;/nro&gt;&lt;xBairro&gt;PARQUE INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3517406&lt;/cMun&gt;&lt;xMun&gt;GUAIRA&lt;/xMun&gt;&lt;CEP&gt;14790000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733302455&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;92660604017662&lt;/CNPJ&gt;&lt;IE&gt;2874585321020&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;xFant&gt;YARA BRASIL&lt;/xFant&gt;&lt;fone&gt;01938849300&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;FAZENDA SALITRE S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MARRUA&lt;/xBairro&gt;&lt;cMun&gt;3166808&lt;/cMun&gt;&lt;xMun&gt;SERRA DO SALITRE&lt;/xMun&gt;&lt;CEP&gt;38760000&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604017158&lt;/CNPJ&gt;&lt;IE&gt;283129851112&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;fone&gt;01333699194&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV ENGENHEIRO PLINIO DE QUEIROZ S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;ZONA INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;CUBATAO&lt;/xMun&gt;&lt;CEP&gt;11570000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;email&gt;LUCIANO.PINTO@YARA.COM&lt;/email&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;6493.57&lt;/vTPrest&gt;&lt;vRec&gt;6493.57&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;6114.67&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;378.90&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;237.02&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;60270.26&lt;/vCarga&gt;&lt;proPred&gt;ROCHA&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;48040.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;48.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;60270.26&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;31211292660604017662550500000171731944724056&lt;/chave&gt;&lt;dPrev&gt;2021-12-28&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;docAnt&gt;&lt;emiDocAnt&gt;&lt;CNPJ&gt;50505924000703&lt;/CNPJ&gt;&lt;IE&gt;0034911940042&lt;/IE&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;idDocAnt&gt;&lt;idDocAntEle&gt;&lt;chCTe&gt;31211250505924000703570010000085911000085914&lt;/chCTe&gt;&lt;/idDocAntEle&gt;&lt;/idDocAnt&gt;&lt;/emiDocAnt&gt;&lt;/docAnt&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;02625527&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211204400329000109570010000605821000605820&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211204400329000109570010000605821000605820"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;12P6hxsdH8saM20I5HXQbCC1e80=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;bKyRYaBXfJR9/I2wSdUYGBdq5Kf5Fijr5f2BqQ1fTWyaypCAU2cAk+ERoPfvzfbIPKt/n8jE46YZm1Udw6Hv2Rd/aqmYp+ZLwiBXUBZoHQ7+z7f9CzqzhV2U0lxGiq3DCD0vIjUpGzfgMX0ulKJS3I3RJiH3R7+L1dqwImrme1Mg7TNGcOl4PerbZTV6SmV6DIOh/DRaBiXmI2WDbe5baDK5Qj672t3uwGSR4psAInVMqd/HuZDQR7n2VFvutYtgVoCRxQ71CdXOwEaOA1wimucpakVTO/RZALHPZZD4x9CWm4IK1skH7VWIu+pAJQ5vD9ClggG8EZYDPS2qemY3rw==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHNzCCBR+gAwIBAgIIfFghCRNtqPgwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDIwMFoXDTIyMDkxNDEzNDIwMFowgdwxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDEPMA0GA1UEBxMGR3VhaXJhMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTEwMC4GA1UEAxMnUk9ET1RBQyBUUkFOU1BPUlRFUyBMVERBOjA0NDAwMzI5MDAwMTA5MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAp04ol/u6OamuPQYiuYvmBoabm9447ej3qfCk6KQY+gVddtzabeHC4yK1n9UOseY/2g2Wz2OQuVjZBz1mLb5aKDW9Hx4Hg4JXosEhRgHv+FxtlrgGJps+vVSke1fDiRKB9RxkryP5ngl3fOTaDXyXKAVw5Xir/ireILJkxoa7yItj3qOoX3WXO0e8IBBjeOJ3PyllIvh06I3LHaeqr6+hWxwuNsSxdYVLl+x0J5A1p8O+9MWEgTL6zEuST5aIoeESpEKC/oiOZwHujV8Zp6Ld3tbV45cNmE5qyq0Cv6WMxvySvmtBwBIS/2ftmk8dMnZb+R+iiO4Gh5gEFQ36XU3ezQIDAQABo4ICfTCCAnkwHwYDVR0jBBgwFoAUP9NcqRlN14gWLZgMrwre4U8kFrAwWQYIKwYBBQUHAQEETTBLMEkGCCsGAQUFBzAChj1odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUucDdiMIGvBgNVHREEgacwgaSBFnJvZG90YWNAcm9kb3RhYy5uZXQuYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMOMDQ0MDAzMjkwMDAxMDmgOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBTmf74GOUuAKM5iWH+pal5k4kRQYDAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAKffeE7P7VJywGR4dL48Nfq75Oa0zAPHLV/DXwo/bs847MeSBdauzpEiZ5xsUssJS/n73euRm/aaQ0Ai0fTYDcl6DAj0Bpn0kE3N9MF0/rb/35Ion/zwbhfzLHSby6MuH+NXvZheexyZV+LdWMnTY875AhHqFTLMH/e7TML3AukZFVrZDZ/KyjVGNji6XTmOxg0qt3hiEapOR+ODEqZO6FiYYS/7DGu+akrOzT8eOTddbUUzx2eZ6PctqSV7TZXTYtkfrq9pZgcFMjKUxwtnaQ9iE1ZttFTcVqIOWxPFLc/5pxFRfaFL+/5dhRs777Fox5nHBE9GjaI2alR9fidF4BJ+4UkcEZ17NaS8tzGYuP3XjieSWQD5eEAaGDA4eS+0zpNP6Z30UFqc5gmfj8EZaRuxaAUe+egORdxErP3J7CBPFEei/t1V/+E56JKHe75TgM+hTb+gxKyVThQULKZQgv/OiXD0O+cRBNHx0wNyvr/Srh61E9os66kg37kgfNZnMwBZOG4QmUtjJA5ChzJ99yXk6hNKhWXZrB+WwlBa2X/b/cff2nKx9wnw0ii3xjIAnkcWs2koAw5QaLUpNlHBTdTDVTMYZsXP9fSGKeom+/QDE6tZ5EstYiopzB2LRCGIB/PAwuYJX5fbcyMQTiu0A/6OCjQ3Bk9dK6myCbqSXJDb&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211204400329000109570010000605821000605820&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-28T10:20:29-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214679010526&lt;/nProt&gt;&lt;digVal&gt;12P6hxsdH8saM20I5HXQbCC1e80=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35211204400329000109570010000605931000605930-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211204400329000109570010000605931000605930-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211204400329000109570010000605931000605930"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00060593&lt;/cCT&gt;&lt;CFOP&gt;6360&lt;/CFOP&gt;&lt;natOp&gt;PREST. SERV.TRANSP. A CONT.SUBST. EM REL. AO SERVICO&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;60593&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-30T10:18:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;0&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3517406&lt;/cMunEnv&gt;&lt;xMunEnv&gt;GUAIRA&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;1&lt;/tpServ&gt;&lt;cMunIni&gt;3548500&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTOS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3104007&lt;/cMunFim&gt;&lt;xMunFim&gt;ARAXA&lt;/xMunFim&gt;&lt;UFFim&gt;MG&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma4&gt;&lt;toma&gt;4&lt;/toma&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB&lt;/xFant&gt;&lt;enderToma&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderToma&gt;&lt;/toma4&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Subcontratacao&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;STS&lt;/xOrig&gt;&lt;xDest&gt;ARX&lt;/xDest&gt;&lt;xRota&gt;STSARX&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTOS&lt;/origCalc&gt;&lt;destCalc&gt;ARAXA&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 168,92;CT-e EMITIDO SOMENTE P/EFEITO DE COBRANCA, NAO INC.ICMS, CONF.INC I DO ART.205 DO RICMS/00 - SUBCONTRATADO POR TRANSMOB TRANSPORTE LTDA CNPJ:50.505.924/0001-18, N°283322 Referencia do Cliente : 1-283322-1;&lt;/xObs&gt;&lt;ObsCont xCampo="frotas"&gt;&lt;xTexto&gt;C0260&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_clientes"&gt;&lt;xTexto&gt;1-283322-1&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_tons"&gt;&lt;xTexto&gt;185.860000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;WILSON APARECIDO DOS SANTOS&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;077.771.038-22&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;GHL1A73&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FFK5B74&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FMJ8I56&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FPE-8F35&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;04400329000109&lt;/CNPJ&gt;&lt;IE&gt;322079785116&lt;/IE&gt;&lt;xNome&gt;RODOTAC TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;RODOTAC (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOAO JORGE GARCIA LEAL&lt;/xLgr&gt;&lt;nro&gt;607&lt;/nro&gt;&lt;xBairro&gt;PARQUE INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3517406&lt;/cMun&gt;&lt;xMun&gt;GUAIRA&lt;/xMun&gt;&lt;CEP&gt;14790000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733302455&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;00000000000000&lt;/CNPJ&gt;&lt;IE&gt;ISENTO&lt;/IE&gt;&lt;xNome&gt;CANPOTEX LIMITED&lt;/xNome&gt;&lt;xFant&gt;CANPOTEX (COSTADO)&lt;/xFant&gt;&lt;fone&gt;01734445550&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AAAAAA&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;EXTERIOR&lt;/xBairro&gt;&lt;cMun&gt;9999999&lt;/cMun&gt;&lt;xMun&gt;EXTERIOR&lt;/xMun&gt;&lt;CEP&gt;00000000&lt;/CEP&gt;&lt;UF&gt;EX&lt;/UF&gt;&lt;cPais&gt;1490&lt;/cPais&gt;&lt;xPais&gt;CANADA&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;exped&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;xNome&gt;COMPANHIA DOCAS DO ESTADO DE SAO PAULO CODESP&lt;/xNome&gt;&lt;fone&gt;01300000000&lt;/fone&gt;&lt;enderExped&gt;&lt;xLgr&gt;CONSELHEIRO RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;CEP&gt;11015900&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderExped&gt;&lt;/exped&gt;&lt;dest&gt;&lt;CNPJ&gt;88305859001555&lt;/CNPJ&gt;&lt;IE&gt;0027743880010&lt;/IE&gt;&lt;xNome&gt;NUTRIEN AG SOLUTIONS IND E COM PROD AGRI LTDA&lt;/xNome&gt;&lt;fone&gt;01532758780&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;ROD - MG 146 S/N FAZENDA PAO DE ACUCAR&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;ZONA RURAL&lt;/xBairro&gt;&lt;cMun&gt;3104007&lt;/cMun&gt;&lt;xMun&gt;ARAXA&lt;/xMun&gt;&lt;CEP&gt;38183000&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;4627.91&lt;/vTPrest&gt;&lt;vRec&gt;4627.91&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;3760.31&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;867.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;168.92&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;99181.68&lt;/vCarga&gt;&lt;proPred&gt;CLORETO DE POTASSIO 60% K20 GR&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;24900.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;25.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;99181.68&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;31211288305859001555550920000006441365062542&lt;/chave&gt;&lt;dPrev&gt;2021-12-30&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;docAnt&gt;&lt;emiDocAnt&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;idDocAnt&gt;&lt;idDocAntEle&gt;&lt;chCTe&gt;35211250505924000118570010002833221002833221&lt;/chCTe&gt;&lt;/idDocAntEle&gt;&lt;/idDocAnt&gt;&lt;/emiDocAnt&gt;&lt;/docAnt&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;02625527&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211204400329000109570010000605931000605930&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211204400329000109570010000605931000605930"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;2sUJ92204dl7Gih3mkVzeWwa4NE=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;ik1p7qvK/6xEo3qafpzj9oNI3tOXI66DjZbDMG0Os9TJ7X6zJv/MQM5Z7gW1e9yZlm818yCPC3xlJ6arMD990mal2DnZsWqw89wJKQDzaHn5wD/hweaBY0IpBKHt5MUQNsB4hAEQOLenuakCXi+Djwk9NOVLs1tY6DQz97bBdYUdqAoQ83NZ953hTAeulnJqUsNj+pCqP3UPoYPwfCI3oUQyeJdkV729MX0aL+saxkNATpqInLd/SQB64lsUeHieU8rYyTW5aguZN64kUQ3czOnNaZYwUdn4s/cke+040uzntbcD5PdAL/8YmytYZLrbdAEcyD1dvlmHFJpaLEfJIg==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHNzCCBR+gAwIBAgIIfFghCRNtqPgwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDIwMFoXDTIyMDkxNDEzNDIwMFowgdwxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDEPMA0GA1UEBxMGR3VhaXJhMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTEwMC4GA1UEAxMnUk9ET1RBQyBUUkFOU1BPUlRFUyBMVERBOjA0NDAwMzI5MDAwMTA5MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAp04ol/u6OamuPQYiuYvmBoabm9447ej3qfCk6KQY+gVddtzabeHC4yK1n9UOseY/2g2Wz2OQuVjZBz1mLb5aKDW9Hx4Hg4JXosEhRgHv+FxtlrgGJps+vVSke1fDiRKB9RxkryP5ngl3fOTaDXyXKAVw5Xir/ireILJkxoa7yItj3qOoX3WXO0e8IBBjeOJ3PyllIvh06I3LHaeqr6+hWxwuNsSxdYVLl+x0J5A1p8O+9MWEgTL6zEuST5aIoeESpEKC/oiOZwHujV8Zp6Ld3tbV45cNmE5qyq0Cv6WMxvySvmtBwBIS/2ftmk8dMnZb+R+iiO4Gh5gEFQ36XU3ezQIDAQABo4ICfTCCAnkwHwYDVR0jBBgwFoAUP9NcqRlN14gWLZgMrwre4U8kFrAwWQYIKwYBBQUHAQEETTBLMEkGCCsGAQUFBzAChj1odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUucDdiMIGvBgNVHREEgacwgaSBFnJvZG90YWNAcm9kb3RhYy5uZXQuYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMOMDQ0MDAzMjkwMDAxMDmgOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBTmf74GOUuAKM5iWH+pal5k4kRQYDAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAKffeE7P7VJywGR4dL48Nfq75Oa0zAPHLV/DXwo/bs847MeSBdauzpEiZ5xsUssJS/n73euRm/aaQ0Ai0fTYDcl6DAj0Bpn0kE3N9MF0/rb/35Ion/zwbhfzLHSby6MuH+NXvZheexyZV+LdWMnTY875AhHqFTLMH/e7TML3AukZFVrZDZ/KyjVGNji6XTmOxg0qt3hiEapOR+ODEqZO6FiYYS/7DGu+akrOzT8eOTddbUUzx2eZ6PctqSV7TZXTYtkfrq9pZgcFMjKUxwtnaQ9iE1ZttFTcVqIOWxPFLc/5pxFRfaFL+/5dhRs777Fox5nHBE9GjaI2alR9fidF4BJ+4UkcEZ17NaS8tzGYuP3XjieSWQD5eEAaGDA4eS+0zpNP6Z30UFqc5gmfj8EZaRuxaAUe+egORdxErP3J7CBPFEei/t1V/+E56JKHe75TgM+hTb+gxKyVThQULKZQgv/OiXD0O+cRBNHx0wNyvr/Srh61E9os66kg37kgfNZnMwBZOG4QmUtjJA5ChzJ99yXk6hNKhWXZrB+WwlBa2X/b/cff2nKx9wnw0ii3xjIAnkcWs2koAw5QaLUpNlHBTdTDVTMYZsXP9fSGKeom+/QDE6tZ5EstYiopzB2LRCGIB/PAwuYJX5fbcyMQTiu0A/6OCjQ3Bk9dK6myCbqSXJDb&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211204400329000109570010000605931000605930&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-30T10:33:45-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214687644753&lt;/nProt&gt;&lt;digVal&gt;2sUJ92204dl7Gih3mkVzeWwa4NE=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35211204400329000109570010000605941000605945-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211204400329000109570010000605941000605945-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211204400329000109570010000605941000605945"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00060594&lt;/cCT&gt;&lt;CFOP&gt;6360&lt;/CFOP&gt;&lt;natOp&gt;PREST. SERV.TRANSP. A CONT.SUBST. EM REL. AO SERVICO&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;60594&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-30T10:18:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;5&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3517406&lt;/cMunEnv&gt;&lt;xMunEnv&gt;GUAIRA&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;1&lt;/tpServ&gt;&lt;cMunIni&gt;3548500&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTOS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3170107&lt;/cMunFim&gt;&lt;xMunFim&gt;UBERABA&lt;/xMunFim&gt;&lt;UFFim&gt;MG&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma4&gt;&lt;toma&gt;4&lt;/toma&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB&lt;/xFant&gt;&lt;enderToma&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderToma&gt;&lt;/toma4&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Subcontratacao&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;STS&lt;/xOrig&gt;&lt;xDest&gt;UBR&lt;/xDest&gt;&lt;xRota&gt;STSUBR&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTOS&lt;/origCalc&gt;&lt;destCalc&gt;UBERABA&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 175,10;CT-e EMITIDO SOMENTE P/EFEITO DE COBRANCA, NAO INC.ICMS, CONF.INC I DO ART.205 DO RICMS/00 - SUBCONTRATADO POR TRANSMOB TRANSPORTE LTDA CNPJ:50.505.924/0001-18, N°283325 Referencia do Cliente : 1-283325-1;&lt;/xObs&gt;&lt;ObsCont xCampo="frotas"&gt;&lt;xTexto&gt;C0220&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_clientes"&gt;&lt;xTexto&gt;1-283325-1&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_tons"&gt;&lt;xTexto&gt;177.410000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;JOSE MALAGOGIM&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;084.770.188-39&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;DTE6867&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;DKU3317&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;EXN9979&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;BVT-9908&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;04400329000109&lt;/CNPJ&gt;&lt;IE&gt;322079785116&lt;/IE&gt;&lt;xNome&gt;RODOTAC TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;RODOTAC (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOAO JORGE GARCIA LEAL&lt;/xLgr&gt;&lt;nro&gt;607&lt;/nro&gt;&lt;xBairro&gt;PARQUE INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3517406&lt;/cMun&gt;&lt;xMun&gt;GUAIRA&lt;/xMun&gt;&lt;CEP&gt;14790000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733302455&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;00000000000000&lt;/CNPJ&gt;&lt;IE&gt;ISENTO&lt;/IE&gt;&lt;xNome&gt;YARA SWITZERLAND LTD.&lt;/xNome&gt;&lt;xFant&gt;YARA CAIS COMERCIAL&lt;/xFant&gt;&lt;fone&gt;00000000000&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AAAAAAA&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;AAAAA&lt;/xBairro&gt;&lt;cMun&gt;9999999&lt;/cMun&gt;&lt;xMun&gt;EXTERIOR&lt;/xMun&gt;&lt;CEP&gt;00000000&lt;/CEP&gt;&lt;UF&gt;EX&lt;/UF&gt;&lt;cPais&gt;7676&lt;/cPais&gt;&lt;xPais&gt;SUICA&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;exped&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;xNome&gt;COMPANHIA DOCAS DO ESTADO DE SAO PAULO CODESP&lt;/xNome&gt;&lt;fone&gt;01300000000&lt;/fone&gt;&lt;enderExped&gt;&lt;xLgr&gt;CONSELHEIRO RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;CEP&gt;11015900&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderExped&gt;&lt;/exped&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604015457&lt;/CNPJ&gt;&lt;IE&gt;3714585320678&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;fone&gt;03433197198&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV ANTONIO CARLOS GUILLAUMON&lt;/xLgr&gt;&lt;nro&gt;800&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044760&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;4797.17&lt;/vTPrest&gt;&lt;vRec&gt;4797.17&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;3929.57&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;867.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;175.10&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;91128.04&lt;/vCarga&gt;&lt;proPred&gt;16 16 16 YM UNIK 16 GRANULADO&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;27040.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;27.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;91128.04&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;31211292660604015457550760000200271085528499&lt;/chave&gt;&lt;dPrev&gt;2021-12-31&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;docAnt&gt;&lt;emiDocAnt&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;idDocAnt&gt;&lt;idDocAntEle&gt;&lt;chCTe&gt;35211250505924000118570010002833251002833258&lt;/chCTe&gt;&lt;/idDocAntEle&gt;&lt;/idDocAnt&gt;&lt;/emiDocAnt&gt;&lt;/docAnt&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;02625527&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211204400329000109570010000605941000605945&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211204400329000109570010000605941000605945"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;JNoNmdeZA5/CwjX26FEypTlCgeA=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;dh3DRDpp056bhSBjQbcUhtASRpktPiKddduhAHvP0RZvDibdzrBZiqP0jNYdX8bgDxP6aZKsWgLJqwxIUMeEEmhrVHgKf9Ph9Gt/PfbTHUgaG3PVQ1ZPtVxkrO4nAndtOtd1ZX43FU+7DQPopbw6m0Y2YmzSqT0EbyJI3VklzXzymz5bZ/ixii71Z47ShBoTNN8FmvuoLPl6qebO9SHu+MB8WotWw739ynhJcI3pW03dzESs2locv7e3LoGumcK+oZhuC+uGxhq5Rhy5P3lhgEQ6CrT908fsBTBa85oUhIuBxupITCXNr8HN67KFSKNoueazVsSQyj17BNA1edu4lQ==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHNzCCBR+gAwIBAgIIfFghCRNtqPgwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDIwMFoXDTIyMDkxNDEzNDIwMFowgdwxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDEPMA0GA1UEBxMGR3VhaXJhMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTEwMC4GA1UEAxMnUk9ET1RBQyBUUkFOU1BPUlRFUyBMVERBOjA0NDAwMzI5MDAwMTA5MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAp04ol/u6OamuPQYiuYvmBoabm9447ej3qfCk6KQY+gVddtzabeHC4yK1n9UOseY/2g2Wz2OQuVjZBz1mLb5aKDW9Hx4Hg4JXosEhRgHv+FxtlrgGJps+vVSke1fDiRKB9RxkryP5ngl3fOTaDXyXKAVw5Xir/ireILJkxoa7yItj3qOoX3WXO0e8IBBjeOJ3PyllIvh06I3LHaeqr6+hWxwuNsSxdYVLl+x0J5A1p8O+9MWEgTL6zEuST5aIoeESpEKC/oiOZwHujV8Zp6Ld3tbV45cNmE5qyq0Cv6WMxvySvmtBwBIS/2ftmk8dMnZb+R+iiO4Gh5gEFQ36XU3ezQIDAQABo4ICfTCCAnkwHwYDVR0jBBgwFoAUP9NcqRlN14gWLZgMrwre4U8kFrAwWQYIKwYBBQUHAQEETTBLMEkGCCsGAQUFBzAChj1odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUucDdiMIGvBgNVHREEgacwgaSBFnJvZG90YWNAcm9kb3RhYy5uZXQuYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMOMDQ0MDAzMjkwMDAxMDmgOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBTmf74GOUuAKM5iWH+pal5k4kRQYDAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAKffeE7P7VJywGR4dL48Nfq75Oa0zAPHLV/DXwo/bs847MeSBdauzpEiZ5xsUssJS/n73euRm/aaQ0Ai0fTYDcl6DAj0Bpn0kE3N9MF0/rb/35Ion/zwbhfzLHSby6MuH+NXvZheexyZV+LdWMnTY875AhHqFTLMH/e7TML3AukZFVrZDZ/KyjVGNji6XTmOxg0qt3hiEapOR+ODEqZO6FiYYS/7DGu+akrOzT8eOTddbUUzx2eZ6PctqSV7TZXTYtkfrq9pZgcFMjKUxwtnaQ9iE1ZttFTcVqIOWxPFLc/5pxFRfaFL+/5dhRs777Fox5nHBE9GjaI2alR9fidF4BJ+4UkcEZ17NaS8tzGYuP3XjieSWQD5eEAaGDA4eS+0zpNP6Z30UFqc5gmfj8EZaRuxaAUe+egORdxErP3J7CBPFEei/t1V/+E56JKHe75TgM+hTb+gxKyVThQULKZQgv/OiXD0O+cRBNHx0wNyvr/Srh61E9os66kg37kgfNZnMwBZOG4QmUtjJA5ChzJ99yXk6hNKhWXZrB+WwlBa2X/b/cff2nKx9wnw0ii3xjIAnkcWs2koAw5QaLUpNlHBTdTDVTMYZsXP9fSGKeom+/QDE6tZ5EstYiopzB2LRCGIB/PAwuYJX5fbcyMQTiu0A/6OCjQ3Bk9dK6myCbqSXJDb&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211204400329000109570010000605941000605945&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-30T10:33:47-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214687645029&lt;/nProt&gt;&lt;digVal&gt;JNoNmdeZA5/CwjX26FEypTlCgeA=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35211204400329000109570010000605951000605950-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211204400329000109570010000605951000605950-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211204400329000109570010000605951000605950"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00060595&lt;/cCT&gt;&lt;CFOP&gt;6360&lt;/CFOP&gt;&lt;natOp&gt;PREST. SERV.TRANSP. A CONT.SUBST. EM REL. AO SERVICO&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;60595&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-30T10:18:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;0&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3517406&lt;/cMunEnv&gt;&lt;xMunEnv&gt;GUAIRA&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;1&lt;/tpServ&gt;&lt;cMunIni&gt;3548500&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTOS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3170107&lt;/cMunFim&gt;&lt;xMunFim&gt;UBERABA&lt;/xMunFim&gt;&lt;UFFim&gt;MG&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma4&gt;&lt;toma&gt;4&lt;/toma&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB&lt;/xFant&gt;&lt;enderToma&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderToma&gt;&lt;/toma4&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Subcontratacao&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;STS&lt;/xOrig&gt;&lt;xDest&gt;UBR&lt;/xDest&gt;&lt;xRota&gt;STSUBR&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTOS&lt;/origCalc&gt;&lt;destCalc&gt;UBERABA&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 134,82;CT-e EMITIDO SOMENTE P/EFEITO DE COBRANCA, NAO INC.ICMS, CONF.INC I DO ART.205 DO RICMS/00 - SUBCONTRATADO POR TRANSMOB TRANSPORTE LTDA CNPJ:50.505.924/0001-18, N°283326 Referencia do Cliente : 1-283326-1;&lt;/xObs&gt;&lt;ObsCont xCampo="frotas"&gt;&lt;xTexto&gt;C0220&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_clientes"&gt;&lt;xTexto&gt;1-283326-1&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_tons"&gt;&lt;xTexto&gt;177.410000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;JOSE MALAGOGIM&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;084.770.188-39&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;DTE6867&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;DKU3317&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;EXN9979&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;BVT-9908&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;04400329000109&lt;/CNPJ&gt;&lt;IE&gt;322079785116&lt;/IE&gt;&lt;xNome&gt;RODOTAC TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;RODOTAC (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOAO JORGE GARCIA LEAL&lt;/xLgr&gt;&lt;nro&gt;607&lt;/nro&gt;&lt;xBairro&gt;PARQUE INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3517406&lt;/cMun&gt;&lt;xMun&gt;GUAIRA&lt;/xMun&gt;&lt;CEP&gt;14790000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733302455&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;00000000000000&lt;/CNPJ&gt;&lt;IE&gt;ISENTO&lt;/IE&gt;&lt;xNome&gt;YARA SWITZERLAND LTD.&lt;/xNome&gt;&lt;xFant&gt;YARA CAIS COMERCIAL&lt;/xFant&gt;&lt;fone&gt;00000000000&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AAAAAAA&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;AAAAA&lt;/xBairro&gt;&lt;cMun&gt;9999999&lt;/cMun&gt;&lt;xMun&gt;EXTERIOR&lt;/xMun&gt;&lt;CEP&gt;00000000&lt;/CEP&gt;&lt;UF&gt;EX&lt;/UF&gt;&lt;cPais&gt;7676&lt;/cPais&gt;&lt;xPais&gt;SUICA&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;exped&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;xNome&gt;COMPANHIA DOCAS DO ESTADO DE SAO PAULO CODESP&lt;/xNome&gt;&lt;fone&gt;01300000000&lt;/fone&gt;&lt;enderExped&gt;&lt;xLgr&gt;CONSELHEIRO RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;CEP&gt;11015900&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderExped&gt;&lt;/exped&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604015457&lt;/CNPJ&gt;&lt;IE&gt;3714585320678&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;fone&gt;03433197198&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV ANTONIO CARLOS GUILLAUMON&lt;/xLgr&gt;&lt;nro&gt;800&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044760&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;3693.68&lt;/vTPrest&gt;&lt;vRec&gt;3693.68&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;2826.08&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;867.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;134.82&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;70165.90&lt;/vCarga&gt;&lt;proPred&gt;16 16 16 YM UNIK 16 GRANULADO&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;20820.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;21.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;70165.90&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;31211292660604015457550760000200281302910709&lt;/chave&gt;&lt;dPrev&gt;2021-12-31&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;docAnt&gt;&lt;emiDocAnt&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;idDocAnt&gt;&lt;idDocAntEle&gt;&lt;chCTe&gt;35211250505924000118570010002833261002833263&lt;/chCTe&gt;&lt;/idDocAntEle&gt;&lt;/idDocAnt&gt;&lt;/emiDocAnt&gt;&lt;/docAnt&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;02625527&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211204400329000109570010000605951000605950&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211204400329000109570010000605951000605950"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;6fov4jw6RicHgkWjllzPXwudjkU=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;R91MTAE8FCsCMKpKCfLyPCxAur6WmK/91aW1LUpU3//rUwZuTquqD1YByMI4P7taxv1BsYhO6oTBW+3d43OZWnt7ZYxPpq/YtrsQCITSXwqkPYD4pbZibHuVSfrZwPLJu360SSQAEv/ciH6r7FTFx6bi6FdzCU/zPJvnxsIy1WUhFouS5Sk8gpCKZuOvW7J/lXquvnNYXZRPh6Jto6akM8wCJoRQw5mk+kVuqqj9AK5cZ2t+axwq6i83zo/vEUUD50ATMZy4JGsEWnXRGYzfPmN6GMs2PB8qucmHQADOrF2GhS9h06grLfs8bIv8Ijnwi5ovVc4amuIbIz4gGV7BAw==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHNzCCBR+gAwIBAgIIfFghCRNtqPgwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDIwMFoXDTIyMDkxNDEzNDIwMFowgdwxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDEPMA0GA1UEBxMGR3VhaXJhMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTEwMC4GA1UEAxMnUk9ET1RBQyBUUkFOU1BPUlRFUyBMVERBOjA0NDAwMzI5MDAwMTA5MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAp04ol/u6OamuPQYiuYvmBoabm9447ej3qfCk6KQY+gVddtzabeHC4yK1n9UOseY/2g2Wz2OQuVjZBz1mLb5aKDW9Hx4Hg4JXosEhRgHv+FxtlrgGJps+vVSke1fDiRKB9RxkryP5ngl3fOTaDXyXKAVw5Xir/ireILJkxoa7yItj3qOoX3WXO0e8IBBjeOJ3PyllIvh06I3LHaeqr6+hWxwuNsSxdYVLl+x0J5A1p8O+9MWEgTL6zEuST5aIoeESpEKC/oiOZwHujV8Zp6Ld3tbV45cNmE5qyq0Cv6WMxvySvmtBwBIS/2ftmk8dMnZb+R+iiO4Gh5gEFQ36XU3ezQIDAQABo4ICfTCCAnkwHwYDVR0jBBgwFoAUP9NcqRlN14gWLZgMrwre4U8kFrAwWQYIKwYBBQUHAQEETTBLMEkGCCsGAQUFBzAChj1odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUucDdiMIGvBgNVHREEgacwgaSBFnJvZG90YWNAcm9kb3RhYy5uZXQuYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMOMDQ0MDAzMjkwMDAxMDmgOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBTmf74GOUuAKM5iWH+pal5k4kRQYDAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAKffeE7P7VJywGR4dL48Nfq75Oa0zAPHLV/DXwo/bs847MeSBdauzpEiZ5xsUssJS/n73euRm/aaQ0Ai0fTYDcl6DAj0Bpn0kE3N9MF0/rb/35Ion/zwbhfzLHSby6MuH+NXvZheexyZV+LdWMnTY875AhHqFTLMH/e7TML3AukZFVrZDZ/KyjVGNji6XTmOxg0qt3hiEapOR+ODEqZO6FiYYS/7DGu+akrOzT8eOTddbUUzx2eZ6PctqSV7TZXTYtkfrq9pZgcFMjKUxwtnaQ9iE1ZttFTcVqIOWxPFLc/5pxFRfaFL+/5dhRs777Fox5nHBE9GjaI2alR9fidF4BJ+4UkcEZ17NaS8tzGYuP3XjieSWQD5eEAaGDA4eS+0zpNP6Z30UFqc5gmfj8EZaRuxaAUe+egORdxErP3J7CBPFEei/t1V/+E56JKHe75TgM+hTb+gxKyVThQULKZQgv/OiXD0O+cRBNHx0wNyvr/Srh61E9os66kg37kgfNZnMwBZOG4QmUtjJA5ChzJ99yXk6hNKhWXZrB+WwlBa2X/b/cff2nKx9wnw0ii3xjIAnkcWs2koAw5QaLUpNlHBTdTDVTMYZsXP9fSGKeom+/QDE6tZ5EstYiopzB2LRCGIB/PAwuYJX5fbcyMQTiu0A/6OCjQ3Bk9dK6myCbqSXJDb&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211204400329000109570010000605951000605950&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-30T10:33:49-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214687645105&lt;/nProt&gt;&lt;digVal&gt;6fov4jw6RicHgkWjllzPXwudjkU=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35211204400329000109570010000605961000605966-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211204400329000109570010000605961000605966-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211204400329000109570010000605961000605966"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00060596&lt;/cCT&gt;&lt;CFOP&gt;6360&lt;/CFOP&gt;&lt;natOp&gt;PREST. SERV.TRANSP. A CONT.SUBST. EM REL. AO SERVICO&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;60596&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-30T10:18:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;6&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3517406&lt;/cMunEnv&gt;&lt;xMunEnv&gt;GUAIRA&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;1&lt;/tpServ&gt;&lt;cMunIni&gt;3513504&lt;/cMunIni&gt;&lt;xMunIni&gt;CUBATAO&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3170107&lt;/cMunFim&gt;&lt;xMunFim&gt;UBERABA&lt;/xMunFim&gt;&lt;UFFim&gt;MG&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma4&gt;&lt;toma&gt;4&lt;/toma&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB&lt;/xFant&gt;&lt;enderToma&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderToma&gt;&lt;/toma4&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Subcontratacao&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;CBT&lt;/xOrig&gt;&lt;xDest&gt;UBR&lt;/xDest&gt;&lt;xRota&gt;CBTUBR&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;CUBATAO&lt;/origCalc&gt;&lt;destCalc&gt;UBERABA&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 210,86;CT-e EMITIDO SOMENTE P/EFEITO DE COBRANCA, NAO INC.ICMS, CONF.INC I DO ART.205 DO RICMS/00 - SUBCONTRATADO POR TRANSMOB TRANSPORTE LTDA CNPJ:50.505.924/0001-18, N°283342 Referencia do Cliente : 1-283342-1;&lt;/xObs&gt;&lt;ObsCont xCampo="frotas"&gt;&lt;xTexto&gt;C0270&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_clientes"&gt;&lt;xTexto&gt;1-283342-1&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_tons"&gt;&lt;xTexto&gt;122.500000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;RAFAEL RIBEIRO RODRIGUES&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;336.420.228-12&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;FAI5F78&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;EKH2723&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;EKH2724&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;EKH-2722&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;04400329000109&lt;/CNPJ&gt;&lt;IE&gt;322079785116&lt;/IE&gt;&lt;xNome&gt;RODOTAC TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;RODOTAC (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOAO JORGE GARCIA LEAL&lt;/xLgr&gt;&lt;nro&gt;607&lt;/nro&gt;&lt;xBairro&gt;PARQUE INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3517406&lt;/cMun&gt;&lt;xMun&gt;GUAIRA&lt;/xMun&gt;&lt;CEP&gt;14790000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733302455&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;06225292000147&lt;/CNPJ&gt;&lt;IE&gt;283108491118&lt;/IE&gt;&lt;xNome&gt;TERLOC - TERMINAL LOGISTICO CESARI LTDA&lt;/xNome&gt;&lt;xFant&gt;TERLOC- TER. CESARI.&lt;/xFant&gt;&lt;fone&gt;01321028013&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AV ENGENHEIRO PLINIO DE QUEIROZ S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xCpl&gt;SP 55&lt;/xCpl&gt;&lt;xBairro&gt;PIACAGUERA&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;CUBATAO&lt;/xMun&gt;&lt;CEP&gt;11570000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604015457&lt;/CNPJ&gt;&lt;IE&gt;3714585320678&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;fone&gt;03433197198&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV ANTONIO CARLOS GUILLAUMON&lt;/xLgr&gt;&lt;nro&gt;800&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044760&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;5777.10&lt;/vTPrest&gt;&lt;vRec&gt;5777.10&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;4909.50&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;867.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;210.86&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;158934.86&lt;/vCarga&gt;&lt;proPred&gt;16 16 16 YM UNIK 16 GRANULADO&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;47160.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;1.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;158934.86&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35211206225292000147550010006131931012667061&lt;/chave&gt;&lt;dPrev&gt;2021-12-31&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;docAnt&gt;&lt;emiDocAnt&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;idDocAnt&gt;&lt;idDocAntEle&gt;&lt;chCTe&gt;35211250505924000118570010002833421002833429&lt;/chCTe&gt;&lt;/idDocAntEle&gt;&lt;/idDocAnt&gt;&lt;/emiDocAnt&gt;&lt;/docAnt&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;02625527&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211204400329000109570010000605961000605966&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211204400329000109570010000605961000605966"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;Cv8SGXRnv3HGiYbo9+nHpnIfgpQ=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;XD38d2dk0YbkapI+nHFftkeLlYY6EURRQDnpU5FeC9OcLIjYbcCD5jxKCV38J+3WmIguFtt97NSNIoDc4jBm1+6s3gWGxKEI/uv2PC/+vJWRXMEIXQenKBT8CYV7HeyPapAQBSEzD+PlMUf4+uCvBDEE0XK43AOqphNwS3a81TzEGqd+IxyEAWUaAF2a8vOOuv+VQUj3TOQLaq5D+FHFhOTHWkDYU6ZqP8zWjIvHkYvnottsOpCnI7kijdscyGJhhgUfhU6Gj+ZH/KyDq0skzhDtxzza2qIu4vghR2mLwd0XQYSX4b0ETNTtyZ4oiqg/NL+tJ7p2SF5puefCs0MzBw==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHNzCCBR+gAwIBAgIIfFghCRNtqPgwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDIwMFoXDTIyMDkxNDEzNDIwMFowgdwxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDEPMA0GA1UEBxMGR3VhaXJhMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTEwMC4GA1UEAxMnUk9ET1RBQyBUUkFOU1BPUlRFUyBMVERBOjA0NDAwMzI5MDAwMTA5MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAp04ol/u6OamuPQYiuYvmBoabm9447ej3qfCk6KQY+gVddtzabeHC4yK1n9UOseY/2g2Wz2OQuVjZBz1mLb5aKDW9Hx4Hg4JXosEhRgHv+FxtlrgGJps+vVSke1fDiRKB9RxkryP5ngl3fOTaDXyXKAVw5Xir/ireILJkxoa7yItj3qOoX3WXO0e8IBBjeOJ3PyllIvh06I3LHaeqr6+hWxwuNsSxdYVLl+x0J5A1p8O+9MWEgTL6zEuST5aIoeESpEKC/oiOZwHujV8Zp6Ld3tbV45cNmE5qyq0Cv6WMxvySvmtBwBIS/2ftmk8dMnZb+R+iiO4Gh5gEFQ36XU3ezQIDAQABo4ICfTCCAnkwHwYDVR0jBBgwFoAUP9NcqRlN14gWLZgMrwre4U8kFrAwWQYIKwYBBQUHAQEETTBLMEkGCCsGAQUFBzAChj1odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUucDdiMIGvBgNVHREEgacwgaSBFnJvZG90YWNAcm9kb3RhYy5uZXQuYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMOMDQ0MDAzMjkwMDAxMDmgOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBTmf74GOUuAKM5iWH+pal5k4kRQYDAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAKffeE7P7VJywGR4dL48Nfq75Oa0zAPHLV/DXwo/bs847MeSBdauzpEiZ5xsUssJS/n73euRm/aaQ0Ai0fTYDcl6DAj0Bpn0kE3N9MF0/rb/35Ion/zwbhfzLHSby6MuH+NXvZheexyZV+LdWMnTY875AhHqFTLMH/e7TML3AukZFVrZDZ/KyjVGNji6XTmOxg0qt3hiEapOR+ODEqZO6FiYYS/7DGu+akrOzT8eOTddbUUzx2eZ6PctqSV7TZXTYtkfrq9pZgcFMjKUxwtnaQ9iE1ZttFTcVqIOWxPFLc/5pxFRfaFL+/5dhRs777Fox5nHBE9GjaI2alR9fidF4BJ+4UkcEZ17NaS8tzGYuP3XjieSWQD5eEAaGDA4eS+0zpNP6Z30UFqc5gmfj8EZaRuxaAUe+egORdxErP3J7CBPFEei/t1V/+E56JKHe75TgM+hTb+gxKyVThQULKZQgv/OiXD0O+cRBNHx0wNyvr/Srh61E9os66kg37kgfNZnMwBZOG4QmUtjJA5ChzJ99yXk6hNKhWXZrB+WwlBa2X/b/cff2nKx9wnw0ii3xjIAnkcWs2koAw5QaLUpNlHBTdTDVTMYZsXP9fSGKeom+/QDE6tZ5EstYiopzB2LRCGIB/PAwuYJX5fbcyMQTiu0A/6OCjQ3Bk9dK6myCbqSXJDb&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211204400329000109570010000605961000605966&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-30T10:33:50-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214687645129&lt;/nProt&gt;&lt;digVal&gt;Cv8SGXRnv3HGiYbo9+nHpnIfgpQ=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35211204400329000109570010000605971000605971-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211204400329000109570010000605971000605971-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211204400329000109570010000605971000605971"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00060597&lt;/cCT&gt;&lt;CFOP&gt;6360&lt;/CFOP&gt;&lt;natOp&gt;PREST. SERV.TRANSP. A CONT.SUBST. EM REL. AO SERVICO&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;60597&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-30T10:18:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;1&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3517406&lt;/cMunEnv&gt;&lt;xMunEnv&gt;GUAIRA&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;1&lt;/tpServ&gt;&lt;cMunIni&gt;3513504&lt;/cMunIni&gt;&lt;xMunIni&gt;CUBATAO&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3170107&lt;/cMunFim&gt;&lt;xMunFim&gt;UBERABA&lt;/xMunFim&gt;&lt;UFFim&gt;MG&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma4&gt;&lt;toma&gt;4&lt;/toma&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB&lt;/xFant&gt;&lt;enderToma&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderToma&gt;&lt;/toma4&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Subcontratacao&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;CBT&lt;/xOrig&gt;&lt;xDest&gt;UBR&lt;/xDest&gt;&lt;xRota&gt;CBTUBR&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;CUBATAO&lt;/origCalc&gt;&lt;destCalc&gt;UBERABA&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 210,37;CT-e EMITIDO SOMENTE P/EFEITO DE COBRANCA, NAO INC.ICMS, CONF.INC I DO ART.205 DO RICMS/00 - SUBCONTRATADO POR TRANSMOB TRANSPORTE LTDA CNPJ:50.505.924/0001-18, N°283346 Referencia do Cliente : 1-283346-1;&lt;/xObs&gt;&lt;ObsCont xCampo="frotas"&gt;&lt;xTexto&gt;C0210&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_clientes"&gt;&lt;xTexto&gt;1-283346-1&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_tons"&gt;&lt;xTexto&gt;122.500000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;ALEX HENRIQUE DO NASCIMENTO&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;307.951.808-02&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;FOB3119&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;GCW5B44&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FWU0J56&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FXX-5085&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;04400329000109&lt;/CNPJ&gt;&lt;IE&gt;322079785116&lt;/IE&gt;&lt;xNome&gt;RODOTAC TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;RODOTAC (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOAO JORGE GARCIA LEAL&lt;/xLgr&gt;&lt;nro&gt;607&lt;/nro&gt;&lt;xBairro&gt;PARQUE INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3517406&lt;/cMun&gt;&lt;xMun&gt;GUAIRA&lt;/xMun&gt;&lt;CEP&gt;14790000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733302455&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;06225292000147&lt;/CNPJ&gt;&lt;IE&gt;283108491118&lt;/IE&gt;&lt;xNome&gt;TERLOC - TERMINAL LOGISTICO CESARI LTDA&lt;/xNome&gt;&lt;xFant&gt;TERLOC- TER. CESARI.&lt;/xFant&gt;&lt;fone&gt;01321028013&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AV ENGENHEIRO PLINIO DE QUEIROZ S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xCpl&gt;SP 55&lt;/xCpl&gt;&lt;xBairro&gt;PIACAGUERA&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;CUBATAO&lt;/xMun&gt;&lt;CEP&gt;11570000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604015457&lt;/CNPJ&gt;&lt;IE&gt;3714585320678&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;fone&gt;03433197198&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV ANTONIO CARLOS GUILLAUMON&lt;/xLgr&gt;&lt;nro&gt;800&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044760&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;5763.63&lt;/vTPrest&gt;&lt;vRec&gt;5763.63&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;4896.03&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;867.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;0.00&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;158564.15&lt;/vCarga&gt;&lt;proPred&gt;16 16 16 YM UNIK 16 GRANULADO&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;47050.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;1.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;158564.15&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35211206225292000147550010006132001012667246&lt;/chave&gt;&lt;dPrev&gt;2021-12-31&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;docAnt&gt;&lt;emiDocAnt&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;idDocAnt&gt;&lt;idDocAntEle&gt;&lt;chCTe&gt;35211250505924000118570010002833461002833460&lt;/chCTe&gt;&lt;/idDocAntEle&gt;&lt;/idDocAnt&gt;&lt;/emiDocAnt&gt;&lt;/docAnt&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;02625527&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211204400329000109570010000605971000605971&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211204400329000109570010000605971000605971"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;xdm1lb0HoFEFpofi1u08dGufrQo=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;oA6ABCJi1LjI/5SAmX/4/PHtnIdqDQVpGSuYEzMz0H7YuGkPnzlrmFkjmaZvwvRzzg4uI4XjO0pHXc78BTuiUpQ77lOywysGyJC8v6AC2WXIB0cP+NiMN9Daftf3FYOmvlv82xVpCXR1IkNCyZMkMJppXEGpolZaZWVFS3X8s5Y2DBlALI5HDcnqvCh0yw3LHrmgE7NTGjGFYu0IBAnhHxZ4LWMprCCCeNOsN25YlzCS5i2YE/VyS8Us1xYdsmZyJIYaRI9W2xH2+aQm1upCZdn+INb1ZZEC/axtNb0rKMp9rfCd6879hNuHq3fKTBLMlqdVW7IZsbWSSuoMsVmxsA==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHNzCCBR+gAwIBAgIIfFghCRNtqPgwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDIwMFoXDTIyMDkxNDEzNDIwMFowgdwxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDEPMA0GA1UEBxMGR3VhaXJhMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTEwMC4GA1UEAxMnUk9ET1RBQyBUUkFOU1BPUlRFUyBMVERBOjA0NDAwMzI5MDAwMTA5MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAp04ol/u6OamuPQYiuYvmBoabm9447ej3qfCk6KQY+gVddtzabeHC4yK1n9UOseY/2g2Wz2OQuVjZBz1mLb5aKDW9Hx4Hg4JXosEhRgHv+FxtlrgGJps+vVSke1fDiRKB9RxkryP5ngl3fOTaDXyXKAVw5Xir/ireILJkxoa7yItj3qOoX3WXO0e8IBBjeOJ3PyllIvh06I3LHaeqr6+hWxwuNsSxdYVLl+x0J5A1p8O+9MWEgTL6zEuST5aIoeESpEKC/oiOZwHujV8Zp6Ld3tbV45cNmE5qyq0Cv6WMxvySvmtBwBIS/2ftmk8dMnZb+R+iiO4Gh5gEFQ36XU3ezQIDAQABo4ICfTCCAnkwHwYDVR0jBBgwFoAUP9NcqRlN14gWLZgMrwre4U8kFrAwWQYIKwYBBQUHAQEETTBLMEkGCCsGAQUFBzAChj1odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUucDdiMIGvBgNVHREEgacwgaSBFnJvZG90YWNAcm9kb3RhYy5uZXQuYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMOMDQ0MDAzMjkwMDAxMDmgOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBTmf74GOUuAKM5iWH+pal5k4kRQYDAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAKffeE7P7VJywGR4dL48Nfq75Oa0zAPHLV/DXwo/bs847MeSBdauzpEiZ5xsUssJS/n73euRm/aaQ0Ai0fTYDcl6DAj0Bpn0kE3N9MF0/rb/35Ion/zwbhfzLHSby6MuH+NXvZheexyZV+LdWMnTY875AhHqFTLMH/e7TML3AukZFVrZDZ/KyjVGNji6XTmOxg0qt3hiEapOR+ODEqZO6FiYYS/7DGu+akrOzT8eOTddbUUzx2eZ6PctqSV7TZXTYtkfrq9pZgcFMjKUxwtnaQ9iE1ZttFTcVqIOWxPFLc/5pxFRfaFL+/5dhRs777Fox5nHBE9GjaI2alR9fidF4BJ+4UkcEZ17NaS8tzGYuP3XjieSWQD5eEAaGDA4eS+0zpNP6Z30UFqc5gmfj8EZaRuxaAUe+egORdxErP3J7CBPFEei/t1V/+E56JKHe75TgM+hTb+gxKyVThQULKZQgv/OiXD0O+cRBNHx0wNyvr/Srh61E9os66kg37kgfNZnMwBZOG4QmUtjJA5ChzJ99yXk6hNKhWXZrB+WwlBa2X/b/cff2nKx9wnw0ii3xjIAnkcWs2koAw5QaLUpNlHBTdTDVTMYZsXP9fSGKeom+/QDE6tZ5EstYiopzB2LRCGIB/PAwuYJX5fbcyMQTiu0A/6OCjQ3Bk9dK6myCbqSXJDb&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211204400329000109570010000605971000605971&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-30T10:33:52-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214687645175&lt;/nProt&gt;&lt;digVal&gt;xdm1lb0HoFEFpofi1u08dGufrQo=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35211250505924000118570010002833221002833221-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211250505924000118570010002833221002833221-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211250505924000118570010002833221002833221"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00283322&lt;/cCT&gt;&lt;CFOP&gt;6352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;283322&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-29T11:30:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;1&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3548500&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTOS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3104007&lt;/cMunFim&gt;&lt;xMunFim&gt;ARAXA&lt;/xMunFim&gt;&lt;UFFim&gt;MG&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;SILVIA MARTINS&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;STS&lt;/xOrig&gt;&lt;xDest&gt;ARX&lt;/xDest&gt;&lt;xRota&gt;STSARX&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTOS&lt;/origCalc&gt;&lt;destCalc&gt;ARAXA&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 1.164,08; Referencia do Cliente : 21660;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;C0260&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;21660&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;220.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;WILSON APARECIDO DOS SANTOS&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;077.771.038-22&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;GHL1A73&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FFK5B74&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FMJ8I56&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FPE-8F35&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;00000000000000&lt;/CNPJ&gt;&lt;IE&gt;ISENTO&lt;/IE&gt;&lt;xNome&gt;CANPOTEX LIMITED&lt;/xNome&gt;&lt;xFant&gt;CANPOTEX (COSTADO)&lt;/xFant&gt;&lt;fone&gt;01734445550&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AAAAAA&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;EXTERIOR&lt;/xBairro&gt;&lt;cMun&gt;9999999&lt;/cMun&gt;&lt;xMun&gt;EXTERIOR&lt;/xMun&gt;&lt;CEP&gt;00000000&lt;/CEP&gt;&lt;UF&gt;EX&lt;/UF&gt;&lt;cPais&gt;1490&lt;/cPais&gt;&lt;xPais&gt;CANADA&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;exped&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;xNome&gt;COMPANHIA DOCAS DO ESTADO DE SAO PAULO CODESP&lt;/xNome&gt;&lt;fone&gt;01300000000&lt;/fone&gt;&lt;enderExped&gt;&lt;xLgr&gt;CONSELHEIRO RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;CEP&gt;11015900&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderExped&gt;&lt;/exped&gt;&lt;dest&gt;&lt;CNPJ&gt;88305859001555&lt;/CNPJ&gt;&lt;IE&gt;0027743880010&lt;/IE&gt;&lt;xNome&gt;NUTRIEN AG SOLUTIONS IND E COM PROD AGRI LTDA&lt;/xNome&gt;&lt;fone&gt;01532758780&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;ROD - MG 146 S/N FAZENDA PAO DE ACUCAR&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;ZONA RURAL&lt;/xBairro&gt;&lt;cMun&gt;3104007&lt;/cMun&gt;&lt;xMun&gt;ARAXA&lt;/xMun&gt;&lt;CEP&gt;38183000&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;5478.00&lt;/vTPrest&gt;&lt;vRec&gt;5478.00&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;4610.40&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;867.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS00&gt;&lt;CST&gt;00&lt;/CST&gt;&lt;vBC&gt;5478.00&lt;/vBC&gt;&lt;pICMS&gt;12.00&lt;/pICMS&gt;&lt;vICMS&gt;657.36&lt;/vICMS&gt;&lt;/ICMS00&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;1164.08&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;99181.68&lt;/vCarga&gt;&lt;proPred&gt;KCL 60%-CLORETO DE POTASSIO&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;24900.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;25.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;99181.68&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;31211288305859001555550920000006441365062542&lt;/chave&gt;&lt;dPrev&gt;2021-12-29&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211250505924000118570010002833221002833221&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211250505924000118570010002833221002833221"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;x7Yo0m2aoxPyHS7weXWBiKA/0Mg=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;vr56jvaf0Z2MFo1R+fcERry9SUmHwujO8qdLP5XFOze3xWqyV4G62ggs8LQ3Izm8i0Nmn25mVdjdeYD8ljfE99bs5fDfHJkSzIG8enkNQgdnkfW05PHz7lzgM5YaTukpzdJLPk1ma9PzzhLKH4gAFk93g0R1sNsAxDq+IptjvLJNuHJyzVl2Nl9GI/yYFU2NwlK5fFhxmlySBepadnx+XqVQ5MBtJXL0G4dpVedUkUUpUgACTl6YkaMRmzIAFncTbdzeq/6dGbQMKi1+aOaEvISm6ST4M+zUB6/OE3Agtic9o4pQSeAaOq/7rwr/9oiefe9vURcJ26qUlQeDAqOgKQ==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211250505924000118570010002833221002833221&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-29T11:32:41-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214683822160&lt;/nProt&gt;&lt;digVal&gt;x7Yo0m2aoxPyHS7weXWBiKA/0Mg=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35211250505924000118570010002833251002833258-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211250505924000118570010002833251002833258-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211250505924000118570010002833251002833258"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00283325&lt;/cCT&gt;&lt;CFOP&gt;6352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;283325&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-29T14:12:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;8&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3548500&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTOS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3170107&lt;/cMunFim&gt;&lt;xMunFim&gt;UBERABA&lt;/xMunFim&gt;&lt;UFFim&gt;MG&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;SILVIA MARTINS&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;STS&lt;/xOrig&gt;&lt;xDest&gt;UBR&lt;/xDest&gt;&lt;xRota&gt;STSUBR&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTOS&lt;/origCalc&gt;&lt;destCalc&gt;UBERABA&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 1.206,66; Referencia do Cliente : 266921;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;C0220&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;266921&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;210.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;JOSE MALAGOGIM&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;084.770.188-39&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;DTE6867&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;DKU3317&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;EXN9979&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;BVT-9908&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;00000000000000&lt;/CNPJ&gt;&lt;IE&gt;ISENTO&lt;/IE&gt;&lt;xNome&gt;YARA SWITZERLAND LTD.&lt;/xNome&gt;&lt;xFant&gt;YARA CAIS COMERCIAL&lt;/xFant&gt;&lt;fone&gt;00000000000&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AAAAAAA&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;AAAAA&lt;/xBairro&gt;&lt;cMun&gt;9999999&lt;/cMun&gt;&lt;xMun&gt;EXTERIOR&lt;/xMun&gt;&lt;CEP&gt;00000000&lt;/CEP&gt;&lt;UF&gt;EX&lt;/UF&gt;&lt;cPais&gt;7676&lt;/cPais&gt;&lt;xPais&gt;SUICA&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;exped&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;xNome&gt;COMPANHIA DOCAS DO ESTADO DE SAO PAULO CODESP&lt;/xNome&gt;&lt;fone&gt;01300000000&lt;/fone&gt;&lt;enderExped&gt;&lt;xLgr&gt;CONSELHEIRO RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;CEP&gt;11015900&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderExped&gt;&lt;/exped&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604015457&lt;/CNPJ&gt;&lt;IE&gt;3714585320678&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;fone&gt;03433197198&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV ANTONIO CARLOS GUILLAUMON&lt;/xLgr&gt;&lt;nro&gt;800&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044760&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;5678.40&lt;/vTPrest&gt;&lt;vRec&gt;5678.40&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;4810.80&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;867.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS00&gt;&lt;CST&gt;00&lt;/CST&gt;&lt;vBC&gt;5678.40&lt;/vBC&gt;&lt;pICMS&gt;12.00&lt;/pICMS&gt;&lt;vICMS&gt;681.41&lt;/vICMS&gt;&lt;/ICMS00&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;1206.66&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;91128.04&lt;/vCarga&gt;&lt;proPred&gt;16 16 16 YM UNIK 16 GRANULADO&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;27040.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;27.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;91128.04&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;31211292660604015457550760000200271085528499&lt;/chave&gt;&lt;dPrev&gt;2021-12-30&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211250505924000118570010002833251002833258&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211250505924000118570010002833251002833258"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;XQ4xOMlsW1fTisGNBhkrite9wog=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;frdUjQBwKMtFMIOzQvdm+BJM3TdwZ9tuVa8A/1ehw/mhdvUsVtbRDrbfT16xLH2i0ccKyDOJg9buIpBCE8143Aqj72fuxIqWd5g3UwP87+u3kJkCFRwnpSHn9FsWqBTzVBjOjhtT3kOBraAVcfwQSDxbSkcMh/6vzFuXnqjIfFaX0G/amrI3f1r4Rg2BtWD4SvxpV+lo4tk8Fi/raGQfzfspRA8o0IxrTotAzLONhYXR9i+W9n8PRnkbeft4ZjFtuvHbCWHWwlYHpffOwKAcWQ+rxYSLJ1OcA/KWnxKbZoRO06+QrzXqHrd6UM/eSaS9T6x/FevawhPZEOy64NMjKg==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211250505924000118570010002833251002833258&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-29T14:14:14-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214684334616&lt;/nProt&gt;&lt;digVal&gt;XQ4xOMlsW1fTisGNBhkrite9wog=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35211250505924000118570010002833261002833263-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211250505924000118570010002833261002833263-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211250505924000118570010002833261002833263"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00283326&lt;/cCT&gt;&lt;CFOP&gt;6352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;283326&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-29T14:13:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;3&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3548500&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTOS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3170107&lt;/cMunFim&gt;&lt;xMunFim&gt;UBERABA&lt;/xMunFim&gt;&lt;UFFim&gt;MG&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;SILVIA MARTINS&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;STS&lt;/xOrig&gt;&lt;xDest&gt;UBR&lt;/xDest&gt;&lt;xRota&gt;STSUBR&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTOS&lt;/origCalc&gt;&lt;destCalc&gt;UBERABA&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 929,09; Referencia do Cliente : 266921;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;C0220&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;266921&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;210.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;JOSE MALAGOGIM&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;084.770.188-39&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;DTE6867&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;DKU3317&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;EXN9979&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;BVT-9908&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;00000000000000&lt;/CNPJ&gt;&lt;IE&gt;ISENTO&lt;/IE&gt;&lt;xNome&gt;YARA SWITZERLAND LTD.&lt;/xNome&gt;&lt;xFant&gt;YARA CAIS COMERCIAL&lt;/xFant&gt;&lt;fone&gt;00000000000&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AAAAAAA&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;AAAAA&lt;/xBairro&gt;&lt;cMun&gt;9999999&lt;/cMun&gt;&lt;xMun&gt;EXTERIOR&lt;/xMun&gt;&lt;CEP&gt;00000000&lt;/CEP&gt;&lt;UF&gt;EX&lt;/UF&gt;&lt;cPais&gt;7676&lt;/cPais&gt;&lt;xPais&gt;SUICA&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;exped&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;xNome&gt;COMPANHIA DOCAS DO ESTADO DE SAO PAULO CODESP&lt;/xNome&gt;&lt;fone&gt;01300000000&lt;/fone&gt;&lt;enderExped&gt;&lt;xLgr&gt;CONSELHEIRO RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;CEP&gt;11015900&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderExped&gt;&lt;/exped&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604015457&lt;/CNPJ&gt;&lt;IE&gt;3714585320678&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;fone&gt;03433197198&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV ANTONIO CARLOS GUILLAUMON&lt;/xLgr&gt;&lt;nro&gt;800&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044760&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;4372.20&lt;/vTPrest&gt;&lt;vRec&gt;4372.20&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;3504.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;867.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS00&gt;&lt;CST&gt;00&lt;/CST&gt;&lt;vBC&gt;4372.20&lt;/vBC&gt;&lt;pICMS&gt;12.00&lt;/pICMS&gt;&lt;vICMS&gt;524.66&lt;/vICMS&gt;&lt;/ICMS00&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;929.09&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;70165.90&lt;/vCarga&gt;&lt;proPred&gt;16 16 16 YM UNIK 16 GRANULADO&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;20820.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;21.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;70165.90&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;31211292660604015457550760000200281302910709&lt;/chave&gt;&lt;dPrev&gt;2021-12-30&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211250505924000118570010002833261002833263&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211250505924000118570010002833261002833263"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;zhBU/0cFgHHgfaHL69Bm3mcOjE0=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;rhnbnzydsDL4yqpJBdOtwYWqLWmTL0BLfboB9OXE+uStMz715/DVRouX3vGxjlmF+zgxIx7515B/dipehL9nOr5TE3UcodvlBgh5HZOAKayrHZtoe2H9UClChOf9h0M4fPPqrJyRGITdBq5zubPHa758GNP2o0Pzpb+HgQvSEuRblGmB/qFzbNC15nB/LN8StuAhM5EtSVJ9DpwrgG2gKu1LhVAVSQziZ51N9fr1Qu624cE7tp4EUN9BDuXYlb9MRFNVj0vYIA7WmqAwPNSNVAPSXZ0s5fp53YqVBjt89V0mK5Nct9tTrGzpg4h4jR2/c0B2yVhy/Yv2RHuN+o4cSw==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211250505924000118570010002833261002833263&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-29T14:14:16-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214684334709&lt;/nProt&gt;&lt;digVal&gt;zhBU/0cFgHHgfaHL69Bm3mcOjE0=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35211250505924000118570010002833421002833429-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211250505924000118570010002833421002833429-ret-cons-cte.xml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211250505924000118570010002833421002833429"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00283342&lt;/cCT&gt;&lt;CFOP&gt;6352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;283342&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-30T02:31:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;9&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3513504&lt;/cMunIni&gt;&lt;xMunIni&gt;CUBATAO&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3170107&lt;/cMunFim&gt;&lt;xMunFim&gt;UBERABA&lt;/xMunFim&gt;&lt;UFFim&gt;MG&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;LUIZ FELIPE NETTO DO&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;CBT&lt;/xOrig&gt;&lt;xDest&gt;UBR&lt;/xDest&gt;&lt;xRota&gt;CBTUBR&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;CUBATAO&lt;/origCalc&gt;&lt;destCalc&gt;UBERABA&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 1.453,11; Referencia do Cliente : 4500712092;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;C0270&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;4500712092&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;145.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;RAFAEL RIBEIRO RODRIGUES&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;336.420.228-12&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;FAI5F78&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;EKH2723&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;EKH2724&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;EKH-2722&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;06225292000147&lt;/CNPJ&gt;&lt;IE&gt;283108491118&lt;/IE&gt;&lt;xNome&gt;TERLOC - TERMINAL LOGISTICO CESARI LTDA&lt;/xNome&gt;&lt;xFant&gt;TERLOC- TER. CESARI.&lt;/xFant&gt;&lt;fone&gt;01321028013&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AV ENGENHEIRO PLINIO DE QUEIROZ S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xCpl&gt;SP 55&lt;/xCpl&gt;&lt;xBairro&gt;PIACAGUERA&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;CUBATAO&lt;/xMun&gt;&lt;CEP&gt;11570000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604015457&lt;/CNPJ&gt;&lt;IE&gt;3714585320678&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;fone&gt;03433197198&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV ANTONIO CARLOS GUILLAUMON&lt;/xLgr&gt;&lt;nro&gt;800&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044760&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;6838.20&lt;/vTPrest&gt;&lt;vRec&gt;6838.20&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;5970.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;867.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS00&gt;&lt;CST&gt;00&lt;/CST&gt;&lt;vBC&gt;6838.20&lt;/vBC&gt;&lt;pICMS&gt;12.00&lt;/pICMS&gt;&lt;vICMS&gt;820.58&lt;/vICMS&gt;&lt;/ICMS00&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;1453.11&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;158934.86&lt;/vCarga&gt;&lt;proPred&gt;FERTILIZANTE MINERAL COMPLEXO YARAMILA 16-16-16 GR&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;47160.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;1.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;158934.86&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35211206225292000147550010006131931012667061&lt;/chave&gt;&lt;dPrev&gt;2021-12-30&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211250505924000118570010002833421002833429&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211250505924000118570010002833421002833429"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;hcEwJg1eX0fIGZwz87wTvmVDEHI=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;FFTCvGDwn6RMhLg1vevKO3s6w0sWwnY4TEtipNyIVucYJrE0PqC6ckCvS5LDY03hzBIkylgkkp5E3OZ7w8hIxi5J27h5j8RAAsyUdZ9lrD2NAgEYxyyK/B0IqGWTmcYx+EYbcxkRCsgzBrpuX/AibzCT7wLChb6kYbZyuhFVobqvWMbzSZ9dAG8cpfH9ZDJ8QolgFcYOnjiaoVHhaeDVb7MM9ojSfr87yZhqoz1xph9jTk3AXrwwjP8beDagD1AIO3QCsFdLyQIM0cA1zgCzsr5wDbihR3ssqy5N+xL38FJhIWA9RDDhRR2oJivvxMZ2CaI+xgbvNlBp0Xgb2oZclg==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211250505924000118570010002833421002833429&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-30T02:32:36-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214686468927&lt;/nProt&gt;&lt;digVal&gt;hcEwJg1eX0fIGZwz87wTvmVDEHI=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+    <x:t>35210833931486000564550040000805401453515100.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35210833931486000564550040000805401453515100.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;nfeProc versao="4.00" xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;NFe xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;infNFe Id="NFe35210833931486000564550040000805401453515100" versao="4.00"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cNF&gt;45351510&lt;/cNF&gt;&lt;natOp&gt;VENDA MERC ADQ OU RECEBIDA DE TERCEIROS&lt;/natOp&gt;&lt;mod&gt;55&lt;/mod&gt;&lt;serie&gt;4&lt;/serie&gt;&lt;nNF&gt;80540&lt;/nNF&gt;&lt;dhEmi&gt;2021-08-01T14:01:06-03:00&lt;/dhEmi&gt;&lt;dhSaiEnt&gt;2021-08-01T14:01:06-03:00&lt;/dhSaiEnt&gt;&lt;tpNF&gt;1&lt;/tpNF&gt;&lt;idDest&gt;1&lt;/idDest&gt;&lt;cMunFG&gt;3509254&lt;/cMunFG&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;0&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;finNFe&gt;1&lt;/finNFe&gt;&lt;indFinal&gt;0&lt;/indFinal&gt;&lt;indPres&gt;9&lt;/indPres&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;200&lt;/verProc&gt;&lt;/ide&gt;&lt;emit&gt;&lt;CNPJ&gt;33931486000564&lt;/CNPJ&gt;&lt;xNome&gt;MOSAIC FERTILIZANTES PEK LTDA.&lt;/xNome&gt;&lt;xFant&gt;MOSAIC FERTILIZANTES PEK LTDA.&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;RODOVIA BR-116&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;COMPLEXO INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3509254&lt;/cMun&gt;&lt;xMun&gt;CAJATI&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;CEP&gt;11950000&lt;/CEP&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderEmit&gt;&lt;IE&gt;740011589111&lt;/IE&gt;&lt;CRT&gt;3&lt;/CRT&gt;&lt;/emit&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604017581&lt;/CNPJ&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES SA&lt;/xNome&gt;&lt;enderDest&gt;&lt;xLgr&gt;11AV AVENIDA PROFESS&lt;/xLgr&gt;&lt;nro&gt;1300&lt;/nro&gt;&lt;xBairro&gt;BETEL&lt;/xBairro&gt;&lt;cMun&gt;3536505&lt;/cMun&gt;&lt;xMun&gt;PAULINIA&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;CEP&gt;13148908&lt;/CEP&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;fone&gt;5132301300&lt;/fone&gt;&lt;/enderDest&gt;&lt;indIEDest&gt;1&lt;/indIEDest&gt;&lt;IE&gt;513157609112&lt;/IE&gt;&lt;/dest&gt;&lt;retirada&gt;&lt;CNPJ&gt;02476026000802&lt;/CNPJ&gt;&lt;xLgr&gt;RODOVIA SP 55 ESTRADA CUBATAO KM 65,8&lt;/xLgr&gt;&lt;nro&gt;SN&lt;/nro&gt;&lt;xBairro&gt;ILHA DO CARDOSO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;/retirada&gt;&lt;autXML&gt;&lt;CNPJ&gt;55681274000185&lt;/CNPJ&gt;&lt;/autXML&gt;&lt;det nItem="1"&gt;&lt;prod&gt;&lt;cProd&gt;300500&lt;/cProd&gt;&lt;cEAN&gt;SEM GTIN&lt;/cEAN&gt;&lt;xProd&gt;ENXOFRE IMPORTADO FERTILIZANTE&lt;/xProd&gt;&lt;NCM&gt;25030010&lt;/NCM&gt;&lt;EXTIPI&gt;000&lt;/EXTIPI&gt;&lt;CFOP&gt;5106&lt;/CFOP&gt;&lt;uCom&gt;TO&lt;/uCom&gt;&lt;qCom&gt;35.3000&lt;/qCom&gt;&lt;vUnCom&gt;1343.99&lt;/vUnCom&gt;&lt;vProd&gt;47442.85&lt;/vProd&gt;&lt;cEANTrib&gt;SEM GTIN&lt;/cEANTrib&gt;&lt;uTrib&gt;TO&lt;/uTrib&gt;&lt;qTrib&gt;35.3000&lt;/qTrib&gt;&lt;vUnTrib&gt;1343.99&lt;/vUnTrib&gt;&lt;indTot&gt;1&lt;/indTot&gt;&lt;xPed&gt;3070423&lt;/xPed&gt;&lt;/prod&gt;&lt;imposto&gt;&lt;ICMS&gt;&lt;ICMS00&gt;&lt;orig&gt;6&lt;/orig&gt;&lt;CST&gt;00&lt;/CST&gt;&lt;modBC&gt;3&lt;/modBC&gt;&lt;vBC&gt;0.00&lt;/vBC&gt;&lt;pICMS&gt;0.00&lt;/pICMS&gt;&lt;vICMS&gt;0.00&lt;/vICMS&gt;&lt;/ICMS00&gt;&lt;/ICMS&gt;&lt;IPI&gt;&lt;cEnq&gt;999&lt;/cEnq&gt;&lt;IPINT&gt;&lt;CST&gt;53&lt;/CST&gt;&lt;/IPINT&gt;&lt;/IPI&gt;&lt;PIS&gt;&lt;PISNT&gt;&lt;CST&gt;06&lt;/CST&gt;&lt;/PISNT&gt;&lt;/PIS&gt;&lt;COFINS&gt;&lt;COFINSNT&gt;&lt;CST&gt;06&lt;/CST&gt;&lt;/COFINSNT&gt;&lt;/COFINS&gt;&lt;/imposto&gt;&lt;infAdProd&gt;REVENDA&lt;/infAdProd&gt;&lt;/det&gt;&lt;total&gt;&lt;ICMSTot&gt;&lt;vBC&gt;0.00&lt;/vBC&gt;&lt;vICMS&gt;0.00&lt;/vICMS&gt;&lt;vICMSDeson&gt;0.00&lt;/vICMSDeson&gt;&lt;vFCPUFDest&gt;0.00&lt;/vFCPUFDest&gt;&lt;vICMSUFDest&gt;0.00&lt;/vICMSUFDest&gt;&lt;vICMSUFRemet&gt;0.00&lt;/vICMSUFRemet&gt;&lt;vFCP&gt;0.00&lt;/vFCP&gt;&lt;vBCST&gt;0.00&lt;/vBCST&gt;&lt;vST&gt;0.00&lt;/vST&gt;&lt;vFCPST&gt;0.00&lt;/vFCPST&gt;&lt;vFCPSTRet&gt;0.00&lt;/vFCPSTRet&gt;&lt;vProd&gt;47442.85&lt;/vProd&gt;&lt;vFrete&gt;0.00&lt;/vFrete&gt;&lt;vSeg&gt;0.00&lt;/vSeg&gt;&lt;vDesc&gt;0.00&lt;/vDesc&gt;&lt;vII&gt;0.00&lt;/vII&gt;&lt;vIPI&gt;0.00&lt;/vIPI&gt;&lt;vIPIDevol&gt;0.00&lt;/vIPIDevol&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;vOutro&gt;0.00&lt;/vOutro&gt;&lt;vNF&gt;47442.85&lt;/vNF&gt;&lt;/ICMSTot&gt;&lt;/total&gt;&lt;transp&gt;&lt;modFrete&gt;1&lt;/modFrete&gt;&lt;transporta&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xEnder&gt;AV JOS AUGUSTO CARVALHO 4063&lt;/xEnder&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;/transporta&gt;&lt;veicTransp&gt;&lt;placa&gt;FIJ9641&lt;/placa&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;/veicTransp&gt;&lt;vol&gt;&lt;qVol&gt;35&lt;/qVol&gt;&lt;esp&gt;GRANEL&lt;/esp&gt;&lt;marca&gt;ENXOFRE IMPORTADO FERTILIZANTE&lt;/marca&gt;&lt;nVol&gt;0&lt;/nVol&gt;&lt;pesoL&gt;35300.000&lt;/pesoL&gt;&lt;pesoB&gt;35300.000&lt;/pesoB&gt;&lt;/vol&gt;&lt;/transp&gt;&lt;cobr&gt;&lt;fat&gt;&lt;nFat&gt;80540&lt;/nFat&gt;&lt;vOrig&gt;47442.85&lt;/vOrig&gt;&lt;vDesc&gt;0.00&lt;/vDesc&gt;&lt;vLiq&gt;47442.85&lt;/vLiq&gt;&lt;/fat&gt;&lt;dup&gt;&lt;nDup&gt;001&lt;/nDup&gt;&lt;dVenc&gt;2021-08-11&lt;/dVenc&gt;&lt;vDup&gt;47442.85&lt;/vDup&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;pag&gt;&lt;detPag&gt;&lt;tPag&gt;01&lt;/tPag&gt;&lt;vPag&gt;47442.85&lt;/vPag&gt;&lt;/detPag&gt;&lt;/pag&gt;&lt;infAdic&gt;&lt;infCpl&gt;BRUTO 56.770 TARA 21.470 LIQUIDO 35.300  CARRETA 2 FMT 2602  CV GBG 7851MERCADORIA SEGUIU DIRETAMENTE DO PORTO DE SANTOS NOS TERMOS DO ARTIGO 125, PARAG. 3 DO RICMSSPMERCADORIA SEGUIU DIRETAMENTE DO PORTO DE SANTOS NOS TERMOS DO ARTIGO 125, PARAG. 3 DO RICMSSPIPI NAO TRIBUTADO CONFORME CAPITULO 25 DA TIPICERTIFICAMOS QUE O PRODUTO ESTA ADEQUADAMENTE ACONDICIONADO PARA SUPORTAR OS RISCOS DE CARREGAMENTO, DESCARREGAMENTO, TRANSBORDO E TRANSPORTE, CONFORME DECRETO N 96.0441988 - PRODUTO PERIGOSO N 1350 - N RISCO 40 CLASSE 4.1PRODUTO IMPORTADO, ARMAZENAR EM LUGAR SECO, COBERTO E AREJADOMERCADORIA SAIDA DO TERMINAL PRIVATIVO DA ULTRAFERTIL - SANTOS-SPVALIDADE DO PRODUTO INDETERMINADANATUREZA DA OPERACAO VENDA DE MERCADORIA ADQUIRIDA OU RECEBIDA DE TERCEIROS, QUE NAO DEVA POR ELE TRANSITARDI 211160904-7, DATA DA DI 17062021, NAVIO ASTRA CENTAURUS, NR. IMP 814NR NF MAE 76260, DATA NF MAE 18062021, PEDIDO 3070423, TIQUETE 399744004305111DATA EFETIVA DE VENCIMENTO 11082021NUMERO DO PEDIDO DO CLIENTE 4500651480&lt;/infCpl&gt;&lt;obsCont xCampo="NR_NF_MAE"&gt;&lt;xTexto&gt;76260&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NR_PEDIDO"&gt;&lt;xTexto&gt;3070423&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NR_IMPORTACAO"&gt;&lt;xTexto&gt;814&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NR_TIQUETE"&gt;&lt;xTexto&gt;399744004305111&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="NAVIO"&gt;&lt;xTexto&gt;ASTRA CENTAURUS&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="CD_TIPO_NF"&gt;&lt;xTexto&gt;S&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="CD_OPERACAO"&gt;&lt;xTexto&gt;09&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;obsCont xCampo="CD_EMPRESA"&gt;&lt;xTexto&gt;1972&lt;/xTexto&gt;&lt;/obsCont&gt;&lt;/infAdic&gt;&lt;compra&gt;&lt;xPed&gt;4500651480&lt;/xPed&gt;&lt;/compra&gt;&lt;infRespTec&gt;&lt;CNPJ&gt;11342233000199&lt;/CNPJ&gt;&lt;xContato&gt;Helpdesk&lt;/xContato&gt;&lt;email&gt;helpdesk@micsistemas.com.br&lt;/email&gt;&lt;fone&gt;1340422786&lt;/fone&gt;&lt;/infRespTec&gt;&lt;/infNFe&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#NFe35210833931486000564550040000805401453515100"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;WvQSucPgbCx9VXO8cprfrlyirVc=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;eQMAqyh1S9VHLPHIhDQsjv4fRSsF7IEwqx4Vvz1ozaPRt3JCivo0oGzombes0XpkUMMbCRu5jLH7yAPRZ124yizPqU5Aa17v5u3EV3KaXzaeSLXDFahJmo4kqV9HQqx3wSRrkAGepVr4Sc72YWttHLySa9t412rWqfkOOSHDbDNeV6Aq8o/xPoRqaYKq5Q+D4zm0NxZ3SjRzBdGmPsuIWjpr6ZYCk91+4q/d4vMzhOOoUkkc191wsVHUoZIU/Nx03K6DHFO2h3dm0JGe2rhdr4K9R9IablruhBY6lCQXe2B0d1oIXBbKW6YtcdG0ieNuDZLYTmjD31N5fGc4aEImBw==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHtTCCBZ2gAwIBAgIIH2uUbVqTFmAwDQYJKoZIhvcNAQELBQAwTDELMAkGA1UEBhMCQlIxEzARBgNVBAoMCklDUC1CcmFzaWwxKDAmBgNVBAMMH1NFUkFTQSBDZXJ0aWZpY2Fkb3JhIERpZ2l0YWwgdjUwHhcNMjAxMTEyMTgyNDAwWhcNMjExMTEyMTgyNDAwWjCB/jELMAkGA1UEBhMCQlIxEzARBgNVBAoMCklDUC1CcmFzaWwxFDASBgNVBAsMCyhFTSBCUkFOQ08pMRgwFgYDVQQLDA8wMDAwMDEwMDk5MDA2NDYxFDASBgNVBAsMCyhFTSBCUkFOQ08pMRQwEgYDVQQLDAsoRU0gQlJBTkNPKTEoMCYGA1UECwwfU0VSQVNBIENlcnRpZmljYWRvcmEgRGlnaXRhbCB2NTEXMBUGA1UECwwONjIxNzM2MjAwMDAxODAxEzARBgNVBAsMClBSRVNFTkNJQUwxJjAkBgNVBAMMHU1PU0FJQyBGRVJUSUxJWkFOVEVTIFAmSyBMVERBMIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAoZjhzt6PA84oNM3gyhw8lvxkLIZQwyJzOpOnUllMAv3hT5xWtckoQzNpCJ+t1zobHSeGyB1msA5swGEaiy5e80A+jGudCbpkKQfldbq0p2BgvgkEsEvJKG9EX/o0O6ymJJJbMRkl8jvTNhJdW3hxIZrf4ysJaY1cIv+ec9v8frJNu+Oz/gBZHzieVg6SfNU8MGfhO7YFFLovTJSqdLo+vfKSXUmrMAAW5W8Bu1pm4jUKCPr9RT78V47vBjCEwln0NQsCorCoFaR0JdouMw7TrQdUj920ZX/qyejTWCMZJP4HtTdpPL1EJMUvpKM6TeoKx6M/V2aqqCHKGicWNv8kkwIDAQABo4IC5jCCAuIwHwYDVR0jBBgwFoAUVnWvSnOy2AjEfftsKBwR1ffBqMwwgZcGCCsGAQUFBwEBBIGKMIGHMEcGCCsGAQUFBzAChjtodHRwOi8vd3d3LmNlcnRpZmljYWRvZGlnaXRhbC5jb20uYnIvY2FkZWlhcy9zZXJhc2FjZHY1LnA3YjA8BggrBgEFBQcwAYYwaHR0cDovL29jc3AuY2VydGlmaWNhZG9kaWdpdGFsLmNvbS5ici9zZXJhc2FjZHY1MIHFBgNVHREEgb0wgbqBHFJFSU5BTERPLkNPUlJFQUBNT1NBSUNDTy5DT02gPgYFYEwBAwSgNRMzMTgxMDE5NjkxNTY1NjIzMDg4MDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoCYGBWBMAQMCoB0TG1NFUkdJTyBMVUlTIENBUlJBTUFPIFZJRUlSQaAZBgVgTAEDA6AQEw4zMzkzMTQ4NjAwMDEzMKAXBgVgTAEDB6AOEwwwMDAwMDAwMDAwMDAwcQYDVR0gBGowaDBmBgZgTAECAQYwXDBaBggrBgEFBQcCARZOaHR0cDovL3B1YmxpY2FjYW8uY2VydGlmaWNhZG9kaWdpdGFsLmNvbS5ici9yZXBvc2l0b3Jpby9kcGMvZGVjbGFyYWNhby1zY2QucGRmMB0GA1UdJQQWMBQGCCsGAQUFBwMCBggrBgEFBQcDBDCBmwYDVR0fBIGTMIGQMEmgR6BFhkNodHRwOi8vd3d3LmNlcnRpZmljYWRvZGlnaXRhbC5jb20uYnIvcmVwb3NpdG9yaW8vbGNyL3NlcmFzYWNkdjUuY3JsMEOgQaA/hj1odHRwOi8vbGNyLmNlcnRpZmljYWRvcy5jb20uYnIvcmVwb3NpdG9yaW8vbGNyL3NlcmFzYWNkdjUuY3JsMB0GA1UdDgQWBBTFmtw06rPT7PBwhOgKVLb+yzqXtjAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAHOdmbJZH747iKn7hYjYNYo31PM9OEyU933pNCBzy8H6GNB0QC45pbofkdlnxpXcBeexFl03mfnK0QRW7qeAr/Bohz3FH7DFfqv3zc9LnU81oaARwU/hnvgI/nBONdnd00aTfsJnwwWLlPYCKfZ044VG0xIS+noWkq4t8P3YkYzjVdwKyBkMYHOG3cmWpv61JYXg5o1s2eDscOpcsqE9EfzK3XQ5SFP3JnqPtJGGKrsKP3iwVfQt3eqj2IdKt1dnw20A14irqZNudBJbTTh6yfbh+oiIyuKUQDnlhhzsWGZd9FjOmmjxr/GrddNEIgsZNXCpiJ19SpicAocuQrgKliPPK0udK5J3Ck++kw0v//XBJ7sqP2UB+xOxuYtMCRACdje1brg39HNKFnW/YllYsHLrX29JHMPC8dqyP9Cky98LEA3Ai4GPbHy7e1BDZ3TDUM1VzHJ18ntc2s1iULzm5ZFAur9LyPySrtg5Dsin4P9HCoguEFfRqOI143/Ya4qgZ18izPq2j9I9gMaq4226Om8NY6cdPMhNNHHdU27a3tcMkTCw73EfXqbxQ/zt4wWCPnRsjFVc8+fQ+HS+PIO53hzDmTxlFaikJUj1V/qaW1suke6O8W85APett9dqV9pt8s2f8mJQnV5VookWSpKqQW1UVbcChPUDKZhvD6TIFBzv&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/NFe&gt;&lt;protNFe versao="4.00"&gt;&lt;infProt Id="Id135210871173944"&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP_NFE_PL009_V4&lt;/verAplic&gt;&lt;chNFe&gt;35210833931486000564550040000805401453515100&lt;/chNFe&gt;&lt;dhRecbto&gt;2021-08-01T14:01:25-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135210871173944&lt;/nProt&gt;&lt;digVal&gt;WvQSucPgbCx9VXO8cprfrlyirVc=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso da NF-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protNFe&gt;&lt;/nfeProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35210850505924000118570010002698471002698478-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35210850505924000118570010002698471002698478-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35210850505924000118570010002698471002698478"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00269847&lt;/cCT&gt;&lt;CFOP&gt;5352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;269847&lt;/nCT&gt;&lt;dhEmi&gt;2021-08-01T14:06:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;8&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.1&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3548500&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTOS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3536505&lt;/cMunFim&gt;&lt;xMunFim&gt;PAULINIA&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;SILVIA MARTINS&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;STS&lt;/xOrig&gt;&lt;xDest&gt;PLN&lt;/xDest&gt;&lt;xRota&gt;STSPLN&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTOS&lt;/origCalc&gt;&lt;destCalc&gt;PAULINIA&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 250,77;ESTADIA APOS 24 HRS SEM RETROACAO. Referencia do Cliente : 3070423;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;C0417&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;3070423&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;76.800000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;EDUARDO DAVANCO BENEDITO&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;224.672.958-00&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;GBG7851&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FIJ9641&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FMT2602&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;33931486000564&lt;/CNPJ&gt;&lt;IE&gt;740011589111&lt;/IE&gt;&lt;xNome&gt;MOSAIC FERTILIZANTES P&amp;amp;K S.A.&lt;/xNome&gt;&lt;xFant&gt;MOSAIC (ANTIGA - VALE)&lt;/xFant&gt;&lt;fone&gt;01333699194&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;RODOVIA BR 116 KM 488,5&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;COMPLEXO INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3509254&lt;/cMun&gt;&lt;xMun&gt;CAJATI&lt;/xMun&gt;&lt;CEP&gt;11950000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;exped&gt;&lt;CNPJ&gt;02476026000802&lt;/CNPJ&gt;&lt;IE&gt;633174875112&lt;/IE&gt;&lt;xNome&gt;ULTRAFERTIL SA&lt;/xNome&gt;&lt;fone&gt;01300000000&lt;/fone&gt;&lt;enderExped&gt;&lt;xLgr&gt;ROD SP 55 CUBATAO GUARUJA&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xCpl&gt;KM 65,8&lt;/xCpl&gt;&lt;xBairro&gt;ILHA DO CARDOSO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;CEP&gt;11015147&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderExped&gt;&lt;/exped&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604017581&lt;/CNPJ&gt;&lt;IE&gt;513157609112&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;fone&gt;05132301300&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AVENIDA PROFESSOR BENEDICTO MONTENEGRO&lt;/xLgr&gt;&lt;nro&gt;1300&lt;/nro&gt;&lt;xBairro&gt;BETEL&lt;/xBairro&gt;&lt;cMun&gt;3536505&lt;/cMun&gt;&lt;xMun&gt;PAULINIA&lt;/xMun&gt;&lt;CEP&gt;13148908&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;email&gt;FISCAL@YARA.COM&lt;/email&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;2711.04&lt;/vTPrest&gt;&lt;vRec&gt;2711.04&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;2546.54&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;164.50&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;250.77&lt;/vTotTrib&gt;&lt;infAdFisco&gt;ICMS DIFERIDO CONFORME ARTIGO 358 DO RICMS&lt;/infAdFisco&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;47442.85&lt;/vCarga&gt;&lt;proPred&gt;ENXOFRE F IMP.&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;35300.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;35.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;47442.85&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35210833931486000564550040000805401453515100&lt;/chave&gt;&lt;dPrev&gt;2021-08-02&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35210850505924000118570010002698471002698478&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35210850505924000118570010002698471002698478"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;FjTwnQk+zqdQPNGgogQzWle6qOk=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;Gegg+HmLBI+2xsWF8vNfTRLzMTe3IBwSXoRRq243QWMBxk4zvWtZilaV0JIyeR5/V/CFnw0cX+V5BmjIAVNY2ETDY5duDfHOccpQ2R+FlDP/IbBHHhpMvodyPdzC2/6FN3VifLb7lpVGZP4GWczGDmC3QrbVaGEz+itr2Ft64XJnmparXe+H3DCJGMDQEp5HpO3oSkzEViotQ8GRjbO10NODsZRkqXRDTJzw+jlH+vDvIn6hegXkYARV2G4yskj7+FJth5xUsEgH1nammojcLM0KEWkd77KGGzBfChQtEYFjUSqv97z2lar9HpQQSj70ZrV4MDHuZqYFSeTwnifvIQ==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIH3TCCBcWgAwIBAgIQGTE263Ik9NKZRTDnjnNARTANBgkqhkiG9w0BAQsFADB0MQswCQYDVQQGEwJCUjETMBEGA1UEChMKSUNQLUJyYXNpbDEtMCsGA1UECxMkQ2VydGlzaWduIENlcnRpZmljYWRvcmEgRGlnaXRhbCBTLkEuMSEwHwYDVQQDExhBQyBDZXJ0aXNpZ24gTXVsdGlwbGEgRzcwHhcNMjAwOTE2MTMzMjQ0WhcNMjEwOTE2MTMzMjQ0WjCBtzELMAkGA1UEBhMCQlIxEzARBgNVBAoMCklDUC1CcmFzaWwxHjAcBgNVBAsMFUFDIENlcnRpc2lnbiBNdWx0aXBsYTEXMBUGA1UECwwOMDA2NzkxNjMwMDAxNDIxGTAXBgNVBAsMEFZpZGVvQ29uZmVyZW5jaWExGzAZBgNVBAsMEkFzc2luYXR1cmEgVGlwbyBBMTEiMCAGA1UEAwwZVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMpHApL9xwNbYn1XdRkSLAdU22065w86ws9GVmg/DyCEuIikdIynnZ8sF/HR+mtlYnk4R6oVMk3zj3DGq0fN7XEY/btbFYz8ihosZKY3OtpMBnj3XYvz9h/PioYczNOb+RUq/QlxaAfkfRWuknZw3aMxbk7qBYG+Hqp6VyD5psRJgJ1hFIcanCl2TPazhN9kQbd+a/t5ykf1wRsaEvXsdMZMc4ym/PP+V0SebCGufWAKbDkrfM1orTPM7gG6nOBO9K31iwIVe4fLgzOyFBpbHRSsPcvqewPWNNhDMiesq+w9welta6ZtbWET4TSoXGO+BAs7mKMjfiVl22VBcx3/5TMCAwEAAaOCAyUwggMhMIGzBgNVHREEgaswgaigPQYFYEwBAwSgNAQyMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDEzNzQ1MTA2U1NQU1CgHAYFYEwBAwKgEwQRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEAQONTA1MDU5MjQwMDAxMTigFwYFYEwBAwegDgQMMDAwMDAwMDAwMDAwgRVGSVNDQUxAUk9ET1RBQy5ORVQuQlIwCQYDVR0TBAIwADAfBgNVHSMEGDAWgBRdcgy/M9K744am6EwGcX5VXAeg1jCBiwYDVR0gBIGDMIGAMH4GBmBMAQIBCzB0MHIGCCsGAQUFBwIBFmZodHRwOi8vaWNwLWJyYXNpbC5jZXJ0aXNpZ24uY29tLmJyL3JlcG9zaXRvcmlvL2RwYy9BQ19DZXJ0aXNpZ25fTXVsdGlwbGEvRFBDX0FDX0NlcnRpU2lnbl9NdWx0aXBsYS5wZGYwgcYGA1UdHwSBvjCBuzBcoFqgWIZWaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9sY3IvQUNDZXJ0aXNpZ25NdWx0aXBsYUc3L0xhdGVzdENSTC5jcmwwW6BZoFeGVWh0dHA6Ly9pY3AtYnJhc2lsLm91dHJhbGNyLmNvbS5ici9yZXBvc2l0b3Jpby9sY3IvQUNDZXJ0aXNpZ25NdWx0aXBsYUc3L0xhdGVzdENSTC5jcmwwDgYDVR0PAQH/BAQDAgXgMB0GA1UdJQQWMBQGCCsGAQUFBwMCBggrBgEFBQcDBDCBtgYIKwYBBQUHAQEEgakwgaYwZAYIKwYBBQUHMAKGWGh0dHA6Ly9pY3AtYnJhc2lsLmNlcnRpc2lnbi5jb20uYnIvcmVwb3NpdG9yaW8vY2VydGlmaWNhZG9zL0FDX0NlcnRpc2lnbl9NdWx0aXBsYV9HNy5wN2MwPgYIKwYBBQUHMAGGMmh0dHA6Ly9vY3NwLWFjLWNlcnRpc2lnbi1tdWx0aXBsYS5jZXJ0aXNpZ24uY29tLmJyMA0GCSqGSIb3DQEBCwUAA4ICAQCgj3CKNy5kS3l7YcSbmGEHrx+/f2rCMs4k/cADprWHmj6T6B2Q/BXXCKSQWxxvKJCz7S3IADGhijD9L1bJgqbBEvejJQ7ckUtVfTbuwdY2S/rhr8sMWHev1lVEfDhYQ5z596OH9/Gt/UEipg5oCqVTI2VUbha0Gf1ve9VQxoUyDwGLTohyczmCVORFcfRDga/EyHeM5MMAbRHm9KFaemv16uagkLX7cVp/qEo7QDQ7DM06Pq2tE2cB+LCsZ3x75zfTH24lHJV7jEN56FeKvlH7U+s3VOdoN7PT0f/OcHREAmTKF1TGxnmd8XdwxDj4HGP0XM5y8M0bh2iPoZLwFidq6jwTirOklMSmgSBlf4/D0q6cpq06EgbIdVw202MzVghUy9RYRN8xqtOhT3ltJapvoFX4YJNgVZ/zA3SHZVDAkECIEPU1/tt8hxRd4T8h2r8Dubw3H2YR/qNNwrlxx+0Lb2V8O7En26WNmwn1na/DXgLpt8KNFosfBLyHkY0TNCEJUxWMaPweb/wfvmV43cFOHsheR8h9Vf/LxJuR8Mv9zPDPSo+HSAhLwywRYY5kKGEtkwjRx4abxnoyfChMFtxSuIUArAXcyVaIF80qmSAiNEifKNnV7Vrct5JtvmrdbQf+HaS3/toF7fUhUPGfsw799JD0Efua/uEb+J+/a1qJQg==&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-05-21-1&lt;/verAplic&gt;&lt;chCTe&gt;35210850505924000118570010002698471002698478&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-08-01T16:00:28-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214019963795&lt;/nProt&gt;&lt;digVal&gt;FjTwnQk+zqdQPNGgogQzWle6qOk=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35210850505924000118570010002729211002729218-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35210850505924000118570010002729211002729218-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35210850505924000118570010002729211002729218"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00272921&lt;/cCT&gt;&lt;CFOP&gt;5352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;272921&lt;/nCT&gt;&lt;dhEmi&gt;2021-08-25T17:40:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;8&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3545159&lt;/cMunIni&gt;&lt;xMunIni&gt;SALTINHO&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3518602&lt;/cMunFim&gt;&lt;xMunFim&gt;GUARIBA&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;0&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;JOAO VICTOR FUREGATO&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;NHO&lt;/xOrig&gt;&lt;xDest&gt;GRB&lt;/xDest&gt;&lt;xRota&gt;NHOGRB&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SALTINHO&lt;/origCalc&gt;&lt;destCalc&gt;GUARIBA&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 212,94;ESTADIA APOS 24 HRS SEM RETROACAO.COOP.: MANOEL DA SILVA CARNEIRO Referencia do Cliente : FRETE 48,00 - DESCARGA MANOEL DA SILVA C;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;C0467&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;FRETE 48,00 - DESCARGA MANOEL DA SILVA C&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;48.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;RAIMUNDO NONATO GOMES DE CASSIA&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;993.935.573-49&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;GJG2355&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;GGS2514&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FMP5856&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FGZ-0695&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;16925334000106&lt;/CNPJ&gt;&lt;IE&gt;759008096119&lt;/IE&gt;&lt;xNome&gt;M G MINERACAO DE CALCARIO LTDA&lt;/xNome&gt;&lt;xFant&gt;M  G MINERACAO&lt;/xFant&gt;&lt;fone&gt;01934391212&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;RODOVIA SP 127 KM 57,3&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;RURAL&lt;/xBairro&gt;&lt;cMun&gt;3545159&lt;/cMun&gt;&lt;xMun&gt;SALTINHO&lt;/xMun&gt;&lt;CEP&gt;13440000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;48662175000190&lt;/CNPJ&gt;&lt;IE&gt;334001401117&lt;/IE&gt;&lt;xNome&gt;COPLANA - COOPERATIVA AGROINDUSTRIAL&lt;/xNome&gt;&lt;fone&gt;01632519200&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AVENIDA ANTONIO ALBINO&lt;/xLgr&gt;&lt;nro&gt;1640&lt;/nro&gt;&lt;xBairro&gt;VILA GARAVELLO&lt;/xBairro&gt;&lt;cMun&gt;3518602&lt;/cMun&gt;&lt;xMun&gt;GUARIBA&lt;/xMun&gt;&lt;CEP&gt;14840000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;2302.08&lt;/vTPrest&gt;&lt;vRec&gt;2302.08&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;1858.38&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;443.70&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;212.94&lt;/vTotTrib&gt;&lt;infAdFisco&gt;ICMS DIFERIDO CONFORME ARTIGO 358 DO RICMS&lt;/infAdFisco&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;3357.20&lt;/vCarga&gt;&lt;proPred&gt;CALCARIO&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;47960.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;0.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;3357.20&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35210816925334000106550010000922661111721091&lt;/chave&gt;&lt;dPrev&gt;2021-08-25&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-08-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35210850505924000118570010002729211002729218&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35210850505924000118570010002729211002729218"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;NbVe988p69NFBLQuX8VbWBpW9y8=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;XpGWhaCpB1r4mTqnCz3dFXTu3TtaeNW26+Mv/SYOd7Iwkpakydu8b3UGbJcOrQXxjtoR3Hama5CMWjPuedmhVGteLEgUhiHIxF4FtP1b01vMLI4wL2ZWVeSto5wqLTVRCgtZ2OiVuVH5XLKsGoreFkjw8Wth5CT8Jqk1YyxUaHDWZnAutA6T91uWecUjgTb8jAykph1VcNC7otwQSc8pSAfhFT55chi0fJAU8q7xKjSHw7twPiul02DHLC5gvOzTElWy98nA0GvBWrn+KOsskFmtaWUsS3dSDGuFeku7Dn6V5G3XCDVYJTNduhPkubuKt76EhoadL00tbz8o1jN8bA==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIH3TCCBcWgAwIBAgIQGTE263Ik9NKZRTDnjnNARTANBgkqhkiG9w0BAQsFADB0MQswCQYDVQQGEwJCUjETMBEGA1UEChMKSUNQLUJyYXNpbDEtMCsGA1UECxMkQ2VydGlzaWduIENlcnRpZmljYWRvcmEgRGlnaXRhbCBTLkEuMSEwHwYDVQQDExhBQyBDZXJ0aXNpZ24gTXVsdGlwbGEgRzcwHhcNMjAwOTE2MTMzMjQ0WhcNMjEwOTE2MTMzMjQ0WjCBtzELMAkGA1UEBhMCQlIxEzARBgNVBAoMCklDUC1CcmFzaWwxHjAcBgNVBAsMFUFDIENlcnRpc2lnbiBNdWx0aXBsYTEXMBUGA1UECwwOMDA2NzkxNjMwMDAxNDIxGTAXBgNVBAsMEFZpZGVvQ29uZmVyZW5jaWExGzAZBgNVBAsMEkFzc2luYXR1cmEgVGlwbyBBMTEiMCAGA1UEAwwZVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMpHApL9xwNbYn1XdRkSLAdU22065w86ws9GVmg/DyCEuIikdIynnZ8sF/HR+mtlYnk4R6oVMk3zj3DGq0fN7XEY/btbFYz8ihosZKY3OtpMBnj3XYvz9h/PioYczNOb+RUq/QlxaAfkfRWuknZw3aMxbk7qBYG+Hqp6VyD5psRJgJ1hFIcanCl2TPazhN9kQbd+a/t5ykf1wRsaEvXsdMZMc4ym/PP+V0SebCGufWAKbDkrfM1orTPM7gG6nOBO9K31iwIVe4fLgzOyFBpbHRSsPcvqewPWNNhDMiesq+w9welta6ZtbWET4TSoXGO+BAs7mKMjfiVl22VBcx3/5TMCAwEAAaOCAyUwggMhMIGzBgNVHREEgaswgaigPQYFYEwBAwSgNAQyMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDEzNzQ1MTA2U1NQU1CgHAYFYEwBAwKgEwQRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEAQONTA1MDU5MjQwMDAxMTigFwYFYEwBAwegDgQMMDAwMDAwMDAwMDAwgRVGSVNDQUxAUk9ET1RBQy5ORVQuQlIwCQYDVR0TBAIwADAfBgNVHSMEGDAWgBRdcgy/M9K744am6EwGcX5VXAeg1jCBiwYDVR0gBIGDMIGAMH4GBmBMAQIBCzB0MHIGCCsGAQUFBwIBFmZodHRwOi8vaWNwLWJyYXNpbC5jZXJ0aXNpZ24uY29tLmJyL3JlcG9zaXRvcmlvL2RwYy9BQ19DZXJ0aXNpZ25fTXVsdGlwbGEvRFBDX0FDX0NlcnRpU2lnbl9NdWx0aXBsYS5wZGYwgcYGA1UdHwSBvjCBuzBcoFqgWIZWaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9sY3IvQUNDZXJ0aXNpZ25NdWx0aXBsYUc3L0xhdGVzdENSTC5jcmwwW6BZoFeGVWh0dHA6Ly9pY3AtYnJhc2lsLm91dHJhbGNyLmNvbS5ici9yZXBvc2l0b3Jpby9sY3IvQUNDZXJ0aXNpZ25NdWx0aXBsYUc3L0xhdGVzdENSTC5jcmwwDgYDVR0PAQH/BAQDAgXgMB0GA1UdJQQWMBQGCCsGAQUFBwMCBggrBgEFBQcDBDCBtgYIKwYBBQUHAQEEgakwgaYwZAYIKwYBBQUHMAKGWGh0dHA6Ly9pY3AtYnJhc2lsLmNlcnRpc2lnbi5jb20uYnIvcmVwb3NpdG9yaW8vY2VydGlmaWNhZG9zL0FDX0NlcnRpc2lnbl9NdWx0aXBsYV9HNy5wN2MwPgYIKwYBBQUHMAGGMmh0dHA6Ly9vY3NwLWFjLWNlcnRpc2lnbi1tdWx0aXBsYS5jZXJ0aXNpZ24uY29tLmJyMA0GCSqGSIb3DQEBCwUAA4ICAQCgj3CKNy5kS3l7YcSbmGEHrx+/f2rCMs4k/cADprWHmj6T6B2Q/BXXCKSQWxxvKJCz7S3IADGhijD9L1bJgqbBEvejJQ7ckUtVfTbuwdY2S/rhr8sMWHev1lVEfDhYQ5z596OH9/Gt/UEipg5oCqVTI2VUbha0Gf1ve9VQxoUyDwGLTohyczmCVORFcfRDga/EyHeM5MMAbRHm9KFaemv16uagkLX7cVp/qEo7QDQ7DM06Pq2tE2cB+LCsZ3x75zfTH24lHJV7jEN56FeKvlH7U+s3VOdoN7PT0f/OcHREAmTKF1TGxnmd8XdwxDj4HGP0XM5y8M0bh2iPoZLwFidq6jwTirOklMSmgSBlf4/D0q6cpq06EgbIdVw202MzVghUy9RYRN8xqtOhT3ltJapvoFX4YJNgVZ/zA3SHZVDAkECIEPU1/tt8hxRd4T8h2r8Dubw3H2YR/qNNwrlxx+0Lb2V8O7En26WNmwn1na/DXgLpt8KNFosfBLyHkY0TNCEJUxWMaPweb/wfvmV43cFOHsheR8h9Vf/LxJuR8Mv9zPDPSo+HSAhLwywRYY5kKGEtkwjRx4abxnoyfChMFtxSuIUArAXcyVaIF80qmSAiNEifKNnV7Vrct5JtvmrdbQf+HaS3/toF7fUhUPGfsw799JD0Efua/uEb+J+/a1qJQg==&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35210850505924000118570010002729211002729218&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-08-25T17:42:16-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214135237155&lt;/nProt&gt;&lt;digVal&gt;NbVe988p69NFBLQuX8VbWBpW9y8=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35210950505924000118570010002738851002738853-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35210950505924000118570010002738851002738853-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35210950505924000118570010002738851002738853"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00273885&lt;/cCT&gt;&lt;CFOP&gt;1206&lt;/CFOP&gt;&lt;natOp&gt;ANULACAO DE VR REF PRESTACAO SERV DE TRANSPORTE&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;273885&lt;/nCT&gt;&lt;dhEmi&gt;2021-09-03T16:04:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;3&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;2&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3545159&lt;/cMunIni&gt;&lt;xMunIni&gt;SALTINHO&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3518602&lt;/cMunFim&gt;&lt;xMunFim&gt;GUARIBA&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;0&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Anulacao&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;NHO&lt;/xOrig&gt;&lt;xDest&gt;GRB&lt;/xDest&gt;&lt;xRota&gt;NHOGRB&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SALTINHO&lt;/origCalc&gt;&lt;destCalc&gt;GUARIBA&lt;/destCalc&gt;&lt;xObs&gt;ANULACAO DE VALOR RELATIVO A PRESTACAO DE SERVICO DE TRANSPORTE REF. AO CT-e 272921 DO DIA 25/08/2021. CONFORME EVENTO DE RECUSA DO TOMADOR M G MINERACAO DE CALCARIO LTDA - CPJ:16.925.334/0001-06.&lt;/xObs&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;RAIMUNDO NONATO GOMES DE CASSIA&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;993.935.573-49&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;GJG2355&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;GGS2514&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FMP5856&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FGZ-0695&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;16925334000106&lt;/CNPJ&gt;&lt;IE&gt;759008096119&lt;/IE&gt;&lt;xNome&gt;M G MINERACAO DE CALCARIO LTDA&lt;/xNome&gt;&lt;xFant&gt;M  G MINERACAO&lt;/xFant&gt;&lt;fone&gt;01934391212&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;RODOVIA SP 127 KM 57,3&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;RURAL&lt;/xBairro&gt;&lt;cMun&gt;3545159&lt;/cMun&gt;&lt;xMun&gt;SALTINHO&lt;/xMun&gt;&lt;CEP&gt;13440000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;48662175000190&lt;/CNPJ&gt;&lt;IE&gt;334001401117&lt;/IE&gt;&lt;xNome&gt;COPLANA - COOPERATIVA AGROINDUSTRIAL&lt;/xNome&gt;&lt;fone&gt;01632519200&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AVENIDA ANTONIO ALBINO&lt;/xLgr&gt;&lt;nro&gt;1640&lt;/nro&gt;&lt;xBairro&gt;VILA GARAVELLO&lt;/xBairro&gt;&lt;cMun&gt;3518602&lt;/cMun&gt;&lt;xMun&gt;GUARIBA&lt;/xMun&gt;&lt;CEP&gt;14840000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;2302.08&lt;/vTPrest&gt;&lt;vRec&gt;2302.08&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;1858.38&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;443.70&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;212.94&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCteAnu&gt;&lt;chCte&gt;35210850505924000118570010002729211002729218&lt;/chCte&gt;&lt;dEmi&gt;2021-09-03&lt;/dEmi&gt;&lt;/infCteAnu&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35210950505924000118570010002738851002738853&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35210950505924000118570010002738851002738853"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;s/XhGvAr9OTHcum4c67oJDf8I3U=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;FEKv6RWtUEfi2+7Cg9rnT7cvLk+MwcovJwISsFi28gRnV6sKI3bwv3Y+fEza8yGz6B06D59SFVmWCP55zBHZWqV8SpWxeBTYvWs+ql33YELQjdx3DLr8gX5syYcwAqI3riwVx7YBch74taxzm6z+g5rtT6WkKFkKUWlAYpvZ7yXjpiwP3L4VujB1UK1hwwpHbZslGG1lkVHX6dttJpm/QwVWJjWFPWBH/4cIqjGhqO3o/5ehs8OwvelIeKNe55s9w3w7iDR1NVolN/aufFAcDl8FYb4IHU9n4fBqRji6mH6DK5t327vuiy2bMU7n1SpRYEQdNbA8poLInVQ4hVJuGw==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIH3TCCBcWgAwIBAgIQGTE263Ik9NKZRTDnjnNARTANBgkqhkiG9w0BAQsFADB0MQswCQYDVQQGEwJCUjETMBEGA1UEChMKSUNQLUJyYXNpbDEtMCsGA1UECxMkQ2VydGlzaWduIENlcnRpZmljYWRvcmEgRGlnaXRhbCBTLkEuMSEwHwYDVQQDExhBQyBDZXJ0aXNpZ24gTXVsdGlwbGEgRzcwHhcNMjAwOTE2MTMzMjQ0WhcNMjEwOTE2MTMzMjQ0WjCBtzELMAkGA1UEBhMCQlIxEzARBgNVBAoMCklDUC1CcmFzaWwxHjAcBgNVBAsMFUFDIENlcnRpc2lnbiBNdWx0aXBsYTEXMBUGA1UECwwOMDA2NzkxNjMwMDAxNDIxGTAXBgNVBAsMEFZpZGVvQ29uZmVyZW5jaWExGzAZBgNVBAsMEkFzc2luYXR1cmEgVGlwbyBBMTEiMCAGA1UEAwwZVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMpHApL9xwNbYn1XdRkSLAdU22065w86ws9GVmg/DyCEuIikdIynnZ8sF/HR+mtlYnk4R6oVMk3zj3DGq0fN7XEY/btbFYz8ihosZKY3OtpMBnj3XYvz9h/PioYczNOb+RUq/QlxaAfkfRWuknZw3aMxbk7qBYG+Hqp6VyD5psRJgJ1hFIcanCl2TPazhN9kQbd+a/t5ykf1wRsaEvXsdMZMc4ym/PP+V0SebCGufWAKbDkrfM1orTPM7gG6nOBO9K31iwIVe4fLgzOyFBpbHRSsPcvqewPWNNhDMiesq+w9welta6ZtbWET4TSoXGO+BAs7mKMjfiVl22VBcx3/5TMCAwEAAaOCAyUwggMhMIGzBgNVHREEgaswgaigPQYFYEwBAwSgNAQyMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDEzNzQ1MTA2U1NQU1CgHAYFYEwBAwKgEwQRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEAQONTA1MDU5MjQwMDAxMTigFwYFYEwBAwegDgQMMDAwMDAwMDAwMDAwgRVGSVNDQUxAUk9ET1RBQy5ORVQuQlIwCQYDVR0TBAIwADAfBgNVHSMEGDAWgBRdcgy/M9K744am6EwGcX5VXAeg1jCBiwYDVR0gBIGDMIGAMH4GBmBMAQIBCzB0MHIGCCsGAQUFBwIBFmZodHRwOi8vaWNwLWJyYXNpbC5jZXJ0aXNpZ24uY29tLmJyL3JlcG9zaXRvcmlvL2RwYy9BQ19DZXJ0aXNpZ25fTXVsdGlwbGEvRFBDX0FDX0NlcnRpU2lnbl9NdWx0aXBsYS5wZGYwgcYGA1UdHwSBvjCBuzBcoFqgWIZWaHR0cDovL2ljcC1icmFzaWwuY2VydGlzaWduLmNvbS5ici9yZXBvc2l0b3Jpby9sY3IvQUNDZXJ0aXNpZ25NdWx0aXBsYUc3L0xhdGVzdENSTC5jcmwwW6BZoFeGVWh0dHA6Ly9pY3AtYnJhc2lsLm91dHJhbGNyLmNvbS5ici9yZXBvc2l0b3Jpby9sY3IvQUNDZXJ0aXNpZ25NdWx0aXBsYUc3L0xhdGVzdENSTC5jcmwwDgYDVR0PAQH/BAQDAgXgMB0GA1UdJQQWMBQGCCsGAQUFBwMCBggrBgEFBQcDBDCBtgYIKwYBBQUHAQEEgakwgaYwZAYIKwYBBQUHMAKGWGh0dHA6Ly9pY3AtYnJhc2lsLmNlcnRpc2lnbi5jb20uYnIvcmVwb3NpdG9yaW8vY2VydGlmaWNhZG9zL0FDX0NlcnRpc2lnbl9NdWx0aXBsYV9HNy5wN2MwPgYIKwYBBQUHMAGGMmh0dHA6Ly9vY3NwLWFjLWNlcnRpc2lnbi1tdWx0aXBsYS5jZXJ0aXNpZ24uY29tLmJyMA0GCSqGSIb3DQEBCwUAA4ICAQCgj3CKNy5kS3l7YcSbmGEHrx+/f2rCMs4k/cADprWHmj6T6B2Q/BXXCKSQWxxvKJCz7S3IADGhijD9L1bJgqbBEvejJQ7ckUtVfTbuwdY2S/rhr8sMWHev1lVEfDhYQ5z596OH9/Gt/UEipg5oCqVTI2VUbha0Gf1ve9VQxoUyDwGLTohyczmCVORFcfRDga/EyHeM5MMAbRHm9KFaemv16uagkLX7cVp/qEo7QDQ7DM06Pq2tE2cB+LCsZ3x75zfTH24lHJV7jEN56FeKvlH7U+s3VOdoN7PT0f/OcHREAmTKF1TGxnmd8XdwxDj4HGP0XM5y8M0bh2iPoZLwFidq6jwTirOklMSmgSBlf4/D0q6cpq06EgbIdVw202MzVghUy9RYRN8xqtOhT3ltJapvoFX4YJNgVZ/zA3SHZVDAkECIEPU1/tt8hxRd4T8h2r8Dubw3H2YR/qNNwrlxx+0Lb2V8O7En26WNmwn1na/DXgLpt8KNFosfBLyHkY0TNCEJUxWMaPweb/wfvmV43cFOHsheR8h9Vf/LxJuR8Mv9zPDPSo+HSAhLwywRYY5kKGEtkwjRx4abxnoyfChMFtxSuIUArAXcyVaIF80qmSAiNEifKNnV7Vrct5JtvmrdbQf+HaS3/toF7fUhUPGfsw799JD0Efua/uEb+J+/a1qJQg==&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35210950505924000118570010002738851002738853&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-09-03T16:16:44-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214179467517&lt;/nProt&gt;&lt;digVal&gt;s/XhGvAr9OTHcum4c67oJDf8I3U=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35211050505924000118570010002782611002782613-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35211050505924000118570010002782611002782613-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211050505924000118570010002782611002782613"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00278261&lt;/cCT&gt;&lt;CFOP&gt;5352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;278261&lt;/nCT&gt;&lt;dhEmi&gt;2021-10-22T21:55:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;3&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3548500&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTOS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3552403&lt;/cMunFim&gt;&lt;xMunFim&gt;SUMARE&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;STS&lt;/xOrig&gt;&lt;xDest&gt;SUM&lt;/xDest&gt;&lt;xRota&gt;STSSUM&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTOS&lt;/origCalc&gt;&lt;destCalc&gt;SUMARE&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 465,42; Referencia do Cliente : 4500713253;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;C0541&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;4500713253&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;105.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;JOAQUIM CLAUDIO&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;047.602.508-75&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;EBX6139&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;EUP7E61&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;CFP2B93&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;ELY-5762&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;92660604015457&lt;/CNPJ&gt;&lt;IE&gt;3714585320678&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;xFant&gt;YARA BRASIL UBA4&lt;/xFant&gt;&lt;fone&gt;03433197198&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AV ANTONIO CARLOS GUILLAUMON&lt;/xLgr&gt;&lt;nro&gt;800&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044760&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;exped&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;xNome&gt;COMPANHIA DOCAS DO ESTADO DE SAO PAULO CODESP&lt;/xNome&gt;&lt;fone&gt;01300000000&lt;/fone&gt;&lt;enderExped&gt;&lt;xLgr&gt;CONSELHEIRO RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;CEP&gt;11015900&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderExped&gt;&lt;/exped&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604013756&lt;/CNPJ&gt;&lt;IE&gt;671143732119&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;fone&gt;011981959267&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV SAO JUDAS TADEU&lt;/xLgr&gt;&lt;nro&gt;880&lt;/nro&gt;&lt;xCpl&gt;SALA 1&lt;/xCpl&gt;&lt;xBairro&gt;JARDIM SAO JUDAS TADEU (NOVA VENEZA)&lt;/xBairro&gt;&lt;cMun&gt;3552403&lt;/cMun&gt;&lt;xMun&gt;SUMARE&lt;/xMun&gt;&lt;CEP&gt;13180570&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;5031.60&lt;/vTPrest&gt;&lt;vRec&gt;5031.60&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;4785.00&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;246.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;465.42&lt;/vTotTrib&gt;&lt;infAdFisco&gt;ICMS DIFERIDO CONFORME ARTIGO 358 DO RICMS&lt;/infAdFisco&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;102323.58&lt;/vCarga&gt;&lt;proPred&gt;FERTILIZANTE MINERAL SIMPLES CLORETO DE POTASSIO DE 60% DE K&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;47920.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;48.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;102323.58&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;31211092660604015457550760000146221569723315&lt;/chave&gt;&lt;dPrev&gt;2021-10-22&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-10-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211050505924000118570010002782611002782613&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211050505924000118570010002782611002782613"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;/evOzx/xi+u4SoQWMbSH7FqWqbc=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;juHyQQI3tpVVAWNOHzVr0AGbgNHHvhhZnLVUTDQRoCzYz3JfhqJWAdAKHaCgSG0tH3nkU+0ee1Mg7pzh7hFPfHBciv6CEvD+K9zAEf0Oj+AYUFjjIvN3NYwouB5tpRPeLTCvMGxN2IvkD0QheEv21am00mXfG4tY1JT7QE35oY8AH1iXlsxs/ajp8/lL7TxfVsb5DtMUvOMiJYh1WLP7r9uSDejd3JdZgzTqQ9KS+hJkbKe7NCR2qhJXfG1s3oLD7TcqvUlVbBsGnmiL8Mv9uy0ud1Djw3UJnPTC7m2wDjO4HeEZHAe7dUSrmmt24sa8xTBWOtAWekJrhbhV7Xh5lA==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211050505924000118570010002782611002782613&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-10-22T22:09:15-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214387286114&lt;/nProt&gt;&lt;digVal&gt;/evOzx/xi+u4SoQWMbSH7FqWqbc=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35211050505924000118570010002782621002782629-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35211050505924000118570010002782621002782629-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211050505924000118570010002782621002782629"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00278262&lt;/cCT&gt;&lt;CFOP&gt;5352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;278262&lt;/nCT&gt;&lt;dhEmi&gt;2021-10-22T22:11:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;9&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3548500&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTOS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3552403&lt;/cMunFim&gt;&lt;xMunFim&gt;SUMARE&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;JHONATAN FREIRE DOS&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;STS&lt;/xOrig&gt;&lt;xDest&gt;SUM&lt;/xDest&gt;&lt;xRota&gt;STSSUM&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTOS&lt;/origCalc&gt;&lt;destCalc&gt;SUMARE&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 466,59; Referencia do Cliente : 4500713253;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;C0272&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;4500713253&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;105.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;PAULO DOMINGOS SARANZO&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;981.204.178-87&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;FKH7H31&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FPE2F87&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FNT3C38&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FIJ-3I38&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;92660604015457&lt;/CNPJ&gt;&lt;IE&gt;3714585320678&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;xFant&gt;YARA BRASIL UBA4&lt;/xFant&gt;&lt;fone&gt;03433197198&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AV ANTONIO CARLOS GUILLAUMON&lt;/xLgr&gt;&lt;nro&gt;800&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044760&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;exped&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;xNome&gt;COMPANHIA DOCAS DO ESTADO DE SAO PAULO CODESP&lt;/xNome&gt;&lt;fone&gt;01300000000&lt;/fone&gt;&lt;enderExped&gt;&lt;xLgr&gt;CONSELHEIRO RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;CEP&gt;11015900&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderExped&gt;&lt;/exped&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604013756&lt;/CNPJ&gt;&lt;IE&gt;671143732119&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;fone&gt;011981959267&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV SAO JUDAS TADEU&lt;/xLgr&gt;&lt;nro&gt;880&lt;/nro&gt;&lt;xCpl&gt;SALA 1&lt;/xCpl&gt;&lt;xBairro&gt;JARDIM SAO JUDAS TADEU (NOVA VENEZA)&lt;/xBairro&gt;&lt;cMun&gt;3552403&lt;/cMun&gt;&lt;xMun&gt;SUMARE&lt;/xMun&gt;&lt;CEP&gt;13180570&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;5044.20&lt;/vTPrest&gt;&lt;vRec&gt;5044.20&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;4797.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;246.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;466.59&lt;/vTotTrib&gt;&lt;infAdFisco&gt;ICMS DIFERIDO CONFORME ARTIGO 358 DO RICMS&lt;/infAdFisco&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;102579.81&lt;/vCarga&gt;&lt;proPred&gt;FERTILIZANTE MINERAL SIMPLES CLORETO DE POTASSIO DE 60% DE K&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;48040.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;48.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;102579.81&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;31211092660604015457550760000146171184325883&lt;/chave&gt;&lt;dPrev&gt;2021-10-22&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-10-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211050505924000118570010002782621002782629&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211050505924000118570010002782621002782629"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;oNaY7I6lD3QJ91rtpJVwmvzw/Nc=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;DWvvNNEISJ+igJQiR3IYQ1jDzgdzWkuLfnDflIKNgbwcWvWehOD6Qyrs7NOMcrHefCHJyt5wd1RQ0oXBT2RzieiZvXDxvYZJwyegQqqJYwEOaKGohOzn/5e/XumvdBBg4CuNbyOGVsZfy3ivOKSpOAYMHGlEH9rpIAZUk5p8dMM+tiG4e/c459V5rjzWFXRCvSFpr4AHoeqldb/SrHJt1O13qW0JHW1Ku7DNoeLBj7zR+VmaKaQN5vQmg9hhDcc7OlUESjgX0yo3DNa+1rX0lKwOLlbM0558fU4xGImD+0lJAuwUeeEIxsINWXMncCR1Km4L62r3gmhZkSlJcD2EPQ==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211050505924000118570010002782621002782629&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-10-22T22:12:31-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214387299187&lt;/nProt&gt;&lt;digVal&gt;oNaY7I6lD3QJ91rtpJVwmvzw/Nc=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35211050505924000118570010002782671002782676-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35211050505924000118570010002782671002782676-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211050505924000118570010002782671002782676"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00278267&lt;/cCT&gt;&lt;CFOP&gt;5352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;278267&lt;/nCT&gt;&lt;dhEmi&gt;2021-10-23T00:08:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;6&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3548500&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTOS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3552403&lt;/cMunFim&gt;&lt;xMunFim&gt;SUMARE&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;LUIZ FELIPE NETTO DO&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;STS&lt;/xOrig&gt;&lt;xDest&gt;SUM&lt;/xDest&gt;&lt;xRota&gt;STSSUM&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTOS&lt;/origCalc&gt;&lt;destCalc&gt;SUMARE&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 465,52; Referencia do Cliente : 4500713253;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;C0537&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;4500713253&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;105.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;ANDERSON LUIS APARECIDO DOS PASSOS&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;138.634.038-35&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;FWX8247&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;EXF7334&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;ERH2076&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;EGJ-4985&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;92660604015457&lt;/CNPJ&gt;&lt;IE&gt;3714585320678&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;xFant&gt;YARA BRASIL UBA4&lt;/xFant&gt;&lt;fone&gt;03433197198&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AV ANTONIO CARLOS GUILLAUMON&lt;/xLgr&gt;&lt;nro&gt;800&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044760&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;exped&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;xNome&gt;COMPANHIA DOCAS DO ESTADO DE SAO PAULO CODESP&lt;/xNome&gt;&lt;fone&gt;01300000000&lt;/fone&gt;&lt;enderExped&gt;&lt;xLgr&gt;CONSELHEIRO RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;CEP&gt;11015900&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderExped&gt;&lt;/exped&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604013756&lt;/CNPJ&gt;&lt;IE&gt;671143732119&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;fone&gt;011981959267&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV SAO JUDAS TADEU&lt;/xLgr&gt;&lt;nro&gt;880&lt;/nro&gt;&lt;xCpl&gt;SALA 1&lt;/xCpl&gt;&lt;xBairro&gt;JARDIM SAO JUDAS TADEU (NOVA VENEZA)&lt;/xBairro&gt;&lt;cMun&gt;3552403&lt;/cMun&gt;&lt;xMun&gt;SUMARE&lt;/xMun&gt;&lt;CEP&gt;13180570&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;5032.65&lt;/vTPrest&gt;&lt;vRec&gt;5032.65&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;4786.05&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;246.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;465.52&lt;/vTotTrib&gt;&lt;infAdFisco&gt;ICMS DIFERIDO CONFORME ARTIGO 358 DO RICMS&lt;/infAdFisco&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;102344.93&lt;/vCarga&gt;&lt;proPred&gt;FERTILIZANTE MINERAL SIMPLES CLORETO DE POTASSIO DE 60% DE K&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;47930.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;48.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;102344.93&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;31211092660604015457550760000146311031134436&lt;/chave&gt;&lt;dPrev&gt;2021-10-23&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-10-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211050505924000118570010002782671002782676&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211050505924000118570010002782671002782676"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;YrIpBuxwJQQr6B7nt8X89961ZGQ=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;F+UpGCvYVHLUQO/G2miGGpx/CaJnYTrmZANxFAd/wgyaFfruaYcvLpkRZSLpleZa3tMNABHaeWAZzgibKiQLR2aNHtcwZcgg/XYjd+FsujJUE4NdDqmAaXZxjBAPt7zzhWDjU4N1oK7DumxBe/iai5NBrrvzyPHBpCakbcqpSbs+h+txl5nWgLyrfB9hVPEzvKMGD29Kdf2eQG+MqxLYzV+r1GS0+Wub7wATBD70HnuFOYTkKKYnrJURK3kMJJ9vnnqaCA1e7sQhDK5K/SLMbY0urQDkL+gp97x4YzpLYwimSibyJUxeaSJZmgGaO7aRBGQMiAxKaMVQlTqs00Y/bA==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211050505924000118570010002782671002782676&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-10-23T00:10:23-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214387595573&lt;/nProt&gt;&lt;digVal&gt;YrIpBuxwJQQr6B7nt8X89961ZGQ=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35211050505924000118570010002785081002785085-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35211050505924000118570010002785081002785085-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211050505924000118570010002785081002785085"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00278508&lt;/cCT&gt;&lt;CFOP&gt;5932&lt;/CFOP&gt;&lt;natOp&gt;PR.SERV.TRANSP.INIC.FORA ESTAD&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;278508&lt;/nCT&gt;&lt;dhEmi&gt;2021-10-26T10:18:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;5&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;5213806&lt;/cMunIni&gt;&lt;xMunIni&gt;MORRINHOS&lt;/xMunIni&gt;&lt;UFIni&gt;GO&lt;/UFIni&gt;&lt;cMunFim&gt;5206206&lt;/cMunFim&gt;&lt;xMunFim&gt;CRISTALINA&lt;/xMunFim&gt;&lt;UFFim&gt;GO&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;MOR&lt;/xOrig&gt;&lt;xDest&gt;C2A&lt;/xDest&gt;&lt;xRota&gt;MORC2A&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;MORRINHOS&lt;/origCalc&gt;&lt;destCalc&gt;CRISTALINA&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 163,24;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;C0256&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;80.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;JOAO CARLOS CHIQUETO DIAS&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;077.433.128-36&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;GHD3J81&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FZO9G07&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FLA8A69&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;GIK-5F98&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;88305859002101&lt;/CNPJ&gt;&lt;IE&gt;107857405&lt;/IE&gt;&lt;xNome&gt;NUTRIEN SOLUCOES AGRICOLAS LTDA&lt;/xNome&gt;&lt;xFant&gt;NUTRIEN MORRINHOS&lt;/xFant&gt;&lt;fone&gt;01532758780&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;VIA SECUNDARIA&lt;/xLgr&gt;&lt;nro&gt;8&lt;/nro&gt;&lt;xCpl&gt;QUADRA9 LOTE 7&lt;/xCpl&gt;&lt;xBairro&gt;DISTRITO AGROINDUSTRIAL DE MORRINHOS&lt;/xBairro&gt;&lt;cMun&gt;5213806&lt;/cMun&gt;&lt;xMun&gt;MORRINHOS&lt;/xMun&gt;&lt;CEP&gt;75650000&lt;/CEP&gt;&lt;UF&gt;GO&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;88305859002012&lt;/CNPJ&gt;&lt;IE&gt;107770857&lt;/IE&gt;&lt;xNome&gt;NUTRIEN SOLUCOES AGRICOLAS LTDA&lt;/xNome&gt;&lt;fone&gt;01532758780&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;RODOVIA BR 050 KM 104 S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;ZONA RURAL&lt;/xBairro&gt;&lt;cMun&gt;5206206&lt;/cMun&gt;&lt;xMun&gt;CRISTALINA&lt;/xMun&gt;&lt;CEP&gt;73850000&lt;/CEP&gt;&lt;UF&gt;GO&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;email&gt;ROBERTO.DAMIAO@NUTRIENAGSOLUTIONS.COM.BR&lt;/email&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;1764.80&lt;/vTPrest&gt;&lt;vRec&gt;1764.80&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;1764.80&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;163.24&lt;/vTotTrib&gt;&lt;infAdFisco&gt;ISENCAO DO ICMS CONF.RCTE - GO/1977 ANEXO IX, ART.7°, XLI&lt;/infAdFisco&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;63534.56&lt;/vCarga&gt;&lt;proPred&gt;UREIA GRANULADA&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;22060.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;0.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;63534.56&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;52211088305859002101550230000027711001975667&lt;/chave&gt;&lt;dPrev&gt;2021-10-26&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-10-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211050505924000118570010002785081002785085&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211050505924000118570010002785081002785085"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;QFzexdP2zmD8KlsZH7NlzkmSrFA=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;uyWf1xAl4MtJmCc0KIA1Ox/m4jmMJzWVxf1+jLJVXOEo0LuGQ9UpykqI3UxPI8aJJQmAGRsyOfB26ooDbz2X1S9MfAmz/Vl5NaiO/hkwKDjO2s96QR4VWbJkVatAFdrkQ3JWpJf43nJWhVg00BjlDeRsjA8+/IbB8r7/4cmsIESMhRw5PTABeYa3MQSIPSlo426nwt/PkmHC+/9mRCYuXGvWViLyHEc5+xTafMr9yS48XwJsc/u9f+ayCImgrLqBQBo82BrVMQ7IER4YyhDExvTpz9QrkagTXCKdCCSzVa53je9VoJqyu3VGYsr9OIn2MXGw9jrAFvQX7xe7uIjqCA==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211050505924000118570010002785081002785085&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-10-26T11:43:14-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214398262958&lt;/nProt&gt;&lt;digVal&gt;QFzexdP2zmD8KlsZH7NlzkmSrFA=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35211204400329000109570010000605251000605255-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35211204400329000109570010000605251000605255-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211204400329000109570010000605251000605255"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00060525&lt;/cCT&gt;&lt;CFOP&gt;5360&lt;/CFOP&gt;&lt;natOp&gt;PREST. SERV. TRANSP. A CONT. SUBST. EM REL. AO SERVICO&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;60525&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-22T15:00:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;5&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3517406&lt;/cMunEnv&gt;&lt;xMunEnv&gt;GUAIRA&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;1&lt;/tpServ&gt;&lt;cMunIni&gt;3513504&lt;/cMunIni&gt;&lt;xMunIni&gt;CUBATAO&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3525904&lt;/cMunFim&gt;&lt;xMunFim&gt;JUNDIAI&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma4&gt;&lt;toma&gt;4&lt;/toma&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB&lt;/xFant&gt;&lt;enderToma&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderToma&gt;&lt;/toma4&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Subcontratacao&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;CBT&lt;/xOrig&gt;&lt;xDest&gt;JND&lt;/xDest&gt;&lt;xRota&gt;CBTJND&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;CUBATAO&lt;/origCalc&gt;&lt;destCalc&gt;JUNDIAI&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 57,88;CT-e EMITIDO SOMENTE P/EFEITO DE COBRANCA, NAO INC.ICMS, CONF.INC I DO ART.205 DO RICMS/00 - SUBCONTRATADO POR TRANSMOB TRANSPORTE LTDA CNPJ:50.505.924/0001-18, N°282946 Referencia do Cliente : 1-282946-1;&lt;/xObs&gt;&lt;ObsCont xCampo="frotas"&gt;&lt;xTexto&gt;C0254&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_clientes"&gt;&lt;xTexto&gt;1-282946-1&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_tons"&gt;&lt;xTexto&gt;54.720000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;DIVANJIR DOS SANTOS&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;141.798.608-56&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;EGG3H59&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FKM6A76&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FPZ2F54&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FPC-8J55&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;04400329000109&lt;/CNPJ&gt;&lt;IE&gt;322079785116&lt;/IE&gt;&lt;xNome&gt;RODOTAC TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;RODOTAC (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOAO JORGE GARCIA LEAL&lt;/xLgr&gt;&lt;nro&gt;607&lt;/nro&gt;&lt;xBairro&gt;PARQUE INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3517406&lt;/cMun&gt;&lt;xMun&gt;GUAIRA&lt;/xMun&gt;&lt;CEP&gt;14790000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733302455&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;06225292000147&lt;/CNPJ&gt;&lt;IE&gt;283108491118&lt;/IE&gt;&lt;xNome&gt;TERLOC - TERMINAL LOGISTICO CESARI LTDA&lt;/xNome&gt;&lt;xFant&gt;TERLOC- TER. CESARI.&lt;/xFant&gt;&lt;fone&gt;01321028013&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AV ENGENHEIRO PLINIO DE QUEIROZ S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xCpl&gt;SP 55&lt;/xCpl&gt;&lt;xBairro&gt;PIACAGUERA&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;CUBATAO&lt;/xMun&gt;&lt;CEP&gt;11570000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;44777951000147&lt;/CNPJ&gt;&lt;IE&gt;407401398115&lt;/IE&gt;&lt;xNome&gt;ADUFERTIL FERTILIZANTES LTDA&lt;/xNome&gt;&lt;fone&gt;01133795000&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV BETA&lt;/xLgr&gt;&lt;nro&gt;461&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3525904&lt;/cMun&gt;&lt;xMun&gt;JUNDIAI&lt;/xMun&gt;&lt;CEP&gt;13213070&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;1585.79&lt;/vTPrest&gt;&lt;vRec&gt;1585.79&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;1466.09&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;119.70&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;57.88&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;38151.01&lt;/vCarga&gt;&lt;proPred&gt;SAM GR&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;28980.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;1.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;38151.01&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35211206225292000147550010006105071012602148&lt;/chave&gt;&lt;dPrev&gt;2021-12-22&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;docAnt&gt;&lt;emiDocAnt&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;idDocAnt&gt;&lt;idDocAntEle&gt;&lt;chCTe&gt;35211250505924000118570010002829461002829461&lt;/chCTe&gt;&lt;/idDocAntEle&gt;&lt;/idDocAnt&gt;&lt;/emiDocAnt&gt;&lt;/docAnt&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;02625527&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211204400329000109570010000605251000605255&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211204400329000109570010000605251000605255"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;ldZIKwdkH5l4+jwFJltNZ9R/EWA=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;eADhsiTLaBYyXf9Ion+RkZALbH7rWRWDFDh1uK7zFcYSpIFQv9g4qcPq+f3nColFvTi9Lo/W4Zjd0Wd8K2Jg8BPmAOipskl73cm3ucC/q1SWb+tPeqWtN/KjMgeysdn2kF3YPmh6blQib1ptn4q0X3JezUPVD3CUHWvFV+VOVIUawC5TJ14CoKioY/dMFI2hg25NJPv8jDbgXBv+QAohMZVj+y5D/fTG9X4rZWa9Sfnq4D6AMluZAAlxkRHlh+Z4mE9X4DdhrSLUC31ms8ChqLlE3BsfIzLa7/3rvsO34VfsO268JbOP2eQupkGJhMaisrayTMGEWCdKZtuODU52xA==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHNzCCBR+gAwIBAgIIfFghCRNtqPgwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDIwMFoXDTIyMDkxNDEzNDIwMFowgdwxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDEPMA0GA1UEBxMGR3VhaXJhMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTEwMC4GA1UEAxMnUk9ET1RBQyBUUkFOU1BPUlRFUyBMVERBOjA0NDAwMzI5MDAwMTA5MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAp04ol/u6OamuPQYiuYvmBoabm9447ej3qfCk6KQY+gVddtzabeHC4yK1n9UOseY/2g2Wz2OQuVjZBz1mLb5aKDW9Hx4Hg4JXosEhRgHv+FxtlrgGJps+vVSke1fDiRKB9RxkryP5ngl3fOTaDXyXKAVw5Xir/ireILJkxoa7yItj3qOoX3WXO0e8IBBjeOJ3PyllIvh06I3LHaeqr6+hWxwuNsSxdYVLl+x0J5A1p8O+9MWEgTL6zEuST5aIoeESpEKC/oiOZwHujV8Zp6Ld3tbV45cNmE5qyq0Cv6WMxvySvmtBwBIS/2ftmk8dMnZb+R+iiO4Gh5gEFQ36XU3ezQIDAQABo4ICfTCCAnkwHwYDVR0jBBgwFoAUP9NcqRlN14gWLZgMrwre4U8kFrAwWQYIKwYBBQUHAQEETTBLMEkGCCsGAQUFBzAChj1odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUucDdiMIGvBgNVHREEgacwgaSBFnJvZG90YWNAcm9kb3RhYy5uZXQuYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMOMDQ0MDAzMjkwMDAxMDmgOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBTmf74GOUuAKM5iWH+pal5k4kRQYDAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAKffeE7P7VJywGR4dL48Nfq75Oa0zAPHLV/DXwo/bs847MeSBdauzpEiZ5xsUssJS/n73euRm/aaQ0Ai0fTYDcl6DAj0Bpn0kE3N9MF0/rb/35Ion/zwbhfzLHSby6MuH+NXvZheexyZV+LdWMnTY875AhHqFTLMH/e7TML3AukZFVrZDZ/KyjVGNji6XTmOxg0qt3hiEapOR+ODEqZO6FiYYS/7DGu+akrOzT8eOTddbUUzx2eZ6PctqSV7TZXTYtkfrq9pZgcFMjKUxwtnaQ9iE1ZttFTcVqIOWxPFLc/5pxFRfaFL+/5dhRs777Fox5nHBE9GjaI2alR9fidF4BJ+4UkcEZ17NaS8tzGYuP3XjieSWQD5eEAaGDA4eS+0zpNP6Z30UFqc5gmfj8EZaRuxaAUe+egORdxErP3J7CBPFEei/t1V/+E56JKHe75TgM+hTb+gxKyVThQULKZQgv/OiXD0O+cRBNHx0wNyvr/Srh61E9os66kg37kgfNZnMwBZOG4QmUtjJA5ChzJ99yXk6hNKhWXZrB+WwlBa2X/b/cff2nKx9wnw0ii3xjIAnkcWs2koAw5QaLUpNlHBTdTDVTMYZsXP9fSGKeom+/QDE6tZ5EstYiopzB2LRCGIB/PAwuYJX5fbcyMQTiu0A/6OCjQ3Bk9dK6myCbqSXJDb&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211204400329000109570010000605251000605255&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-22T15:15:56-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214662605292&lt;/nProt&gt;&lt;digVal&gt;ldZIKwdkH5l4+jwFJltNZ9R/EWA=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35211204400329000109570010000605261000605260-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35211204400329000109570010000605261000605260-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211204400329000109570010000605261000605260"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00060526&lt;/cCT&gt;&lt;CFOP&gt;5360&lt;/CFOP&gt;&lt;natOp&gt;PREST. SERV. TRANSP. A CONT. SUBST. EM REL. AO SERVICO&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;60526&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-22T15:00:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;0&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3517406&lt;/cMunEnv&gt;&lt;xMunEnv&gt;GUAIRA&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;1&lt;/tpServ&gt;&lt;cMunIni&gt;3513504&lt;/cMunIni&gt;&lt;xMunIni&gt;CUBATAO&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3525904&lt;/cMunFim&gt;&lt;xMunFim&gt;JUNDIAI&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma4&gt;&lt;toma&gt;4&lt;/toma&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB&lt;/xFant&gt;&lt;enderToma&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderToma&gt;&lt;/toma4&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Subcontratacao&lt;/xCaracAd&gt;&lt;xEmi&gt;CARLOS ALBERTO DA SI&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;CBT&lt;/xOrig&gt;&lt;xDest&gt;JND&lt;/xDest&gt;&lt;xRota&gt;CBTJND&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;CUBATAO&lt;/origCalc&gt;&lt;destCalc&gt;JUNDIAI&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 36,83;CT-e EMITIDO SOMENTE P/EFEITO DE COBRANCA, NAO INC.ICMS, CONF.INC I DO ART.205 DO RICMS/00 - SUBCONTRATADO POR TRANSMOB TRANSPORTE LTDA CNPJ:50.505.924/0001-18, N°282947 Referencia do Cliente : 1-282947-1;&lt;/xObs&gt;&lt;ObsCont xCampo="frotas"&gt;&lt;xTexto&gt;C0254&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_clientes"&gt;&lt;xTexto&gt;1-282947-1&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_tons"&gt;&lt;xTexto&gt;54.720000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;DIVANJIR DOS SANTOS&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;141.798.608-56&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;EGG3H59&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FKM6A76&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FPZ2F54&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FPC-8J55&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;04400329000109&lt;/CNPJ&gt;&lt;IE&gt;322079785116&lt;/IE&gt;&lt;xNome&gt;RODOTAC TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;RODOTAC (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOAO JORGE GARCIA LEAL&lt;/xLgr&gt;&lt;nro&gt;607&lt;/nro&gt;&lt;xBairro&gt;PARQUE INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3517406&lt;/cMun&gt;&lt;xMun&gt;GUAIRA&lt;/xMun&gt;&lt;CEP&gt;14790000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733302455&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;06225292000147&lt;/CNPJ&gt;&lt;IE&gt;283108491118&lt;/IE&gt;&lt;xNome&gt;TERLOC - TERMINAL LOGISTICO CESARI LTDA&lt;/xNome&gt;&lt;xFant&gt;TERLOC- TER. CESARI.&lt;/xFant&gt;&lt;fone&gt;01321028013&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AV ENGENHEIRO PLINIO DE QUEIROZ S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xCpl&gt;SP 55&lt;/xCpl&gt;&lt;xBairro&gt;PIACAGUERA&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;CUBATAO&lt;/xMun&gt;&lt;CEP&gt;11570000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;44777951000147&lt;/CNPJ&gt;&lt;IE&gt;407401398115&lt;/IE&gt;&lt;xNome&gt;ADUFERTIL FERTILIZANTES LTDA&lt;/xNome&gt;&lt;fone&gt;01133795000&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV BETA&lt;/xLgr&gt;&lt;nro&gt;461&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3525904&lt;/cMun&gt;&lt;xMun&gt;JUNDIAI&lt;/xMun&gt;&lt;CEP&gt;13213070&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;1009.04&lt;/vTPrest&gt;&lt;vRec&gt;1009.04&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;889.34&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;119.70&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;36.83&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;35637.14&lt;/vCarga&gt;&lt;proPred&gt;SAM GR&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;18440.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;1.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;35637.14&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35211206225292000147550010006105091012602193&lt;/chave&gt;&lt;dPrev&gt;2021-12-22&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;docAnt&gt;&lt;emiDocAnt&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;idDocAnt&gt;&lt;idDocAntEle&gt;&lt;chCTe&gt;35211250505924000118570010002829471002829477&lt;/chCTe&gt;&lt;/idDocAntEle&gt;&lt;/idDocAnt&gt;&lt;/emiDocAnt&gt;&lt;/docAnt&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;02625527&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211204400329000109570010000605261000605260&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211204400329000109570010000605261000605260"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;N6ZI6PhlhM7KefcSQzFkaQRVB2Q=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;TV1b+9J1j5bcOIK1Nj843UQJpIImTfsMw/K0G0dUZYTzS1dKtqexnRuy0vifPDlOJRczFdjmNgGI6ouEVOZWG8tKE9oCvKw6FGenun0g+CmcadV3nkdxvW0db0w6V+NeyDBdUnA1MRYV5Dt2IMbfpic7QZ2AF93UMQEuQFS31DBTQpyldMLKuaYF/HXoo4bfwE3yKX+0AyVyeYoztxJGWrGQL4OPo44ONx/JPJfYke8GOgqQzBIYLxFaiwNAuHVTarxclyjRRt+cB34swdWB5NH2xlsDbOgJfUmW7TjzE16ovjjHtjdlGGijvRnupXXgzo8w79O/JuWsJI4KgKD2Dg==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHNzCCBR+gAwIBAgIIfFghCRNtqPgwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDIwMFoXDTIyMDkxNDEzNDIwMFowgdwxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDEPMA0GA1UEBxMGR3VhaXJhMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTEwMC4GA1UEAxMnUk9ET1RBQyBUUkFOU1BPUlRFUyBMVERBOjA0NDAwMzI5MDAwMTA5MIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAp04ol/u6OamuPQYiuYvmBoabm9447ej3qfCk6KQY+gVddtzabeHC4yK1n9UOseY/2g2Wz2OQuVjZBz1mLb5aKDW9Hx4Hg4JXosEhRgHv+FxtlrgGJps+vVSke1fDiRKB9RxkryP5ngl3fOTaDXyXKAVw5Xir/ireILJkxoa7yItj3qOoX3WXO0e8IBBjeOJ3PyllIvh06I3LHaeqr6+hWxwuNsSxdYVLl+x0J5A1p8O+9MWEgTL6zEuST5aIoeESpEKC/oiOZwHujV8Zp6Ld3tbV45cNmE5qyq0Cv6WMxvySvmtBwBIS/2ftmk8dMnZb+R+iiO4Gh5gEFQ36XU3ezQIDAQABo4ICfTCCAnkwHwYDVR0jBBgwFoAUP9NcqRlN14gWLZgMrwre4U8kFrAwWQYIKwYBBQUHAQEETTBLMEkGCCsGAQUFBzAChj1odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUucDdiMIGvBgNVHREEgacwgaSBFnJvZG90YWNAcm9kb3RhYy5uZXQuYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMOMDQ0MDAzMjkwMDAxMDmgOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBTmf74GOUuAKM5iWH+pal5k4kRQYDAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAKffeE7P7VJywGR4dL48Nfq75Oa0zAPHLV/DXwo/bs847MeSBdauzpEiZ5xsUssJS/n73euRm/aaQ0Ai0fTYDcl6DAj0Bpn0kE3N9MF0/rb/35Ion/zwbhfzLHSby6MuH+NXvZheexyZV+LdWMnTY875AhHqFTLMH/e7TML3AukZFVrZDZ/KyjVGNji6XTmOxg0qt3hiEapOR+ODEqZO6FiYYS/7DGu+akrOzT8eOTddbUUzx2eZ6PctqSV7TZXTYtkfrq9pZgcFMjKUxwtnaQ9iE1ZttFTcVqIOWxPFLc/5pxFRfaFL+/5dhRs777Fox5nHBE9GjaI2alR9fidF4BJ+4UkcEZ17NaS8tzGYuP3XjieSWQD5eEAaGDA4eS+0zpNP6Z30UFqc5gmfj8EZaRuxaAUe+egORdxErP3J7CBPFEei/t1V/+E56JKHe75TgM+hTb+gxKyVThQULKZQgv/OiXD0O+cRBNHx0wNyvr/Srh61E9os66kg37kgfNZnMwBZOG4QmUtjJA5ChzJ99yXk6hNKhWXZrB+WwlBa2X/b/cff2nKx9wnw0ii3xjIAnkcWs2koAw5QaLUpNlHBTdTDVTMYZsXP9fSGKeom+/QDE6tZ5EstYiopzB2LRCGIB/PAwuYJX5fbcyMQTiu0A/6OCjQ3Bk9dK6myCbqSXJDb&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211204400329000109570010000605261000605260&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-22T15:15:58-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214662605521&lt;/nProt&gt;&lt;digVal&gt;N6ZI6PhlhM7KefcSQzFkaQRVB2Q=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35211250505924000118570010002829241002829243-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35211250505924000118570010002829241002829243-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211250505924000118570010002829241002829243"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00282924&lt;/cCT&gt;&lt;CFOP&gt;5352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;282924&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-19T21:59:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;3&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3548500&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTOS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3525904&lt;/cMunFim&gt;&lt;xMunFim&gt;JUNDIAI&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;Joao Maria de Mendon&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;STS&lt;/xOrig&gt;&lt;xDest&gt;JND&lt;/xDest&gt;&lt;xRota&gt;STSJND&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTOS&lt;/origCalc&gt;&lt;destCalc&gt;JUNDIAI&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 371,10; Referencia do Cliente : 202781021;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;EJW8394&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;202781021&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;88.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;LUIZ ROBERTO TASSANI&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;077.770.888-40&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;EJW8394&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;EJW8395&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;EJW8396&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;00000000000000&lt;/CNPJ&gt;&lt;IE&gt;ISENTO&lt;/IE&gt;&lt;xNome&gt;CANPOTEX LIMITED&lt;/xNome&gt;&lt;xFant&gt;CANPOTEX (COSTADO)&lt;/xFant&gt;&lt;fone&gt;01734445550&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AAAAAA&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;EXTERIOR&lt;/xBairro&gt;&lt;cMun&gt;9999999&lt;/cMun&gt;&lt;xMun&gt;EXTERIOR&lt;/xMun&gt;&lt;CEP&gt;00000000&lt;/CEP&gt;&lt;UF&gt;EX&lt;/UF&gt;&lt;cPais&gt;1490&lt;/cPais&gt;&lt;xPais&gt;CANADA&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;exped&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;xNome&gt;COMPANHIA DOCAS DO ESTADO DE SAO PAULO CODESP&lt;/xNome&gt;&lt;fone&gt;01300000000&lt;/fone&gt;&lt;enderExped&gt;&lt;xLgr&gt;CONSELHEIRO RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;CEP&gt;11015900&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderExped&gt;&lt;/exped&gt;&lt;dest&gt;&lt;CNPJ&gt;44777951000147&lt;/CNPJ&gt;&lt;IE&gt;407401398115&lt;/IE&gt;&lt;xNome&gt;ADUFERTIL FERTILIZANTES LTDA&lt;/xNome&gt;&lt;fone&gt;01133795000&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV BETA&lt;/xLgr&gt;&lt;nro&gt;461&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3525904&lt;/cMun&gt;&lt;xMun&gt;JUNDIAI&lt;/xMun&gt;&lt;CEP&gt;13213070&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;4011.92&lt;/vTPrest&gt;&lt;vRec&gt;4011.92&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;3876.82&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;135.10&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;371.11&lt;/vTotTrib&gt;&lt;infAdFisco&gt;ICMS DIFERIDO CONFORME ARTIGO 358 DO RICMS&lt;/infAdFisco&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;173917.19&lt;/vCarga&gt;&lt;proPred&gt;CLORETO DE POTASSIO 60% K2O GR&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;45590.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;46.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;173917.19&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35211244777951000147550100000493081425466807&lt;/chave&gt;&lt;dPrev&gt;2021-12-19&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211250505924000118570010002829241002829243&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211250505924000118570010002829241002829243"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;vi1LoYui2bDW9uAhgIkLxS3Mr8g=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;ITJYuc06bLq23J6MYegrDIVA7xSD98ardmRWimAqdRlCF53CL+0eUaG03auEUNgexxx20NhwJvFDfyeWA/OYdeE5DFNB82PALaFFbvjqL4Pp6sYYXwN3Fk/Okqg2sE/XBT5IlFs/nx8Jw6LM2RTTcap/hOeyXeHmGOOI9bpP5BXYjv5FxPblqfUHZFF0aPDNhcRuSc/qi9cM/BZ/z/7ErAkzaY5AQwa5OTtW1Ypmm6Lbwmn7ifsaAKZi6cADb1C4GFH8gf2v69reubb/LrM1/ca+CGFVOOtB0mqnDP2JnKwaEiJFmLXpXybGnyEZH+xbayIJhD8t1vwyGr1zl1ezpg==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211250505924000118570010002829241002829243&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-19T22:00:00-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214647612307&lt;/nProt&gt;&lt;digVal&gt;vi1LoYui2bDW9uAhgIkLxS3Mr8g=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35211250505924000118570010002829251002829259-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35211250505924000118570010002829251002829259-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211250505924000118570010002829251002829259"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00282925&lt;/cCT&gt;&lt;CFOP&gt;5352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;282925&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-19T22:42:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;9&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3548500&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTOS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3525904&lt;/cMunFim&gt;&lt;xMunFim&gt;JUNDIAI&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;LUIZ FELIPE NETTO DO&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;STS&lt;/xOrig&gt;&lt;xDest&gt;JND&lt;/xDest&gt;&lt;xRota&gt;STSJND&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTOS&lt;/origCalc&gt;&lt;destCalc&gt;JUNDIAI&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 224,50; Referencia do Cliente : 202781021;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;A0015&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;202781021&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;88.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;LUCIANO DA SILVA&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;195.087.408-76&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;EOE3080&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;EOE3031&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;EOE3033&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;EOE-3032&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;00000000000000&lt;/CNPJ&gt;&lt;IE&gt;ISENTO&lt;/IE&gt;&lt;xNome&gt;CANPOTEX LIMITED&lt;/xNome&gt;&lt;xFant&gt;CANPOTEX (COSTADO)&lt;/xFant&gt;&lt;fone&gt;01734445550&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AAAAAA&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;EXTERIOR&lt;/xBairro&gt;&lt;cMun&gt;9999999&lt;/cMun&gt;&lt;xMun&gt;EXTERIOR&lt;/xMun&gt;&lt;CEP&gt;00000000&lt;/CEP&gt;&lt;UF&gt;EX&lt;/UF&gt;&lt;cPais&gt;1490&lt;/cPais&gt;&lt;xPais&gt;CANADA&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;exped&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;xNome&gt;COMPANHIA DOCAS DO ESTADO DE SAO PAULO CODESP&lt;/xNome&gt;&lt;fone&gt;01300000000&lt;/fone&gt;&lt;enderExped&gt;&lt;xLgr&gt;CONSELHEIRO RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;CEP&gt;11015900&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderExped&gt;&lt;/exped&gt;&lt;dest&gt;&lt;CNPJ&gt;44777951000147&lt;/CNPJ&gt;&lt;IE&gt;407401398115&lt;/IE&gt;&lt;xNome&gt;ADUFERTIL FERTILIZANTES LTDA&lt;/xNome&gt;&lt;fone&gt;01133795000&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV BETA&lt;/xLgr&gt;&lt;nro&gt;461&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3525904&lt;/cMun&gt;&lt;xMun&gt;JUNDIAI&lt;/xMun&gt;&lt;CEP&gt;13213070&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;2427.04&lt;/vTPrest&gt;&lt;vRec&gt;2427.04&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;2253.34&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;173.70&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;224.51&lt;/vTotTrib&gt;&lt;infAdFisco&gt;ICMS DIFERIDO CONFORME ARTIGO 358 DO RICMS&lt;/infAdFisco&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;105212.46&lt;/vCarga&gt;&lt;proPred&gt;CLORETO DE POTASSIO 60% K2O GR&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;27580.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;28.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;105212.46&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35211244777951000147550100000493151560263484&lt;/chave&gt;&lt;dPrev&gt;2021-12-19&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211250505924000118570010002829251002829259&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211250505924000118570010002829251002829259"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;w5sz64Mgisb0MnyztuBJn0PK+ts=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;le79mbpPIjEQBJCqjf9JqKPpxcq/U8YZ7+0NrLnw9BC3VxBrdES9ZDQxr0HBRBz+BK+uqOJEdb7bYdq9UQpWLeZimLafqLPgX82I96tXLs3BqhgaFCBY5oGWWZRL+vOPai2gai+1l4Os15g1qN8SIBTQlxn03ONTnPW5/KAnBer9Bk1rNPC6gAsCWWQ5A+tDlDlQFhffYvVbm9t4XzfCFX3BWDAyX1nyWNp6ZAHOAiE6YCogRsqjh5bJQXMdpRZ5BRGAluwKgCGVpCFWMwznt8SZ7DVT6G9gzatydcKNP7Tdx5E9kXlVJylI8Hat2CjwDrWets0rqpdBKc1OjFYDUg==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211250505924000118570010002829251002829259&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-19T22:45:31-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214647705523&lt;/nProt&gt;&lt;digVal&gt;w5sz64Mgisb0MnyztuBJn0PK+ts=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35211250505924000118570010002829261002829264-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35211250505924000118570010002829261002829264-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211250505924000118570010002829261002829264"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00282926&lt;/cCT&gt;&lt;CFOP&gt;5352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;282926&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-19T22:44:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;4&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3548500&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTOS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3525904&lt;/cMunFim&gt;&lt;xMunFim&gt;JUNDIAI&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;LUIZ FELIPE NETTO DO&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;STS&lt;/xOrig&gt;&lt;xDest&gt;JND&lt;/xDest&gt;&lt;xRota&gt;STSJND&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTOS&lt;/origCalc&gt;&lt;destCalc&gt;JUNDIAI&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 227,59; Referencia do Cliente : 202781021;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;A0015&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;202781021&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;88.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;LUCIANO DA SILVA&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;195.087.408-76&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;EOE3080&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;EOE3031&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;EOE3033&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;EOE-3032&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;00000000000000&lt;/CNPJ&gt;&lt;IE&gt;ISENTO&lt;/IE&gt;&lt;xNome&gt;CANPOTEX LIMITED&lt;/xNome&gt;&lt;xFant&gt;CANPOTEX (COSTADO)&lt;/xFant&gt;&lt;fone&gt;01734445550&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AAAAAA&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;EXTERIOR&lt;/xBairro&gt;&lt;cMun&gt;9999999&lt;/cMun&gt;&lt;xMun&gt;EXTERIOR&lt;/xMun&gt;&lt;CEP&gt;00000000&lt;/CEP&gt;&lt;UF&gt;EX&lt;/UF&gt;&lt;cPais&gt;1490&lt;/cPais&gt;&lt;xPais&gt;CANADA&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;exped&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;xNome&gt;COMPANHIA DOCAS DO ESTADO DE SAO PAULO CODESP&lt;/xNome&gt;&lt;fone&gt;01300000000&lt;/fone&gt;&lt;enderExped&gt;&lt;xLgr&gt;CONSELHEIRO RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;CEP&gt;11015900&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderExped&gt;&lt;/exped&gt;&lt;dest&gt;&lt;CNPJ&gt;44777951000147&lt;/CNPJ&gt;&lt;IE&gt;407401398115&lt;/IE&gt;&lt;xNome&gt;ADUFERTIL FERTILIZANTES LTDA&lt;/xNome&gt;&lt;fone&gt;01133795000&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV BETA&lt;/xLgr&gt;&lt;nro&gt;461&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3525904&lt;/cMun&gt;&lt;xMun&gt;JUNDIAI&lt;/xMun&gt;&lt;CEP&gt;13213070&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;2460.48&lt;/vTPrest&gt;&lt;vRec&gt;2460.48&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;2286.78&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;173.70&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;227.60&lt;/vTotTrib&gt;&lt;infAdFisco&gt;ICMS DIFERIDO CONFORME ARTIGO 358 DO RICMS&lt;/infAdFisco&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;106662.09&lt;/vCarga&gt;&lt;proPred&gt;CLORETO DE POTASSIO 60% K2O GR&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;27960.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;28.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;106662.09&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35211244777951000147550100000493171454114270&lt;/chave&gt;&lt;dPrev&gt;2021-12-19&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211250505924000118570010002829261002829264&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211250505924000118570010002829261002829264"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;LrkpinZ74iOGCeaOg7EGgt59fF8=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;BY5GIIO7xkVSkoujtZI3IuM6/XbRUWUGRVeeuovI9d5ssOZi1k+7xL8pf1n7W2TTCQ4hwUiltWvw5TaSMPlkXeypHXIH+rfMnD5zzRVKfBkOmHW2Raikcg9G1yVYqfT+2Qjhc3ysVDKXLMra8ZBWhUREbhFFjIJHWqYXEbhIcJNwjVA1SZyPx8trQnF6om4w5OytvFPRzGnYpLWP3g8h95CNIwUbgIqh9zbOLSNTNyq0Gsj1Ay4zna+wKTQjv6cuE7g+0ERurNSpSaLv20hmfegxrhD4ZqgpnnQZetTwnU41VVBa9xab/HGkVvphgnA1T7KtresrvzReDlPDxrUd2A==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211250505924000118570010002829261002829264&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-19T22:45:33-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214647705594&lt;/nProt&gt;&lt;digVal&gt;LrkpinZ74iOGCeaOg7EGgt59fF8=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35211250505924000118570010002829291002829290-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35211250505924000118570010002829291002829290-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211250505924000118570010002829291002829290"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00282929&lt;/cCT&gt;&lt;CFOP&gt;5352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;282929&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-20T03:30:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;0&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3548500&lt;/cMunIni&gt;&lt;xMunIni&gt;SANTOS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3525904&lt;/cMunFim&gt;&lt;xMunFim&gt;JUNDIAI&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;Joao Maria de Mendon&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;STS&lt;/xOrig&gt;&lt;xDest&gt;JND&lt;/xDest&gt;&lt;xRota&gt;STSJND&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;SANTOS&lt;/origCalc&gt;&lt;destCalc&gt;JUNDIAI&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 347,09; Referencia do Cliente : 202781021;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;DAE8849&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;202781021&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;88.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;ROBERTO PEREIRA DE CARVALHO&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;269.940.968-58&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;DAE8849&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FYW3987&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;00000000000000&lt;/CNPJ&gt;&lt;IE&gt;ISENTO&lt;/IE&gt;&lt;xNome&gt;CANPOTEX LIMITED&lt;/xNome&gt;&lt;xFant&gt;CANPOTEX (COSTADO)&lt;/xFant&gt;&lt;fone&gt;01734445550&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AAAAAA&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;EXTERIOR&lt;/xBairro&gt;&lt;cMun&gt;9999999&lt;/cMun&gt;&lt;xMun&gt;EXTERIOR&lt;/xMun&gt;&lt;CEP&gt;00000000&lt;/CEP&gt;&lt;UF&gt;EX&lt;/UF&gt;&lt;cPais&gt;1490&lt;/cPais&gt;&lt;xPais&gt;CANADA&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;exped&gt;&lt;CNPJ&gt;44837524000107&lt;/CNPJ&gt;&lt;IE&gt;633123490119&lt;/IE&gt;&lt;xNome&gt;COMPANHIA DOCAS DO ESTADO DE SAO PAULO CODESP&lt;/xNome&gt;&lt;fone&gt;01300000000&lt;/fone&gt;&lt;enderExped&gt;&lt;xLgr&gt;CONSELHEIRO RODRIGUES ALVES&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xBairro&gt;MACUCO&lt;/xBairro&gt;&lt;cMun&gt;3548500&lt;/cMun&gt;&lt;xMun&gt;SANTOS&lt;/xMun&gt;&lt;CEP&gt;11015900&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderExped&gt;&lt;/exped&gt;&lt;dest&gt;&lt;CNPJ&gt;44777951000147&lt;/CNPJ&gt;&lt;IE&gt;407401398115&lt;/IE&gt;&lt;xNome&gt;ADUFERTIL FERTILIZANTES LTDA&lt;/xNome&gt;&lt;fone&gt;01133795000&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV BETA&lt;/xLgr&gt;&lt;nro&gt;461&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3525904&lt;/cMun&gt;&lt;xMun&gt;JUNDIAI&lt;/xMun&gt;&lt;CEP&gt;13213070&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;3752.32&lt;/vTPrest&gt;&lt;vRec&gt;3752.32&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;3617.22&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;135.10&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;OUTROSVALORES&lt;/xNome&gt;&lt;vComp&gt;0.00&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;347.09&lt;/vTotTrib&gt;&lt;infAdFisco&gt;ICMS DIFERIDO CONFORME ARTIGO 358 DO RICMS&lt;/infAdFisco&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;162663.50&lt;/vCarga&gt;&lt;proPred&gt;CLORETO DE POTASSIO 60% K2O GR&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;42640.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;43.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;162663.50&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35211244777951000147550100000493591660076613&lt;/chave&gt;&lt;dPrev&gt;2021-12-20&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211250505924000118570010002829291002829290&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211250505924000118570010002829291002829290"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;in1bu0lMFS2liMIgo55M+v1fcTQ=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;clF2N762qW+QcCibSGD6h7CW2/YibFTENKWAqzhJ8dGcZqfw6FIk9cO6yDL/owWgTlVuff1Q2AtkC+wm2VoGGHp71qUPIZetnuosjhD3PoLg2sR6uf9jIAuof8QWKUy4L989SqSuiOwKMFtrsvKqyoEHx/vMvIlMOJRm8BOyGDYd4MkoRKCVIwPwWBIuK4C1P1JtXV4Xvc6RPPgPhm6aV+Sq6uFQgmY7cmfl7xosreBvyiJyFvMSoa1sM1LILoDoQELMXgYY4hYO8UWeO7DaKX9Fmk52l0L3hlvxNldqTvrYQYw2WiCMAvioHONjXbN5a32Y332mLMOkxSh9zxj6cQ==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211250505924000118570010002829291002829290&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-20T03:31:11-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214648097685&lt;/nProt&gt;&lt;digVal&gt;in1bu0lMFS2liMIgo55M+v1fcTQ=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35211250505924000118570010002829411002829414-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35211250505924000118570010002829411002829414-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211250505924000118570010002829411002829414"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00282941&lt;/cCT&gt;&lt;CFOP&gt;5353&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/COMERCIO&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;282941&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-20T17:55:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;4&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3509502&lt;/cMunIni&gt;&lt;xMunIni&gt;CAMPINAS&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3539509&lt;/cMunFim&gt;&lt;xMunFim&gt;PITANGUEIRAS&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;DIEGO VITOR SOARES C&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;CPN&lt;/xOrig&gt;&lt;xDest&gt;PIT&lt;/xDest&gt;&lt;xRota&gt;CPNPIT&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;CAMPINAS&lt;/origCalc&gt;&lt;destCalc&gt;PITANGUEIRAS&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 389,61;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;A0022&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;75.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;JOAO BRUNO&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;100.211.638-47&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;GBG7I51&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FJX0A74&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FJX0A78&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;61560934000172&lt;/CNPJ&gt;&lt;IE&gt;244360928110&lt;/IE&gt;&lt;xNome&gt;COOP. CENT. FERTIL. COOPERFERTIL&lt;/xNome&gt;&lt;xFant&gt;COOPERFERTIL&lt;/xFant&gt;&lt;fone&gt;01932811181&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AV COMENDADOR ALADINO SELMI&lt;/xLgr&gt;&lt;nro&gt;4910&lt;/nro&gt;&lt;xBairro&gt;VILA SAN MARTIN&lt;/xBairro&gt;&lt;cMun&gt;3509502&lt;/cMun&gt;&lt;xMun&gt;CAMPINAS&lt;/xMun&gt;&lt;CEP&gt;13069096&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;06203812000110&lt;/CNPJ&gt;&lt;IE&gt;543023210112&lt;/IE&gt;&lt;xNome&gt;GT COMERCIO E SERVICOS AGRICOLAS LTDA - ME&lt;/xNome&gt;&lt;fone&gt;01639571427&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;HUM&lt;/xLgr&gt;&lt;nro&gt;307&lt;/nro&gt;&lt;xBairro&gt;PREDIO DISTRITO DE IBITIUVA&lt;/xBairro&gt;&lt;cMun&gt;3539509&lt;/cMun&gt;&lt;xMun&gt;PITANGUEIRAS&lt;/xMun&gt;&lt;CEP&gt;14760000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;4212.00&lt;/vTPrest&gt;&lt;vRec&gt;4212.00&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;3738.80&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;473.20&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;389.61&lt;/vTotTrib&gt;&lt;infAdFisco&gt;ICMS DIFERIDO CONFORME ARTIGO 358 DO RICMS&lt;/infAdFisco&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;16848.00&lt;/vCarga&gt;&lt;proPred&gt;VARREDURA&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;56160.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;0.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;16848.00&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35211261560934000172550040001973431125280004&lt;/chave&gt;&lt;dPrev&gt;2021-12-20&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211250505924000118570010002829411002829414&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211250505924000118570010002829411002829414"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;EVMZ/KsR+WCgjCL4fliEoNvxf4k=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;Kw3ps3o7OpjCeFMxqKX8zLNHDNDFvRdhF3vAf3T1yZT3yWlFAlCIKe8ZEFQRHuj4PMfJaquPyEqRbnYeIdshOcU8B0btjnkdB9Vxp6/Z7GbH1e5ne6DLmixCjY+mIO9Tlh0agyEfgthi+G2k3R432QHoESIconB75aupg0OldicFYW3NzBmbiNKIMLtY7aQKXfuZgE5kBtjk1zgnMP+0IJNWUeSZGixSVqsQ29uAMIiC7vo/lFaFnqY2w2KwHxr4RWQrJrq4rhl07N8ZMa1qm39BH13RmgPyUOSFUvYOZFVdyC90eMfIgtz2jPCkiOmZYZq0JUnpPgNfD5y55tsNLg==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211250505924000118570010002829411002829414&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-20T17:56:43-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214651899295&lt;/nProt&gt;&lt;digVal&gt;EVMZ/KsR+WCgjCL4fliEoNvxf4k=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35211250505924000118570010002829461002829461-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\35211250505924000118570010002829461002829461-ret-cons-cte.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211250505924000118570010002829461002829461"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00282946&lt;/cCT&gt;&lt;CFOP&gt;5352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;282946&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-20T20:54:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;1&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3513504&lt;/cMunIni&gt;&lt;xMunIni&gt;CUBATAO&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3525904&lt;/cMunFim&gt;&lt;xMunFim&gt;JUNDIAI&lt;/xMunFim&gt;&lt;UFFim&gt;SP&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;JHONATAN FREIRE DOS&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;CBT&lt;/xOrig&gt;&lt;xDest&gt;JND&lt;/xDest&gt;&lt;xRota&gt;CBTJND&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;CUBATAO&lt;/origCalc&gt;&lt;destCalc&gt;JUNDIAI&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 152,80;ESTADIA APOS 24 HRS SEM RETROACAO. Referencia do Cliente : 2420821;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;C0254&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;2420821&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;57.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;DIVANJIR DOS SANTOS&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;141.798.608-56&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;EGG3H59&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;FKM6A76&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FPZ2F54&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FPC-8J55&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;06225292000147&lt;/CNPJ&gt;&lt;IE&gt;283108491118&lt;/IE&gt;&lt;xNome&gt;TERLOC - TERMINAL LOGISTICO CESARI LTDA&lt;/xNome&gt;&lt;xFant&gt;TERLOC- TER. CESARI.&lt;/xFant&gt;&lt;fone&gt;01321028013&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AV ENGENHEIRO PLINIO DE QUEIROZ S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xCpl&gt;SP 55&lt;/xCpl&gt;&lt;xBairro&gt;PIACAGUERA&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;CUBATAO&lt;/xMun&gt;&lt;CEP&gt;11570000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;44777951000147&lt;/CNPJ&gt;&lt;IE&gt;407401398115&lt;/IE&gt;&lt;xNome&gt;ADUFERTIL FERTILIZANTES LTDA&lt;/xNome&gt;&lt;fone&gt;01133795000&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV BETA&lt;/xLgr&gt;&lt;nro&gt;461&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;3525904&lt;/cMun&gt;&lt;xMun&gt;JUNDIAI&lt;/xMun&gt;&lt;CEP&gt;13213070&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;1651.86&lt;/vTPrest&gt;&lt;vRec&gt;1651.86&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;1532.16&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;119.70&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS45&gt;&lt;CST&gt;51&lt;/CST&gt;&lt;/ICMS45&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;152.80&lt;/vTotTrib&gt;&lt;infAdFisco&gt;ICMS DIFERIDO CONFORME ARTIGO 358 DO RICMS&lt;/infAdFisco&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;38151.01&lt;/vCarga&gt;&lt;proPred&gt;SAM GR&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;28980.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;1.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;38151.01&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35211206225292000147550010006105071012602148&lt;/chave&gt;&lt;dPrev&gt;2021-12-20&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211250505924000118570010002829461002829461&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211250505924000118570010002829461002829461"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;g9kE7JmZJGNox71yJp7JbSgy0mA=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;BAGxo3Bg9mfmyMNGhF78LD4xPAezzlW0BV5wIMZ3xJqhUAWXbMOKFroyAHjXnJ7fK9P0AMnCYMPV84oHzix0isOj9uaUtuzLeBV1w9Hxp2Cb5/g6O8MciQIZXi/qICq6pYWoh0Wdl1nQtSTe3ONes6SUP9TNf+8725ixxG81wqEK2c0YpnhpWmAGBzq/DOM8jG7vUqwaKimxo/W/ErwmTSSpzCLyn2mmzRTNBjm4fR34bCU7yilNo2/xKVUCfeDGUfpZZRioiXZllWw7H54k+38lJKpJgKFvVGAsvo0mXrxFugkHb2Hzfy1OOhCpbDFVTFub+/tNqLWIqLLas0nzwg==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211250505924000118570010002829461002829461&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-20T20:56:50-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214652631424&lt;/nProt&gt;&lt;digVal&gt;g9kE7JmZJGNox71yJp7JbSgy0mA=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
+  </x:si>
+  <x:si>
+    <x:t>52211088305859002101550230000027711001975667.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Stars\Desktop\TRANSMOB\52211088305859002101550230000027711001975667.xml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>&lt;nfeProc versao="4.00" xmlns="http://www.portalfiscal.inf.br/nfe"&gt;&lt;NFe&gt;&lt;infNFe Id="NFe52211088305859002101550230000027711001975667" versao="4.00"&gt;&lt;ide&gt;&lt;cUF&gt;52&lt;/cUF&gt;&lt;cNF&gt;00197566&lt;/cNF&gt;&lt;natOp&gt;TRANSF DE MERCA ADQ 3ROS&lt;/natOp&gt;&lt;mod&gt;55&lt;/mod&gt;&lt;serie&gt;23&lt;/serie&gt;&lt;nNF&gt;2771&lt;/nNF&gt;&lt;dhEmi&gt;2021-10-14T08:37:26-03:00&lt;/dhEmi&gt;&lt;dhSaiEnt&gt;2021-10-14T08:37:26-03:00&lt;/dhSaiEnt&gt;&lt;tpNF&gt;1&lt;/tpNF&gt;&lt;idDest&gt;1&lt;/idDest&gt;&lt;cMunFG&gt;5213806&lt;/cMunFG&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;7&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;finNFe&gt;1&lt;/finNFe&gt;&lt;indFinal&gt;0&lt;/indFinal&gt;&lt;indPres&gt;9&lt;/indPres&gt;&lt;indIntermed&gt;0&lt;/indIntermed&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.88.0&lt;/verProc&gt;&lt;/ide&gt;&lt;emit&gt;&lt;CNPJ&gt;88305859002101&lt;/CNPJ&gt;&lt;xNome&gt;NUTRIEN AG SOLUTIONS INDUSTRIA E COMERCI&lt;/xNome&gt;&lt;xFant&gt;NUTRIEN SOLUCOES AGRICOLAS LTDA&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;QUADRA9 LOTE 7&lt;/xLgr&gt;&lt;nro&gt;86&lt;/nro&gt;&lt;xBairro&gt;DISTRITO AGROINDUSTRIAL&lt;/xBairro&gt;&lt;cMun&gt;5213806&lt;/cMun&gt;&lt;xMun&gt;Morrinhos - GO&lt;/xMun&gt;&lt;UF&gt;GO&lt;/UF&gt;&lt;CEP&gt;75650000&lt;/CEP&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;Brasil&lt;/xPais&gt;&lt;/enderEmit&gt;&lt;IE&gt;107857405&lt;/IE&gt;&lt;CRT&gt;3&lt;/CRT&gt;&lt;/emit&gt;&lt;dest&gt;&lt;CNPJ&gt;88305859002012&lt;/CNPJ&gt;&lt;xNome&gt;NUTRIEN AG SOLUTIONS IND COM PROD AGR LT&lt;/xNome&gt;&lt;enderDest&gt;&lt;xLgr&gt;RODOVIA BR 050&lt;/xLgr&gt;&lt;nro&gt;S/N&lt;/nro&gt;&lt;xBairro&gt;ZONA RURAL&lt;/xBairro&gt;&lt;cMun&gt;5206206&lt;/cMun&gt;&lt;xMun&gt;Cristalina - GO&lt;/xMun&gt;&lt;UF&gt;GO&lt;/UF&gt;&lt;CEP&gt;73850000&lt;/CEP&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;Brasil&lt;/xPais&gt;&lt;/enderDest&gt;&lt;indIEDest&gt;1&lt;/indIEDest&gt;&lt;IE&gt;107770857&lt;/IE&gt;&lt;email&gt;workflow@ibonline.com.br&lt;/email&gt;&lt;/dest&gt;&lt;det nItem="1"&gt;&lt;prod&gt;&lt;cProd&gt;F460000GR&lt;/cProd&gt;&lt;cEAN&gt;SEM GTIN&lt;/cEAN&gt;&lt;xProd&gt;UREIA 46%N GRANULADA&lt;/xProd&gt;&lt;NCM&gt;31021010&lt;/NCM&gt;&lt;CFOP&gt;5152&lt;/CFOP&gt;&lt;uCom&gt;t&lt;/uCom&gt;&lt;qCom&gt;22.0600&lt;/qCom&gt;&lt;vUnCom&gt;2880.079782&lt;/vUnCom&gt;&lt;vProd&gt;63534.56&lt;/vProd&gt;&lt;cEANTrib&gt;SEM GTIN&lt;/cEANTrib&gt;&lt;uTrib&gt;t&lt;/uTrib&gt;&lt;qTrib&gt;22.0600&lt;/qTrib&gt;&lt;vUnTrib&gt;2880.079782&lt;/vUnTrib&gt;&lt;indTot&gt;1&lt;/indTot&gt;&lt;/prod&gt;&lt;imposto&gt;&lt;ICMS&gt;&lt;ICMS40&gt;&lt;orig&gt;0&lt;/orig&gt;&lt;CST&gt;40&lt;/CST&gt;&lt;/ICMS40&gt;&lt;/ICMS&gt;&lt;IPI&gt;&lt;cEnq&gt;999&lt;/cEnq&gt;&lt;IPINT&gt;&lt;CST&gt;53&lt;/CST&gt;&lt;/IPINT&gt;&lt;/IPI&gt;&lt;II&gt;&lt;vBC&gt;0.00&lt;/vBC&gt;&lt;vDespAdu&gt;0.00&lt;/vDespAdu&gt;&lt;vII&gt;0.00&lt;/vII&gt;&lt;vIOF&gt;0.00&lt;/vIOF&gt;&lt;/II&gt;&lt;PIS&gt;&lt;PISNT&gt;&lt;CST&gt;06&lt;/CST&gt;&lt;/PISNT&gt;&lt;/PIS&gt;&lt;COFINS&gt;&lt;COFINSNT&gt;&lt;CST&gt;06&lt;/CST&gt;&lt;/COFINSNT&gt;&lt;/COFINS&gt;&lt;/imposto&gt;&lt;/det&gt;&lt;total&gt;&lt;ICMSTot&gt;&lt;vBC&gt;0.00&lt;/vBC&gt;&lt;vICMS&gt;0.00&lt;/vICMS&gt;&lt;vICMSDeson&gt;0.00&lt;/vICMSDeson&gt;&lt;vFCPUFDest&gt;0.00&lt;/vFCPUFDest&gt;&lt;vICMSUFDest&gt;0.00&lt;/vICMSUFDest&gt;&lt;vICMSUFRemet&gt;0.00&lt;/vICMSUFRemet&gt;&lt;vFCP&gt;0.00&lt;/vFCP&gt;&lt;vBCST&gt;0.00&lt;/vBCST&gt;&lt;vST&gt;0.00&lt;/vST&gt;&lt;vFCPST&gt;0.00&lt;/vFCPST&gt;&lt;vFCPSTRet&gt;0.00&lt;/vFCPSTRet&gt;&lt;vProd&gt;63534.56&lt;/vProd&gt;&lt;vFrete&gt;0.00&lt;/vFrete&gt;&lt;vSeg&gt;0.00&lt;/vSeg&gt;&lt;vDesc&gt;0.00&lt;/vDesc&gt;&lt;vII&gt;0.00&lt;/vII&gt;&lt;vIPI&gt;0.00&lt;/vIPI&gt;&lt;vIPIDevol&gt;0.00&lt;/vIPIDevol&gt;&lt;vPIS&gt;0.00&lt;/vPIS&gt;&lt;vCOFINS&gt;0.00&lt;/vCOFINS&gt;&lt;vOutro&gt;0.00&lt;/vOutro&gt;&lt;vNF&gt;63534.56&lt;/vNF&gt;&lt;/ICMSTot&gt;&lt;retTrib /&gt;&lt;/total&gt;&lt;transp&gt;&lt;modFrete&gt;1&lt;/modFrete&gt;&lt;transporta&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xEnder&gt;AVENIDA JOSE AUGUSTO DE CARVAL&lt;/xEnder&gt;&lt;xMun&gt;Bebedouro - SP&lt;/xMun&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;/transporta&gt;&lt;veicTransp&gt;&lt;placa&gt;FLA8069&lt;/placa&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;/veicTransp&gt;&lt;vol&gt;&lt;qVol&gt;0&lt;/qVol&gt;&lt;esp&gt;FERT MP&lt;/esp&gt;&lt;pesoL&gt;22.060&lt;/pesoL&gt;&lt;pesoB&gt;22.060&lt;/pesoB&gt;&lt;/vol&gt;&lt;/transp&gt;&lt;cobr /&gt;&lt;pag&gt;&lt;detPag&gt;&lt;tPag&gt;90&lt;/tPag&gt;&lt;vPag&gt;0.00&lt;/vPag&gt;&lt;/detPag&gt;&lt;/pag&gt;&lt;infAdic&gt;&lt;infCpl&gt;ISENÇÃO DO ICMS CONF. ART. 41º, INCISO I, DECRETO LEI 45.490/00 DO RICMS/00 E    CONVÊNIO 100/97. CONFORME A LEI NO. 7802/89, 9974/00 E DECRETO 4774/02.         DECLARAMOS QUE OS PRODUTOS ESTÃO ADEQUADAMENTE ACONDICIONADOS PARA SUPORTAR OS  RISCOS NORMAISE CARREGAMENTO, DESCARREGAMENTO, TRANSBORDO E TRANSPORTE,       CONFORME A REGULAMENTAÇÃO EM VIGOR.                                            * * * F R E T E    F O B * * * Nome do Motorista: .                                        Pedido:21002074-OH .&lt;/infCpl&gt;&lt;/infAdic&gt;&lt;infRespTec&gt;&lt;CNPJ&gt;00910509000171&lt;/CNPJ&gt;&lt;xContato&gt;Bruna Michele Barbosa&lt;/xContato&gt;&lt;email&gt;bruna.barbosa@thomsonreuters.com&lt;/email&gt;&lt;fone&gt;11997731642&lt;/fone&gt;&lt;/infRespTec&gt;&lt;/infNFe&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#NFe52211088305859002101550230000027711001975667"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;MIgUhLvCxCrAjwlRmxx/abv7l64=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;sV3MFYMaQV4LH0WWNQz+fk80PDTocRjvWGjh9SUA6FCjzYZbEpmpnqGrCUVhipQSg7+gdaZS++1jlHC4/vbxH0VWorQ4wmPKdEXcixfQyK/7ZFsfBiDXcuJvtRCuhvYjMvl/E8wY8Vi6c10VxU5t+PJRIO1eWuUnvKnr5fcWuBptIYXDo2OLrFeh3FYUgmCONarTV+jl7ZFjgb8IMqXU33yTxtumJ1uMWMmWSpATIctUIFQ8r5NIm5VhNDPfo6LbBRUoZMfqK1OwGa4QoW6HvLkoOzXXu8z8UE168pJZM83absw7HWw2uV8HZ/LoYPuKRMksErwwyJgaYmTyaFeDEQ==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIH6DCCBdCgAwIBAgIQRpp9vhTPQXz4JBSXbYhINDANBgkqhkiG9w0BAQsFADBzMQswCQYDVQQGEwJCUjETMBEGA1UECgwKSUNQLUJyYXNpbDEtMCsGA1UECwwkQ2VydGlzaWduIENlcnRpZmljYWRvcmEgRGlnaXRhbCBTLkEuMSAwHgYDVQQDDBdBQyBJbnN0aXR1dG8gRmVuYWNvbiBHNDAeFw0yMTAzMTIxODI1NTJaFw0yMjAzMTIxODI1NTJaMIG6MQswCQYDVQQGEwJCUjETMBEGA1UECgwKSUNQLUJyYXNpbDEXMBUGA1UECwwONjI2MzY2NzUwMDAxODkxGzAZBgNVBAsMEkFzc2luYXR1cmEgVGlwbyBBMTESMBAGA1UECwwJRU0gQlJBTkNPMRMwEQYDVQQLDApQUkVTRU5DSUFMMTcwNQYDVQQDDC5OVVRSSUVOIFNPTFVDT0VTIEFHUklDT0xBUyBMVERBOjg4MzA1ODU5MDAwMTUwMIIBIjANBgkqhkiG9w0BAQEFAAOCAQ8AMIIBCgKCAQEAyKd57LcM4g4Mvfkswc1qtfN+Y3s5VFHbZC/Ezc928JUcCpT6NqePK0bTd3dcsGlM+vBEwmhmaSWUU9To3M6VNz8PrRwvg5bv5w8HlZA2Qg1R6sesLfS82eAo010ayeteywCEZXIbHsZuouJ7nN89490iAYqqheNNVZ0nBEpg0tA29JwBE8OPFtioK05o3buBW2yy9Cpd6+6OGSCfXpN+dFx07VCvBnV4kVBZVAxT3wtXr5vs5+AZRHX+GCmS21meP0UUzWJ/ehdt1q3i2qBUHpe4qPSzhzGwNDPyiNI0ZzH28UgD5AJkEcl2Vd0c55pp1aSa00auODLoVCZw2vB3RQIDAQABo4IDLjCCAyowgcMGA1UdEQSBuzCBuKBCBgVgTAEDBKA5BDcyMDA3MTk3MTE0MzQzMzEwODMzMDAwMDAwMDAwMDAwMDAwMDAwMjAxNzQxNDMwMDAwMFNTUFNQoB4GBWBMAQMCoBUEE0xVSVMgQ0FSTE9TIENFUlJFU0mgGQYFYEwBAwOgEAQOODgzMDU4NTkwMDAxNTCgFwYFYEwBAwegDgQMMDAwMDAwMDAwMDAwgR50aWFnby5mcmVpdGFzQGdydXBvdGVjYWdyby5jb20wCQYDVR0TBAIwADAfBgNVHSMEGDAWgBQLkD9OvSFHYa/OFkWUD3oHe5IRUTCBiAYDVR0gBIGAMH4wfAYGYEwBAgEhMHIwcAYIKwYBBQUHAgEWZGh0dHA6Ly9pY3AtYnJhc2lsLmFjZmVuYWNvbi5jb20uYnIvcmVwb3NpdG9yaW8vZHBjL0FDLUluc3RpdHV0by1GZW5hY29uL0RQQ19BQ19JbnN0aXR1dG9fRmVuYWNvbi5wZGYwgcQGA1UdHwSBvDCBuTBboFmgV4ZVaHR0cDovL2ljcC1icmFzaWwuYWNmZW5hY29uLmNvbS5ici9yZXBvc2l0b3Jpby9sY3IvQUNJbnN0aXR1dG9GZW5hY29uRzQvTGF0ZXN0Q1JMLmNybDBaoFigVoZUaHR0cDovL2ljcC1icmFzaWwub3V0cmFsY3IuY29tLmJyL3JlcG9zaXRvcmlvL2xjci9BQ0luc3RpdHV0b0ZlbmFjb25HNC9MYXRlc3RDUkwuY3JsMA4GA1UdDwEB/wQEAwIF4DAdBgNVHSUEFjAUBggrBgEFBQcDAgYIKwYBBQUHAwQwgbQGCCsGAQUFBwEBBIGnMIGkMGMGCCsGAQUFBzAChldodHRwOi8vaWNwLWJyYXNpbC5hY2ZlbmFjb24uY29tLmJyL3JlcG9zaXRvcmlvL2NlcnRpZmljYWRvcy9BQ19JbnN0aXR1dG9fRmVuYWNvbl9HNC5wN2MwPQYIKwYBBQUHMAGGMWh0dHA6Ly9vY3NwLWFjLWluc3RpdHV0by1mZW5hY29uLmNlcnRpc2lnbi5jb20uYnIwDQYJKoZIhvcNAQELBQADggIBAIjXjPQQXEZVVZEoFnlz+/rYqXBBQCNzMvm1xCKjiNBil1xoX77HsfrM+GG8tpJdKVYqC6HaIOli6PDqTdQDxZC40tbn2RxF/LQAn/DWUT5f5zuHhr/Smh6KuiSyAx/B2G2rMv/wD9iHmP2U7MKUpivcspUkwpVmnw2H/YoGlpSxbkqYqWpJM9Ek/2+gOq5a+FmcRknb25o3kF+clBgiHz1EohowS10Fp/kfLAxV8kdDK4D8ZjZwPmqtrnr6CgyS0FERjAU9t3qE8w1PttlyUfRqR86HRB5aOM7qKobjMvSD0ZK+76CNr73SVQXjRD8A5ZGkITbNDFJulAnM2NfGly7qYYs52ul3F7eWx5FklvkG1eqim8PMJNma172fKhS4uCQyGakTdE39z49b10MF0V4JsORUIptI3nePw5M3EtdGItz9VQDaCh27udGOWPsIT2lwgwwZe9/uTBeunInNpdMki/znZsRaqNczZoWB4dTZSN5691e4wyzZnctSNjzP4tGVnK2iM2HXLbUvMB892TOHDFedCkSFyQBqyc2I/rq9I27aEsbOlO5mBY87aB0qa1IJHrqZzZg71jBUB9yoxjdoyuJkBMfBvPuVujone7l2YrQ7tm6xvWeW//vKDIPDgW/zYSTK1WLrVE/Npq70rmTb38I7x3aaPrkpQzcLGrnB&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/NFe&gt;&lt;protNFe versao="4.00"&gt;&lt;infProt Id="ID152214483573159"&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;0.0.1&lt;/verAplic&gt;&lt;chNFe&gt;52211088305859002101550230000027711001975667&lt;/chNFe&gt;&lt;dhRecbto&gt;2021-10-14T08:38:12-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;152214483573159&lt;/nProt&gt;&lt;digVal&gt;MIgUhLvCxCrAjwlRmxx/abv7l64=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso da NF-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protNFe&gt;&lt;/nfeProc&gt;</x:t>
   </x:si>
   <x:si>
     <x:t>35211250505924000118570010002833461002833460-ret-cons-cte.xml</x:t>
   </x:si>
   <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\35211250505924000118570010002833461002833460-ret-cons-cte.xml</x:t>
+    <x:t>C:\Users\Stars\Desktop\RODOTAC\Operações Subcontratadas\35211250505924000118570010002833461002833460-ret-cons-cte.xml</x:t>
   </x:si>
   <x:si>
     <x:t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;cteProc xmlns="http://www.portalfiscal.inf.br/cte" versao="3.00"&gt;&lt;CTe xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infCte versao="3.00" Id="CTe35211250505924000118570010002833461002833460"&gt;&lt;ide&gt;&lt;cUF&gt;35&lt;/cUF&gt;&lt;cCT&gt;00283346&lt;/cCT&gt;&lt;CFOP&gt;6352&lt;/CFOP&gt;&lt;natOp&gt;PREST.SERV.TRANSP.P/INDUSTRIA&lt;/natOp&gt;&lt;mod&gt;57&lt;/mod&gt;&lt;serie&gt;1&lt;/serie&gt;&lt;nCT&gt;283346&lt;/nCT&gt;&lt;dhEmi&gt;2021-12-30T02:47:00-03:00&lt;/dhEmi&gt;&lt;tpImp&gt;1&lt;/tpImp&gt;&lt;tpEmis&gt;1&lt;/tpEmis&gt;&lt;cDV&gt;0&lt;/cDV&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;tpCTe&gt;0&lt;/tpCTe&gt;&lt;procEmi&gt;0&lt;/procEmi&gt;&lt;verProc&gt;3.0.5.26&lt;/verProc&gt;&lt;cMunEnv&gt;3506102&lt;/cMunEnv&gt;&lt;xMunEnv&gt;BEBEDOURO&lt;/xMunEnv&gt;&lt;UFEnv&gt;SP&lt;/UFEnv&gt;&lt;modal&gt;01&lt;/modal&gt;&lt;tpServ&gt;0&lt;/tpServ&gt;&lt;cMunIni&gt;3513504&lt;/cMunIni&gt;&lt;xMunIni&gt;CUBATAO&lt;/xMunIni&gt;&lt;UFIni&gt;SP&lt;/UFIni&gt;&lt;cMunFim&gt;3170107&lt;/cMunFim&gt;&lt;xMunFim&gt;UBERABA&lt;/xMunFim&gt;&lt;UFFim&gt;MG&lt;/UFFim&gt;&lt;retira&gt;1&lt;/retira&gt;&lt;indIEToma&gt;1&lt;/indIEToma&gt;&lt;toma3&gt;&lt;toma&gt;3&lt;/toma&gt;&lt;/toma3&gt;&lt;/ide&gt;&lt;compl&gt;&lt;xCaracAd&gt;Normal&lt;/xCaracAd&gt;&lt;xEmi&gt;LUIZ FELIPE NETTO DO&lt;/xEmi&gt;&lt;fluxo&gt;&lt;xOrig&gt;CBT&lt;/xOrig&gt;&lt;xDest&gt;UBR&lt;/xDest&gt;&lt;xRota&gt;CBTUBR&lt;/xRota&gt;&lt;/fluxo&gt;&lt;origCalc&gt;CUBATAO&lt;/origCalc&gt;&lt;destCalc&gt;UBERABA&lt;/destCalc&gt;&lt;xObs&gt;Total Aproximado de Impostos : 1.449,73; Referencia do Cliente : 4500712092;&lt;/xObs&gt;&lt;ObsCont xCampo="frota"&gt;&lt;xTexto&gt;C0210&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="ref_cliente"&gt;&lt;xTexto&gt;4500712092&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="vlr_tarifa_ton"&gt;&lt;xTexto&gt;145.000000&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="motorista"&gt;&lt;xTexto&gt;ALEX HENRIQUE DO NASCIMENTO&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="cpf_motorista"&gt;&lt;xTexto&gt;307.951.808-02&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa"&gt;&lt;xTexto&gt;FOB3119&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa2"&gt;&lt;xTexto&gt;GCW5B44&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="placa3"&gt;&lt;xTexto&gt;FWU0J56&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;ObsCont xCampo="dolly"&gt;&lt;xTexto&gt;FXX-5085&lt;/xTexto&gt;&lt;/ObsCont&gt;&lt;/compl&gt;&lt;emit&gt;&lt;CNPJ&gt;50505924000118&lt;/CNPJ&gt;&lt;IE&gt;210015572118&lt;/IE&gt;&lt;xNome&gt;TRANSMOB TRANSPORTES LTDA&lt;/xNome&gt;&lt;xFant&gt;TRANSMOB (MATRIZ)&lt;/xFant&gt;&lt;enderEmit&gt;&lt;xLgr&gt;AVENIDA JOSE AUGUSTO DE CARVALHO&lt;/xLgr&gt;&lt;nro&gt;4063&lt;/nro&gt;&lt;xBairro&gt;DISTR INDUSTRIAL II&lt;/xBairro&gt;&lt;cMun&gt;3506102&lt;/cMun&gt;&lt;xMun&gt;BEBEDOURO&lt;/xMun&gt;&lt;CEP&gt;14711338&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;fone&gt;01733445555&lt;/fone&gt;&lt;/enderEmit&gt;&lt;/emit&gt;&lt;rem&gt;&lt;CNPJ&gt;06225292000147&lt;/CNPJ&gt;&lt;IE&gt;283108491118&lt;/IE&gt;&lt;xNome&gt;TERLOC - TERMINAL LOGISTICO CESARI LTDA&lt;/xNome&gt;&lt;xFant&gt;TERLOC- TER. CESARI.&lt;/xFant&gt;&lt;fone&gt;01321028013&lt;/fone&gt;&lt;enderReme&gt;&lt;xLgr&gt;AV ENGENHEIRO PLINIO DE QUEIROZ S/N&lt;/xLgr&gt;&lt;nro&gt;0&lt;/nro&gt;&lt;xCpl&gt;SP 55&lt;/xCpl&gt;&lt;xBairro&gt;PIACAGUERA&lt;/xBairro&gt;&lt;cMun&gt;3513504&lt;/cMun&gt;&lt;xMun&gt;CUBATAO&lt;/xMun&gt;&lt;CEP&gt;11570000&lt;/CEP&gt;&lt;UF&gt;SP&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderReme&gt;&lt;/rem&gt;&lt;dest&gt;&lt;CNPJ&gt;92660604015457&lt;/CNPJ&gt;&lt;IE&gt;3714585320678&lt;/IE&gt;&lt;xNome&gt;YARA BRASIL FERTILIZANTES S/A&lt;/xNome&gt;&lt;fone&gt;03433197198&lt;/fone&gt;&lt;enderDest&gt;&lt;xLgr&gt;AV ANTONIO CARLOS GUILLAUMON&lt;/xLgr&gt;&lt;nro&gt;800&lt;/nro&gt;&lt;xBairro&gt;DISTRITO INDUSTRIAL III&lt;/xBairro&gt;&lt;cMun&gt;3170107&lt;/cMun&gt;&lt;xMun&gt;UBERABA&lt;/xMun&gt;&lt;CEP&gt;38044760&lt;/CEP&gt;&lt;UF&gt;MG&lt;/UF&gt;&lt;cPais&gt;1058&lt;/cPais&gt;&lt;xPais&gt;BRASIL&lt;/xPais&gt;&lt;/enderDest&gt;&lt;/dest&gt;&lt;vPrest&gt;&lt;vTPrest&gt;6822.25&lt;/vTPrest&gt;&lt;vRec&gt;6822.25&lt;/vRec&gt;&lt;Comp&gt;&lt;xNome&gt;FRETE PESO&lt;/xNome&gt;&lt;vComp&gt;5954.65&lt;/vComp&gt;&lt;/Comp&gt;&lt;Comp&gt;&lt;xNome&gt;PEDAGIO&lt;/xNome&gt;&lt;vComp&gt;867.60&lt;/vComp&gt;&lt;/Comp&gt;&lt;/vPrest&gt;&lt;imp&gt;&lt;ICMS&gt;&lt;ICMS00&gt;&lt;CST&gt;00&lt;/CST&gt;&lt;vBC&gt;6822.25&lt;/vBC&gt;&lt;pICMS&gt;12.00&lt;/pICMS&gt;&lt;vICMS&gt;818.67&lt;/vICMS&gt;&lt;/ICMS00&gt;&lt;/ICMS&gt;&lt;vTotTrib&gt;1449.73&lt;/vTotTrib&gt;&lt;/imp&gt;&lt;infCTeNorm&gt;&lt;infCarga&gt;&lt;vCarga&gt;158564.15&lt;/vCarga&gt;&lt;proPred&gt;FERTILIZANTE MINERAL COMPLEXO YARAMILA 16-16-16 GR&lt;/proPred&gt;&lt;infQ&gt;&lt;cUnid&gt;01&lt;/cUnid&gt;&lt;tpMed&gt;PESO BRUTO&lt;/tpMed&gt;&lt;qCarga&gt;47050.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;infQ&gt;&lt;cUnid&gt;03&lt;/cUnid&gt;&lt;tpMed&gt;VOLUMES&lt;/tpMed&gt;&lt;qCarga&gt;1.0000&lt;/qCarga&gt;&lt;/infQ&gt;&lt;vCargaAverb&gt;158564.15&lt;/vCargaAverb&gt;&lt;/infCarga&gt;&lt;infDoc&gt;&lt;infNFe&gt;&lt;chave&gt;35211206225292000147550010006132001012667246&lt;/chave&gt;&lt;dPrev&gt;2021-12-30&lt;/dPrev&gt;&lt;/infNFe&gt;&lt;/infDoc&gt;&lt;infModal versaoModal="3.00"&gt;&lt;rodo&gt;&lt;RNTRC&gt;00279117&lt;/RNTRC&gt;&lt;/rodo&gt;&lt;/infModal&gt;&lt;cobr&gt;&lt;dup&gt;&lt;dVenc&gt;2021-12-01&lt;/dVenc&gt;&lt;/dup&gt;&lt;/cobr&gt;&lt;/infCTeNorm&gt;&lt;/infCte&gt;&lt;infCTeSupl&gt;&lt;qrCodCTe&gt;https://nfe.fazenda.sp.gov.br/CTeConsulta/qrCode?chCTe=35211250505924000118570010002833461002833460&amp;amp;tpAmb=1&lt;/qrCodCTe&gt;&lt;/infCTeSupl&gt;&lt;Signature xmlns="http://www.w3.org/2000/09/xmldsig#"&gt;&lt;SignedInfo&gt;&lt;CanonicalizationMethod Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;SignatureMethod Algorithm="http://www.w3.org/2000/09/xmldsig#rsa-sha1" /&gt;&lt;Reference URI="#CTe35211250505924000118570010002833461002833460"&gt;&lt;Transforms&gt;&lt;Transform Algorithm="http://www.w3.org/2000/09/xmldsig#enveloped-signature" /&gt;&lt;Transform Algorithm="http://www.w3.org/TR/2001/REC-xml-c14n-20010315" /&gt;&lt;/Transforms&gt;&lt;DigestMethod Algorithm="http://www.w3.org/2000/09/xmldsig#sha1" /&gt;&lt;DigestValue&gt;pVqNsPQodQDZa8nYk3QOnZfiZ/g=&lt;/DigestValue&gt;&lt;/Reference&gt;&lt;/SignedInfo&gt;&lt;SignatureValue&gt;nv99cvs6FgNJhwklmS/zwGU0qu5Pg96865SC7sHDzbKYXl88DB/rGnj4tpe1yivfbVEeYqHU6b3t+VWJY6gvGxiZOumj/aZbL0L6VjFcMqsfBWxHxPi6k8ol8Ja5cPSVkoOQrOW1ZZ/bpIFJ6f+xm0WyZ8slOwbOqzaItTHbkHfRjNySj8rzCQpyT2bDkvY+BIrDNVs58fB5+pNZN4lDmE7t4kDbxPJSJpF8JWmodrBCVpSfYrc9qTrYDnRrNH8TDB98/0/f5slbFvYtjesYze57x+gIACRJv0YZHImcm5F+DLVvVboYJqGSzxq8Mpviszb4gisehPV34ou5F3R5GQ==&lt;/SignatureValue&gt;&lt;KeyInfo&gt;&lt;X509Data&gt;&lt;X509Certificate&gt;MIIHPTCCBSWgAwIBAgIIfFghCRNtkJYwDQYJKoZIhvcNAQELBQAwWTELMAkGA1UEBhMCQlIxEzARBgNVBAoTCklDUC1CcmFzaWwxFTATBgNVBAsTDEFDIFNPTFVUSSB2NTEeMBwGA1UEAxMVQUMgQ0VSVElGSUNBIE1JTkFTIHY1MB4XDTIxMDkxNDEzNDAwMFoXDTIyMDkxNDEzNDAwMFowgeAxCzAJBgNVBAYTAkJSMRMwEQYDVQQKEwpJQ1AtQnJhc2lsMQswCQYDVQQIEwJTUDESMBAGA1UEBxMJQmViZWRvdXJvMR4wHAYDVQQLExVBQyBDRVJUSUZJQ0EgTUlOQVMgdjUxFzAVBgNVBAsTDjI3NTk1NTQzMDAwMTU1MRMwEQYDVQQLEwpQcmVzZW5jaWFsMRowGAYDVQQLExFDZXJ0aWZpY2FkbyBQSiBBMTExMC8GA1UEAxMoVFJBTlNNT0IgVFJBTlNQT1JURVMgTFREQTo1MDUwNTkyNDAwMDExODCCASIwDQYJKoZIhvcNAQEBBQADggEPADCCAQoCggEBAMI40MK4AsMUuiLTLItyRnmw3Aq2VbETDpRGYf+cbUcQb6edbInNjkA7fOCrm9v9SbFa1keevkXsT8JhnUvLMxPk1g13I6BLxi12Od8qG9ilise9TtioiFna06XkfC1jBf83k9sdU0zBu3LMjNM+SsRUY4f2RLrDBLUzdEluObD7GwnLGgzc5JJ3FujPOCq6qqnmw+9KcO+DvCinwElgFR1Czw1UGGhScxrGf94d6CDiS48L/X/lMnDVjW9T3mxKzSa/JMMUDuCKeBhYkx04bTSUZuyzTV49yVERbm8lIWlg+wAcKkChPp8IJL8VUFY0BETRjvPoEamFRJQ+adCpiOkCAwEAAaOCAn8wggJ7MB8GA1UdIwQYMBaAFD/TXKkZTdeIFi2YDK8K3uFPJBawMFkGCCsGAQUFBwEBBE0wSzBJBggrBgEFBQcwAoY9aHR0cDovL2NjZC5hY3NvbHV0aS5jb20uYnIvbGNyL2FjLWNlcnRpZmljYW1pbmFzLXNtaW1lLXY1LnA3YjCBsQYDVR0RBIGpMIGmgRh0cmFuc21vYkB0cmFuc21vYi5jb20uYnKgHAYFYEwBAwKgExMRSlVMSU8gQ0VTQVIgQ1VOSEGgGQYFYEwBAwOgEBMONTA1MDU5MjQwMDAxMTigOAYFYEwBAwSgLxMtMjUwMzE5NjMwNDk0NjEwOTgwMzAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwoBcGBWBMAQMHoA4TDDAwMDAwMDAwMDAwMDBiBgNVHSAEWzBZMFcGBmBMAQIBYDBNMEsGCCsGAQUFBwIBFj9odHRwOi8vY2NkLmFjc29sdXRpLmNvbS5ici9kb2NzL2RwYy1hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS5wZGYwHQYDVR0lBBYwFAYIKwYBBQUHAwIGCCsGAQUFBwMEMIGWBgNVHR8EgY4wgYswQ6BBoD+GPWh0dHA6Ly9jY2QuYWNzb2x1dGkuY29tLmJyL2xjci9hYy1jZXJ0aWZpY2FtaW5hcy1zbWltZS12NS5jcmwwRKBCoECGPmh0dHA6Ly9jY2QyLmFjc29sdXRpLmNvbS5ici9sY3IvYWMtY2VydGlmaWNhbWluYXMtc21pbWUtdjUuY3JsMB0GA1UdDgQWBBQl74Lq1KwZP3KATzOTiIWQVRpG2TAOBgNVHQ8BAf8EBAMCBeAwDQYJKoZIhvcNAQELBQADggIBAK55FEonqEtHG3Ykic0XNHNIY8blVBFGRqhKVKUgWf2YScuGtFQgJW84J8XNPTe/phlzbj8OyuD6Jej/s/9whc3rt3OwZ7dfJVGRrDOp2v/Syp+bYWZ36h05SW2t70ViqFhXzSHlxAAbqFzR6qAfBQuPfqQKJQScTr06hbj4ZTCY60RVOmACvmA6bCgOYjqLajIX3dqPo8rGt/K0ZX17TpBW2mL96x/1EHGWdzKGpGguFVvNmY89A18tItY84X9PrOtZSbgO2HTNNelRGp961axWS/Qy3cYUEInTCBBVYGrqEA6ml6NzvN+DwxGX/u5m72C4eZ1wByft8zg/mj7awpen41PWPjrKTJ6Ieyts2WOJLe3n9nH4whY0WkDa5axAjTO4Vf108gG+mbgVl7yOtnEXL4qdgJRWEoaiwcErD07Y7jnT9s8Ixh4FUe4dIVEBhnNamNTz2iW/fplHI6aUO4IKLDqAXA/8n+4SpnUnr3PLgo4phUctRgYhc4bsbbp3cLjWzOyby8KdLqIvJjWhfSLIobfpyMi32fQVDce0aRMIbc24BbQC/lvmWJZNiNt/9W522c3znLkOvHXexvIqWzQEUlVdCh231JLkdLRq12e3I6wEQKIBkQQr9t2iCQg6xplIAn/mNtCHT+pEYqGFJaFAJel9DsFYzpG8IC+8a8WE&lt;/X509Certificate&gt;&lt;/X509Data&gt;&lt;/KeyInfo&gt;&lt;/Signature&gt;&lt;/CTe&gt;&lt;protCTe versao="3.00" xmlns="http://www.portalfiscal.inf.br/cte"&gt;&lt;infProt&gt;&lt;tpAmb&gt;1&lt;/tpAmb&gt;&lt;verAplic&gt;SP-CTe-2021-08-19-1&lt;/verAplic&gt;&lt;chCTe&gt;35211250505924000118570010002833461002833460&lt;/chCTe&gt;&lt;dhRecbto&gt;2021-12-30T02:49:37-03:00&lt;/dhRecbto&gt;&lt;nProt&gt;135214686510642&lt;/nProt&gt;&lt;digVal&gt;pVqNsPQodQDZa8nYk3QOnZfiZ/g=&lt;/digVal&gt;&lt;cStat&gt;100&lt;/cStat&gt;&lt;xMotivo&gt;Autorizado o uso do CT-e&lt;/xMotivo&gt;&lt;/infProt&gt;&lt;/protCTe&gt;&lt;/cteProc&gt;</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Users\Stars\Desktop\RODOTAC\Operações Subcontratadas\35211250505924000118570010002833461002833460-ret-cons-cte.xml</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -995,13 +832,13 @@
     </x:row>
     <x:row r="22" spans="1:3">
       <x:c r="A22" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>65</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>